<commit_message>
Update guest volume estimation using vdW radii from PyMOL v2.5.0
</commit_message>
<xml_diff>
--- a/results/quantitative-analysis.xlsx
+++ b/results/quantitative-analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gyorgy Szaloki\Papers\Cavity calculations\Benchmarking\Structures for benchmarking\QUANTITATIVE ANALYSIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5C5C498-82D0-47B6-9060-E7900CE0A105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7543670-3C34-44CA-998E-BD6F43F9A73E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -243,7 +243,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -266,6 +266,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Liberation Sans"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -802,7 +807,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1059,16 +1064,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1089,6 +1088,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1116,6 +1127,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1497,8 +1509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4587FD2-9A4F-496C-BFF9-32ED9AC29E44}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1554,43 +1566,43 @@
       </c>
       <c r="C2" s="80">
         <f>Calculations!C2</f>
-        <v>126.95</v>
+        <v>161.22999999999999</v>
       </c>
       <c r="D2" s="80">
         <f>Calculations!D2</f>
-        <v>230.81818181818181</v>
+        <v>293.14545454545453</v>
       </c>
       <c r="E2" s="81" t="str">
         <f>ROUND(Calculations!E2,0)&amp;" ("&amp;ROUND(Calculations!F2,1)&amp;"%)"</f>
-        <v>284 (18.7%)</v>
+        <v>284 (-3.2%)</v>
       </c>
       <c r="F2" s="58" t="str">
         <f>ROUND(Calculations!G2,0)&amp;" ("&amp;ROUND(Calculations!H2,1)&amp;"%)"</f>
-        <v>282 (18.2%)</v>
+        <v>282 (-3.8%)</v>
       </c>
       <c r="G2" s="58" t="str">
         <f>ROUND(Calculations!I2,0)&amp;" ("&amp;ROUND(Calculations!J2,1)&amp;"%)"</f>
-        <v>261 (11.6%)</v>
+        <v>261 (-12.3%)</v>
       </c>
       <c r="H2" s="58" t="str">
         <f>ROUND(Calculations!K2,0)&amp;" ("&amp;ROUND(Calculations!L2,1)&amp;"%)"</f>
-        <v>247 (6.7%)</v>
+        <v>247 (-18.5%)</v>
       </c>
       <c r="I2" s="58" t="str">
         <f>ROUND(Calculations!M2,0)&amp;" ("&amp;ROUND(Calculations!N2,1)&amp;"%)"</f>
-        <v>175 (-31.8%)</v>
+        <v>175 (-67.4%)</v>
       </c>
       <c r="J2" s="58" t="str">
         <f>ROUND(Calculations!O2,0)&amp;" ("&amp;ROUND(Calculations!P2,1)&amp;"%)"</f>
-        <v>133 (-73.6%)</v>
+        <v>133 (-120.5%)</v>
       </c>
       <c r="K2" s="58" t="str">
         <f>ROUND(Calculations!Q2,0)&amp;" ("&amp;ROUND(Calculations!R2,1)&amp;"%)"</f>
-        <v>109 (-111.8%)</v>
+        <v>109 (-168.9%)</v>
       </c>
       <c r="L2" s="59" t="str">
         <f>ROUND(Calculations!S2,0)&amp;" ("&amp;ROUND(Calculations!T2,1)&amp;"%)"</f>
-        <v>396 (41.7%)</v>
+        <v>396 (26%)</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1602,43 +1614,43 @@
       </c>
       <c r="C3" s="80">
         <f>Calculations!C3</f>
-        <v>136.82</v>
+        <v>165.19</v>
       </c>
       <c r="D3" s="80">
         <f>Calculations!D3</f>
-        <v>248.76363636363632</v>
+        <v>300.34545454545452</v>
       </c>
       <c r="E3" s="81" t="str">
         <f>ROUND(Calculations!E3,0)&amp;" ("&amp;ROUND(Calculations!F3,1)&amp;"%)"</f>
-        <v>261 (4.8%)</v>
+        <v>261 (-15%)</v>
       </c>
       <c r="F3" s="58" t="str">
         <f>ROUND(Calculations!G3,0)&amp;" ("&amp;ROUND(Calculations!H3,1)&amp;"%)"</f>
-        <v>261 (4.8%)</v>
+        <v>261 (-14.9%)</v>
       </c>
       <c r="G3" s="58" t="str">
         <f>ROUND(Calculations!I3,0)&amp;" ("&amp;ROUND(Calculations!J3,1)&amp;"%)"</f>
-        <v>241 (-3.3%)</v>
+        <v>241 (-24.7%)</v>
       </c>
       <c r="H3" s="58" t="str">
         <f>ROUND(Calculations!K3,0)&amp;" ("&amp;ROUND(Calculations!L3,1)&amp;"%)"</f>
-        <v>246 (-1%)</v>
+        <v>246 (-21.9%)</v>
       </c>
       <c r="I3" s="58" t="str">
         <f>ROUND(Calculations!M3,0)&amp;" ("&amp;ROUND(Calculations!N3,1)&amp;"%)"</f>
-        <v>180 (-38.4%)</v>
+        <v>180 (-67.1%)</v>
       </c>
       <c r="J3" s="58" t="str">
         <f>ROUND(Calculations!O3,0)&amp;" ("&amp;ROUND(Calculations!P3,1)&amp;"%)"</f>
-        <v>90 (-177.7%)</v>
+        <v>90 (-235.3%)</v>
       </c>
       <c r="K3" s="58" t="str">
         <f>ROUND(Calculations!Q3,0)&amp;" ("&amp;ROUND(Calculations!R3,1)&amp;"%)"</f>
-        <v>92 (-170.4%)</v>
+        <v>92 (-226.5%)</v>
       </c>
       <c r="L3" s="59" t="str">
         <f>ROUND(Calculations!S3,0)&amp;" ("&amp;ROUND(Calculations!T3,1)&amp;"%)"</f>
-        <v>267 (6.8%)</v>
+        <v>267 (-12.5%)</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1650,43 +1662,43 @@
       </c>
       <c r="C4" s="80">
         <f>Calculations!C4</f>
-        <v>121.71</v>
+        <v>141.15</v>
       </c>
       <c r="D4" s="80">
         <f>Calculations!D4</f>
-        <v>221.29090909090905</v>
+        <v>256.63636363636363</v>
       </c>
       <c r="E4" s="81" t="str">
         <f>ROUND(Calculations!E4,0)&amp;" ("&amp;ROUND(Calculations!F4,1)&amp;"%)"</f>
-        <v>270 (18.2%)</v>
+        <v>270 (5.1%)</v>
       </c>
       <c r="F4" s="58" t="str">
         <f>ROUND(Calculations!G4,0)&amp;" ("&amp;ROUND(Calculations!H4,1)&amp;"%)"</f>
-        <v>270 (18.1%)</v>
+        <v>270 (5.1%)</v>
       </c>
       <c r="G4" s="58" t="str">
         <f>ROUND(Calculations!I4,0)&amp;" ("&amp;ROUND(Calculations!J4,1)&amp;"%)"</f>
-        <v>253 (12.4%)</v>
+        <v>253 (-1.6%)</v>
       </c>
       <c r="H4" s="58" t="str">
         <f>ROUND(Calculations!K4,0)&amp;" ("&amp;ROUND(Calculations!L4,1)&amp;"%)"</f>
-        <v>277 (20.2%)</v>
+        <v>277 (7.4%)</v>
       </c>
       <c r="I4" s="58" t="str">
         <f>ROUND(Calculations!M4,0)&amp;" ("&amp;ROUND(Calculations!N4,1)&amp;"%)"</f>
-        <v>191 (-16.2%)</v>
+        <v>191 (-34.7%)</v>
       </c>
       <c r="J4" s="58" t="str">
         <f>ROUND(Calculations!O4,0)&amp;" ("&amp;ROUND(Calculations!P4,1)&amp;"%)"</f>
-        <v>113 (-96.2%)</v>
+        <v>113 (-127.6%)</v>
       </c>
       <c r="K4" s="58" t="str">
         <f>ROUND(Calculations!Q4,0)&amp;" ("&amp;ROUND(Calculations!R4,1)&amp;"%)"</f>
-        <v>99 (-123.5%)</v>
+        <v>99 (-159.2%)</v>
       </c>
       <c r="L4" s="59" t="str">
         <f>ROUND(Calculations!S4,0)&amp;" ("&amp;ROUND(Calculations!T4,1)&amp;"%)"</f>
-        <v>335 (33.9%)</v>
+        <v>335 (23.4%)</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1698,43 +1710,43 @@
       </c>
       <c r="C5" s="80">
         <f>Calculations!C5</f>
-        <v>257.93</v>
+        <v>309.69</v>
       </c>
       <c r="D5" s="80">
         <f>Calculations!D5</f>
-        <v>468.96363636363634</v>
+        <v>563.07272727272721</v>
       </c>
       <c r="E5" s="81" t="str">
         <f>ROUND(Calculations!E5,0)&amp;" ("&amp;ROUND(Calculations!F5,1)&amp;"%)"</f>
-        <v>413 (-13.6%)</v>
+        <v>413 (-36.4%)</v>
       </c>
       <c r="F5" s="58" t="str">
         <f>ROUND(Calculations!G5,0)&amp;" ("&amp;ROUND(Calculations!H5,1)&amp;"%)"</f>
-        <v>413 (-13.6%)</v>
+        <v>413 (-36.4%)</v>
       </c>
       <c r="G5" s="58" t="str">
         <f>ROUND(Calculations!I5,0)&amp;" ("&amp;ROUND(Calculations!J5,1)&amp;"%)"</f>
-        <v>410 (-14.3%)</v>
+        <v>410 (-37.2%)</v>
       </c>
       <c r="H5" s="58" t="str">
         <f>ROUND(Calculations!K5,0)&amp;" ("&amp;ROUND(Calculations!L5,1)&amp;"%)"</f>
-        <v>434 (-8%)</v>
+        <v>434 (-29.6%)</v>
       </c>
       <c r="I5" s="58" t="str">
         <f>ROUND(Calculations!M5,0)&amp;" ("&amp;ROUND(Calculations!N5,1)&amp;"%)"</f>
-        <v>343 (-36.7%)</v>
+        <v>343 (-64.2%)</v>
       </c>
       <c r="J5" s="58" t="str">
         <f>ROUND(Calculations!O5,0)&amp;" ("&amp;ROUND(Calculations!P5,1)&amp;"%)"</f>
-        <v>251 (-87%)</v>
+        <v>251 (-124.6%)</v>
       </c>
       <c r="K5" s="58" t="str">
         <f>ROUND(Calculations!Q5,0)&amp;" ("&amp;ROUND(Calculations!R5,1)&amp;"%)"</f>
-        <v>222 (-111.2%)</v>
+        <v>222 (-153.6%)</v>
       </c>
       <c r="L5" s="59" t="str">
         <f>ROUND(Calculations!S5,0)&amp;" ("&amp;ROUND(Calculations!T5,1)&amp;"%)"</f>
-        <v>474 (1.1%)</v>
+        <v>474 (-18.8%)</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1746,39 +1758,39 @@
       </c>
       <c r="C6" s="80">
         <f>Calculations!C6</f>
-        <v>57.4</v>
+        <v>55.06</v>
       </c>
       <c r="D6" s="80">
         <f>Calculations!D6</f>
-        <v>104.36363636363635</v>
+        <v>100.10909090909091</v>
       </c>
       <c r="E6" s="81" t="str">
         <f>ROUND(Calculations!E6,0)&amp;" ("&amp;ROUND(Calculations!F6,1)&amp;"%)"</f>
-        <v>79 (-32.7%)</v>
+        <v>79 (-27.3%)</v>
       </c>
       <c r="F6" s="58" t="str">
         <f>ROUND(Calculations!G6,0)&amp;" ("&amp;ROUND(Calculations!H6,1)&amp;"%)"</f>
-        <v>78 (-33.7%)</v>
+        <v>78 (-28.3%)</v>
       </c>
       <c r="G6" s="58" t="str">
         <f>ROUND(Calculations!I6,0)&amp;" ("&amp;ROUND(Calculations!J6,1)&amp;"%)"</f>
-        <v>44 (-138%)</v>
+        <v>44 (-128.3%)</v>
       </c>
       <c r="H6" s="58" t="str">
         <f>ROUND(Calculations!K6,0)&amp;" ("&amp;ROUND(Calculations!L6,1)&amp;"%)"</f>
-        <v>84 (-23.8%)</v>
+        <v>84 (-18.7%)</v>
       </c>
       <c r="I6" s="58" t="str">
         <f>ROUND(Calculations!M6,0)&amp;" ("&amp;ROUND(Calculations!N6,1)&amp;"%)"</f>
-        <v>29 (-257.4%)</v>
+        <v>29 (-242.8%)</v>
       </c>
       <c r="J6" s="58" t="str">
         <f>ROUND(Calculations!O6,0)&amp;" ("&amp;ROUND(Calculations!P6,1)&amp;"%)"</f>
-        <v>37 (-183.8%)</v>
+        <v>37 (-172.3%)</v>
       </c>
       <c r="K6" s="58" t="str">
         <f>ROUND(Calculations!Q6,0)&amp;" ("&amp;ROUND(Calculations!R6,1)&amp;"%)"</f>
-        <v>11 (-893.9%)</v>
+        <v>11 (-853.4%)</v>
       </c>
       <c r="L6" s="59" t="e">
         <f>ROUND(Calculations!S6,0)&amp;" ("&amp;ROUND(Calculations!T6,1)&amp;"%)"</f>
@@ -1794,39 +1806,39 @@
       </c>
       <c r="C7" s="80">
         <f>Calculations!C7</f>
-        <v>83.64</v>
+        <v>66.59</v>
       </c>
       <c r="D7" s="80">
         <f>Calculations!D7</f>
-        <v>152.07272727272726</v>
+        <v>121.07272727272726</v>
       </c>
       <c r="E7" s="81" t="str">
         <f>ROUND(Calculations!E7,0)&amp;" ("&amp;ROUND(Calculations!F7,1)&amp;"%)"</f>
-        <v>80 (-89.5%)</v>
+        <v>80 (-50.9%)</v>
       </c>
       <c r="F7" s="58" t="str">
         <f>ROUND(Calculations!G7,0)&amp;" ("&amp;ROUND(Calculations!H7,1)&amp;"%)"</f>
-        <v>81 (-87.4%)</v>
+        <v>81 (-49.2%)</v>
       </c>
       <c r="G7" s="58" t="str">
         <f>ROUND(Calculations!I7,0)&amp;" ("&amp;ROUND(Calculations!J7,1)&amp;"%)"</f>
-        <v>55 (-176.1%)</v>
+        <v>55 (-119.8%)</v>
       </c>
       <c r="H7" s="58" t="str">
         <f>ROUND(Calculations!K7,0)&amp;" ("&amp;ROUND(Calculations!L7,1)&amp;"%)"</f>
-        <v>82 (-85.2%)</v>
+        <v>82 (-47.5%)</v>
       </c>
       <c r="I7" s="58" t="str">
         <f>ROUND(Calculations!M7,0)&amp;" ("&amp;ROUND(Calculations!N7,1)&amp;"%)"</f>
-        <v>64 (-139.5%)</v>
+        <v>64 (-90.7%)</v>
       </c>
       <c r="J7" s="58" t="str">
         <f>ROUND(Calculations!O7,0)&amp;" ("&amp;ROUND(Calculations!P7,1)&amp;"%)"</f>
-        <v>40 (-285%)</v>
+        <v>40 (-206.5%)</v>
       </c>
       <c r="K7" s="58" t="str">
         <f>ROUND(Calculations!Q7,0)&amp;" ("&amp;ROUND(Calculations!R7,1)&amp;"%)"</f>
-        <v>11 (-1314.6%)</v>
+        <v>11 (-1026.3%)</v>
       </c>
       <c r="L7" s="59" t="e">
         <f>ROUND(Calculations!S7,0)&amp;" ("&amp;ROUND(Calculations!T7,1)&amp;"%)"</f>
@@ -1842,39 +1854,39 @@
       </c>
       <c r="C8" s="80">
         <f>Calculations!C8</f>
-        <v>505.05</v>
+        <v>520.71</v>
       </c>
       <c r="D8" s="80">
         <f>Calculations!D8</f>
-        <v>918.27272727272725</v>
+        <v>946.74545454545455</v>
       </c>
       <c r="E8" s="81" t="str">
         <f>ROUND(Calculations!E8,0)&amp;" ("&amp;ROUND(Calculations!F8,1)&amp;"%)"</f>
-        <v>755 (-21.6%)</v>
+        <v>755 (-25.4%)</v>
       </c>
       <c r="F8" s="58" t="str">
         <f>ROUND(Calculations!G8,0)&amp;" ("&amp;ROUND(Calculations!H8,1)&amp;"%)"</f>
-        <v>759 (-21%)</v>
+        <v>759 (-24.8%)</v>
       </c>
       <c r="G8" s="58" t="str">
         <f>ROUND(Calculations!I8,0)&amp;" ("&amp;ROUND(Calculations!J8,1)&amp;"%)"</f>
-        <v>708 (-29.7%)</v>
+        <v>708 (-33.7%)</v>
       </c>
       <c r="H8" s="58" t="str">
         <f>ROUND(Calculations!K8,0)&amp;" ("&amp;ROUND(Calculations!L8,1)&amp;"%)"</f>
-        <v>771 (-19.1%)</v>
+        <v>771 (-22.8%)</v>
       </c>
       <c r="I8" s="58" t="str">
         <f>ROUND(Calculations!M8,0)&amp;" ("&amp;ROUND(Calculations!N8,1)&amp;"%)"</f>
-        <v>734 (-25.2%)</v>
+        <v>734 (-29%)</v>
       </c>
       <c r="J8" s="58" t="str">
         <f>ROUND(Calculations!O8,0)&amp;" ("&amp;ROUND(Calculations!P8,1)&amp;"%)"</f>
-        <v>492 (-86.7%)</v>
+        <v>492 (-92.5%)</v>
       </c>
       <c r="K8" s="58" t="str">
         <f>ROUND(Calculations!Q8,0)&amp;" ("&amp;ROUND(Calculations!R8,1)&amp;"%)"</f>
-        <v>385 (-138.5%)</v>
+        <v>385 (-145.9%)</v>
       </c>
       <c r="L8" s="59" t="e">
         <f>ROUND(Calculations!S8,0)&amp;" ("&amp;ROUND(Calculations!T8,1)&amp;"%)"</f>
@@ -1890,39 +1902,39 @@
       </c>
       <c r="C9" s="80">
         <f>Calculations!C9</f>
-        <v>498.11</v>
+        <v>513.66999999999996</v>
       </c>
       <c r="D9" s="80">
         <f>Calculations!D9</f>
-        <v>905.65454545454543</v>
+        <v>933.94545454545437</v>
       </c>
       <c r="E9" s="81" t="str">
         <f>ROUND(Calculations!E9,0)&amp;" ("&amp;ROUND(Calculations!F9,1)&amp;"%)"</f>
-        <v>730 (-24.1%)</v>
+        <v>730 (-28%)</v>
       </c>
       <c r="F9" s="58" t="str">
         <f>ROUND(Calculations!G9,0)&amp;" ("&amp;ROUND(Calculations!H9,1)&amp;"%)"</f>
-        <v>730 (-24%)</v>
+        <v>730 (-27.9%)</v>
       </c>
       <c r="G9" s="58" t="str">
         <f>ROUND(Calculations!I9,0)&amp;" ("&amp;ROUND(Calculations!J9,1)&amp;"%)"</f>
-        <v>747 (-21.2%)</v>
+        <v>747 (-25%)</v>
       </c>
       <c r="H9" s="58" t="str">
         <f>ROUND(Calculations!K9,0)&amp;" ("&amp;ROUND(Calculations!L9,1)&amp;"%)"</f>
-        <v>805 (-12.6%)</v>
+        <v>805 (-16.1%)</v>
       </c>
       <c r="I9" s="58" t="str">
         <f>ROUND(Calculations!M9,0)&amp;" ("&amp;ROUND(Calculations!N9,1)&amp;"%)"</f>
-        <v>704 (-28.6%)</v>
+        <v>704 (-32.7%)</v>
       </c>
       <c r="J9" s="58" t="str">
         <f>ROUND(Calculations!O9,0)&amp;" ("&amp;ROUND(Calculations!P9,1)&amp;"%)"</f>
-        <v>517 (-75.1%)</v>
+        <v>517 (-80.6%)</v>
       </c>
       <c r="K9" s="58" t="str">
         <f>ROUND(Calculations!Q9,0)&amp;" ("&amp;ROUND(Calculations!R9,1)&amp;"%)"</f>
-        <v>409 (-121.4%)</v>
+        <v>409 (-128.3%)</v>
       </c>
       <c r="L9" s="59" t="e">
         <f>ROUND(Calculations!S9,0)&amp;" ("&amp;ROUND(Calculations!T9,1)&amp;"%)"</f>
@@ -1938,39 +1950,39 @@
       </c>
       <c r="C10" s="80">
         <f>Calculations!C10</f>
-        <v>137.37</v>
+        <v>151.88999999999999</v>
       </c>
       <c r="D10" s="80">
         <f>Calculations!D10</f>
-        <v>249.76363636363635</v>
+        <v>276.16363636363633</v>
       </c>
       <c r="E10" s="81" t="str">
         <f>ROUND(Calculations!E10,0)&amp;" ("&amp;ROUND(Calculations!F10,1)&amp;"%)"</f>
-        <v>156 (-60.2%)</v>
+        <v>156 (-77.1%)</v>
       </c>
       <c r="F10" s="58" t="str">
         <f>ROUND(Calculations!G10,0)&amp;" ("&amp;ROUND(Calculations!H10,1)&amp;"%)"</f>
-        <v>155 (-61.6%)</v>
+        <v>155 (-78.7%)</v>
       </c>
       <c r="G10" s="58" t="str">
         <f>ROUND(Calculations!I10,0)&amp;" ("&amp;ROUND(Calculations!J10,1)&amp;"%)"</f>
-        <v>177 (-41.2%)</v>
+        <v>177 (-56.1%)</v>
       </c>
       <c r="H10" s="58" t="str">
         <f>ROUND(Calculations!K10,0)&amp;" ("&amp;ROUND(Calculations!L10,1)&amp;"%)"</f>
-        <v>181 (-38%)</v>
+        <v>181 (-52.6%)</v>
       </c>
       <c r="I10" s="58" t="str">
         <f>ROUND(Calculations!M10,0)&amp;" ("&amp;ROUND(Calculations!N10,1)&amp;"%)"</f>
-        <v>159 (-56.9%)</v>
+        <v>159 (-73.5%)</v>
       </c>
       <c r="J10" s="58" t="str">
         <f>ROUND(Calculations!O10,0)&amp;" ("&amp;ROUND(Calculations!P10,1)&amp;"%)"</f>
-        <v>122 (-104.5%)</v>
+        <v>122 (-126.1%)</v>
       </c>
       <c r="K10" s="58" t="str">
         <f>ROUND(Calculations!Q10,0)&amp;" ("&amp;ROUND(Calculations!R10,1)&amp;"%)"</f>
-        <v>62 (-302.8%)</v>
+        <v>62 (-345.4%)</v>
       </c>
       <c r="L10" s="59" t="e">
         <f>ROUND(Calculations!S10,0)&amp;" ("&amp;ROUND(Calculations!T10,1)&amp;"%)"</f>
@@ -1986,39 +1998,39 @@
       </c>
       <c r="C11" s="80">
         <f>Calculations!C11</f>
-        <v>121.6</v>
+        <v>150.5</v>
       </c>
       <c r="D11" s="80">
         <f>Calculations!D11</f>
-        <v>221.09090909090907</v>
+        <v>273.63636363636363</v>
       </c>
       <c r="E11" s="81" t="str">
         <f>ROUND(Calculations!E11,0)&amp;" ("&amp;ROUND(Calculations!F11,1)&amp;"%)"</f>
-        <v>246 (10.2%)</v>
+        <v>246 (-11.2%)</v>
       </c>
       <c r="F11" s="58" t="str">
         <f>ROUND(Calculations!G11,0)&amp;" ("&amp;ROUND(Calculations!H11,1)&amp;"%)"</f>
-        <v>248 (10.8%)</v>
+        <v>248 (-10.4%)</v>
       </c>
       <c r="G11" s="58" t="str">
         <f>ROUND(Calculations!I11,0)&amp;" ("&amp;ROUND(Calculations!J11,1)&amp;"%)"</f>
-        <v>225 (1.9%)</v>
+        <v>225 (-21.5%)</v>
       </c>
       <c r="H11" s="58" t="str">
         <f>ROUND(Calculations!K11,0)&amp;" ("&amp;ROUND(Calculations!L11,1)&amp;"%)"</f>
-        <v>225 (1.9%)</v>
+        <v>225 (-21.5%)</v>
       </c>
       <c r="I11" s="58" t="str">
         <f>ROUND(Calculations!M11,0)&amp;" ("&amp;ROUND(Calculations!N11,1)&amp;"%)"</f>
-        <v>161 (-37.1%)</v>
+        <v>161 (-69.6%)</v>
       </c>
       <c r="J11" s="58" t="str">
         <f>ROUND(Calculations!O11,0)&amp;" ("&amp;ROUND(Calculations!P11,1)&amp;"%)"</f>
-        <v>125 (-77.4%)</v>
+        <v>125 (-119.5%)</v>
       </c>
       <c r="K11" s="58" t="str">
         <f>ROUND(Calculations!Q11,0)&amp;" ("&amp;ROUND(Calculations!R11,1)&amp;"%)"</f>
-        <v>94 (-135.2%)</v>
+        <v>94 (-191.1%)</v>
       </c>
       <c r="L11" s="59" t="e">
         <f>ROUND(Calculations!S11,0)&amp;" ("&amp;ROUND(Calculations!T11,1)&amp;"%)"</f>
@@ -2034,39 +2046,39 @@
       </c>
       <c r="C12" s="80">
         <f>Calculations!C12</f>
-        <v>248.63</v>
+        <v>219.71</v>
       </c>
       <c r="D12" s="80">
         <f>Calculations!D12</f>
-        <v>452.0545454545454</v>
+        <v>399.47272727272724</v>
       </c>
       <c r="E12" s="81" t="str">
         <f>ROUND(Calculations!E12,0)&amp;" ("&amp;ROUND(Calculations!F12,1)&amp;"%)"</f>
-        <v>229 (-97.3%)</v>
+        <v>229 (-74.4%)</v>
       </c>
       <c r="F12" s="58" t="str">
         <f>ROUND(Calculations!G12,0)&amp;" ("&amp;ROUND(Calculations!H12,1)&amp;"%)"</f>
-        <v>230 (-96.5%)</v>
+        <v>230 (-73.7%)</v>
       </c>
       <c r="G12" s="58" t="str">
         <f>ROUND(Calculations!I12,0)&amp;" ("&amp;ROUND(Calculations!J12,1)&amp;"%)"</f>
-        <v>389 (-16.1%)</v>
+        <v>389 (-2.6%)</v>
       </c>
       <c r="H12" s="58" t="str">
         <f>ROUND(Calculations!K12,0)&amp;" ("&amp;ROUND(Calculations!L12,1)&amp;"%)"</f>
-        <v>652 (30.7%)</v>
+        <v>652 (38.7%)</v>
       </c>
       <c r="I12" s="58" t="str">
         <f>ROUND(Calculations!M12,0)&amp;" ("&amp;ROUND(Calculations!N12,1)&amp;"%)"</f>
-        <v>349 (-29.6%)</v>
+        <v>349 (-14.6%)</v>
       </c>
       <c r="J12" s="58" t="str">
         <f>ROUND(Calculations!O12,0)&amp;" ("&amp;ROUND(Calculations!P12,1)&amp;"%)"</f>
-        <v>114 (-298.2%)</v>
+        <v>114 (-251.9%)</v>
       </c>
       <c r="K12" s="58" t="str">
         <f>ROUND(Calculations!Q12,0)&amp;" ("&amp;ROUND(Calculations!R12,1)&amp;"%)"</f>
-        <v>164 (-175.6%)</v>
+        <v>164 (-143.6%)</v>
       </c>
       <c r="L12" s="59" t="e">
         <f>ROUND(Calculations!S12,0)&amp;" ("&amp;ROUND(Calculations!T12,1)&amp;"%)"</f>
@@ -2082,39 +2094,39 @@
       </c>
       <c r="C13" s="80">
         <f>Calculations!C13</f>
-        <v>269.86</v>
+        <v>306.64</v>
       </c>
       <c r="D13" s="80">
         <f>Calculations!D13</f>
-        <v>490.65454545454543</v>
+        <v>557.5272727272727</v>
       </c>
       <c r="E13" s="81" t="str">
         <f>ROUND(Calculations!E13,0)&amp;" ("&amp;ROUND(Calculations!F13,1)&amp;"%)"</f>
-        <v>494 (0.6%)</v>
+        <v>494 (-13%)</v>
       </c>
       <c r="F13" s="58" t="str">
         <f>ROUND(Calculations!G13,0)&amp;" ("&amp;ROUND(Calculations!H13,1)&amp;"%)"</f>
-        <v>498 (1.4%)</v>
+        <v>498 (-12.1%)</v>
       </c>
       <c r="G13" s="58" t="str">
         <f>ROUND(Calculations!I13,0)&amp;" ("&amp;ROUND(Calculations!J13,1)&amp;"%)"</f>
-        <v>435 (-12.8%)</v>
+        <v>435 (-28.2%)</v>
       </c>
       <c r="H13" s="58" t="str">
         <f>ROUND(Calculations!K13,0)&amp;" ("&amp;ROUND(Calculations!L13,1)&amp;"%)"</f>
-        <v>482 (-1.9%)</v>
+        <v>482 (-15.8%)</v>
       </c>
       <c r="I13" s="58" t="str">
         <f>ROUND(Calculations!M13,0)&amp;" ("&amp;ROUND(Calculations!N13,1)&amp;"%)"</f>
-        <v>401 (-22.4%)</v>
+        <v>401 (-39.1%)</v>
       </c>
       <c r="J13" s="58" t="str">
         <f>ROUND(Calculations!O13,0)&amp;" ("&amp;ROUND(Calculations!P13,1)&amp;"%)"</f>
-        <v>265 (-85%)</v>
+        <v>265 (-110.2%)</v>
       </c>
       <c r="K13" s="58" t="str">
         <f>ROUND(Calculations!Q13,0)&amp;" ("&amp;ROUND(Calculations!R13,1)&amp;"%)"</f>
-        <v>208 (-135.9%)</v>
+        <v>208 (-168%)</v>
       </c>
       <c r="L13" s="59" t="e">
         <f>ROUND(Calculations!S13,0)&amp;" ("&amp;ROUND(Calculations!T13,1)&amp;"%)"</f>
@@ -2130,39 +2142,39 @@
       </c>
       <c r="C14" s="80">
         <f>Calculations!C14</f>
-        <v>510.28</v>
+        <v>526.16999999999996</v>
       </c>
       <c r="D14" s="80">
         <f>Calculations!D14</f>
-        <v>927.78181818181804</v>
+        <v>956.67272727272712</v>
       </c>
       <c r="E14" s="81" t="str">
         <f>ROUND(Calculations!E14,0)&amp;" ("&amp;ROUND(Calculations!F14,1)&amp;"%)"</f>
-        <v>736 (-26%)</v>
+        <v>736 (-29.9%)</v>
       </c>
       <c r="F14" s="58" t="str">
         <f>ROUND(Calculations!G14,0)&amp;" ("&amp;ROUND(Calculations!H14,1)&amp;"%)"</f>
-        <v>738 (-25.7%)</v>
+        <v>738 (-29.6%)</v>
       </c>
       <c r="G14" s="58" t="str">
         <f>ROUND(Calculations!I14,0)&amp;" ("&amp;ROUND(Calculations!J14,1)&amp;"%)"</f>
-        <v>650 (-42.7%)</v>
+        <v>650 (-47.2%)</v>
       </c>
       <c r="H14" s="58" t="str">
         <f>ROUND(Calculations!K14,0)&amp;" ("&amp;ROUND(Calculations!L14,1)&amp;"%)"</f>
-        <v>627 (-47.9%)</v>
+        <v>627 (-52.5%)</v>
       </c>
       <c r="I14" s="58" t="str">
         <f>ROUND(Calculations!M14,0)&amp;" ("&amp;ROUND(Calculations!N14,1)&amp;"%)"</f>
-        <v>606 (-53.2%)</v>
+        <v>606 (-57.9%)</v>
       </c>
       <c r="J14" s="58" t="str">
         <f>ROUND(Calculations!O14,0)&amp;" ("&amp;ROUND(Calculations!P14,1)&amp;"%)"</f>
-        <v>532 (-74.5%)</v>
+        <v>532 (-79.9%)</v>
       </c>
       <c r="K14" s="58" t="str">
         <f>ROUND(Calculations!Q14,0)&amp;" ("&amp;ROUND(Calculations!R14,1)&amp;"%)"</f>
-        <v>319 (-190.8%)</v>
+        <v>319 (-199.9%)</v>
       </c>
       <c r="L14" s="59" t="e">
         <f>ROUND(Calculations!S14,0)&amp;" ("&amp;ROUND(Calculations!T14,1)&amp;"%)"</f>
@@ -2173,44 +2185,44 @@
       <c r="A15" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="94" t="s">
+      <c r="B15" s="92" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="80">
         <f>Calculations!C15</f>
-        <v>601.62</v>
+        <v>619.85</v>
       </c>
       <c r="D15" s="80">
         <f>Calculations!D15</f>
-        <v>1093.8545454545454</v>
+        <v>1127</v>
       </c>
       <c r="E15" s="82" t="str">
         <f>ROUND(Calculations!E15,0)&amp;" ("&amp;ROUND(Calculations!F15,1)&amp;"%)"</f>
-        <v>872 (-25.4%)</v>
+        <v>872 (-29.2%)</v>
       </c>
       <c r="F15" s="83" t="str">
         <f>ROUND(Calculations!G15,0)&amp;" ("&amp;ROUND(Calculations!H15,1)&amp;"%)"</f>
-        <v>868 (-26%)</v>
+        <v>868 (-29.8%)</v>
       </c>
       <c r="G15" s="83" t="str">
         <f>ROUND(Calculations!I15,0)&amp;" ("&amp;ROUND(Calculations!J15,1)&amp;"%)"</f>
-        <v>821 (-33.3%)</v>
+        <v>821 (-37.3%)</v>
       </c>
       <c r="H15" s="83" t="str">
         <f>ROUND(Calculations!K15,0)&amp;" ("&amp;ROUND(Calculations!L15,1)&amp;"%)"</f>
-        <v>811 (-34.8%)</v>
+        <v>811 (-38.9%)</v>
       </c>
       <c r="I15" s="83" t="str">
         <f>ROUND(Calculations!M15,0)&amp;" ("&amp;ROUND(Calculations!N15,1)&amp;"%)"</f>
-        <v>752 (-45.4%)</v>
+        <v>752 (-49.8%)</v>
       </c>
       <c r="J15" s="83" t="str">
         <f>ROUND(Calculations!O15,0)&amp;" ("&amp;ROUND(Calculations!P15,1)&amp;"%)"</f>
-        <v>555 (-97%)</v>
+        <v>555 (-102.9%)</v>
       </c>
       <c r="K15" s="83" t="str">
         <f>ROUND(Calculations!Q15,0)&amp;" ("&amp;ROUND(Calculations!R15,1)&amp;"%)"</f>
-        <v>450 (-143.1%)</v>
+        <v>450 (-150.4%)</v>
       </c>
       <c r="L15" s="84" t="e">
         <f>ROUND(Calculations!S15,0)&amp;" ("&amp;ROUND(Calculations!T15,1)&amp;"%)"</f>
@@ -2218,53 +2230,53 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="92" t="s">
+      <c r="A16" s="90" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="95" t="s">
+      <c r="C16" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="96" t="s">
+      <c r="D16" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="86" t="str">
+      <c r="E16" s="96" t="str">
         <f>ROUND(Calculations!F16,1)&amp;"%"</f>
-        <v>-24.1%</v>
-      </c>
-      <c r="F16" s="87" t="str">
+        <v>-29.7%</v>
+      </c>
+      <c r="F16" s="86" t="str">
         <f>ROUND(Calculations!H16,1)&amp;"%"</f>
-        <v>-24%</v>
-      </c>
-      <c r="G16" s="87" t="str">
+        <v>-29.6%</v>
+      </c>
+      <c r="G16" s="97" t="str">
         <f>ROUND(Calculations!J16,1)&amp;"%"</f>
-        <v>-35.9%</v>
-      </c>
-      <c r="H16" s="87" t="str">
+        <v>-41.1%</v>
+      </c>
+      <c r="H16" s="97" t="str">
         <f>ROUND(Calculations!L16,1)&amp;"%"</f>
-        <v>-15.2%</v>
-      </c>
-      <c r="I16" s="87" t="str">
+        <v>-22.2%</v>
+      </c>
+      <c r="I16" s="97" t="str">
         <f>ROUND(Calculations!N16,1)&amp;"%"</f>
-        <v>-58.5%</v>
-      </c>
-      <c r="J16" s="87" t="str">
+        <v>-66.7%</v>
+      </c>
+      <c r="J16" s="97" t="str">
         <f>ROUND(Calculations!P16,1)&amp;"%"</f>
-        <v>-128.7%</v>
-      </c>
-      <c r="K16" s="87" t="str">
+        <v>-139.3%</v>
+      </c>
+      <c r="K16" s="97" t="str">
         <f>ROUND(Calculations!R16,1)&amp;"%"</f>
-        <v>-290.6%</v>
-      </c>
-      <c r="L16" s="88" t="e">
+        <v>-290%</v>
+      </c>
+      <c r="L16" s="87" t="e">
         <f>ROUND(Calculations!T16,1)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="93" t="s">
+      <c r="A17" s="91" t="s">
         <v>39</v>
       </c>
       <c r="B17" s="56" t="s">
@@ -2276,69 +2288,69 @@
       <c r="D17" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="89" t="str">
+      <c r="E17" s="98" t="str">
         <f>ROUND(Calculations!F17,1)&amp;"%"</f>
-        <v>31.6%</v>
-      </c>
-      <c r="F17" s="90" t="str">
+        <v>30.4%</v>
+      </c>
+      <c r="F17" s="88" t="str">
         <f>ROUND(Calculations!H17,1)&amp;"%"</f>
-        <v>31.6%</v>
-      </c>
-      <c r="G17" s="90" t="str">
+        <v>30.3%</v>
+      </c>
+      <c r="G17" s="99" t="str">
         <f>ROUND(Calculations!J17,1)&amp;"%"</f>
-        <v>39.6%</v>
-      </c>
-      <c r="H17" s="90" t="str">
+        <v>41.1%</v>
+      </c>
+      <c r="H17" s="99" t="str">
         <f>ROUND(Calculations!L17,1)&amp;"%"</f>
-        <v>23.7%</v>
-      </c>
-      <c r="I17" s="90" t="str">
+        <v>28.8%</v>
+      </c>
+      <c r="I17" s="99" t="str">
         <f>ROUND(Calculations!N17,1)&amp;"%"</f>
-        <v>58.5%</v>
-      </c>
-      <c r="J17" s="90" t="str">
+        <v>66.7%</v>
+      </c>
+      <c r="J17" s="99" t="str">
         <f>ROUND(Calculations!P17,1)&amp;"%"</f>
-        <v>128.7%</v>
-      </c>
-      <c r="K17" s="90" t="str">
+        <v>139.3%</v>
+      </c>
+      <c r="K17" s="99" t="str">
         <f>ROUND(Calculations!R17,1)&amp;"%"</f>
-        <v>290.6%</v>
-      </c>
-      <c r="L17" s="91" t="e">
+        <v>290%</v>
+      </c>
+      <c r="L17" s="89" t="e">
         <f>ROUND(Calculations!T17,1)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="100" t="s">
+      <c r="A20" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="101"/>
-      <c r="C20" s="102"/>
+      <c r="B20" s="103"/>
+      <c r="C20" s="104"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="103" t="s">
+      <c r="B21" s="105" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="104"/>
+      <c r="C21" s="106"/>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="98" t="s">
+      <c r="B22" s="100" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="99"/>
+      <c r="C22" s="101"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="D27" s="97"/>
+      <c r="D27" s="95"/>
     </row>
     <row r="34" spans="7:7">
-      <c r="G34" s="97"/>
+      <c r="G34" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2352,10 +2364,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T32"/>
+  <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -2440,67 +2452,67 @@
         <v>13</v>
       </c>
       <c r="C2" s="36">
-        <v>126.95</v>
+        <v>161.22999999999999</v>
       </c>
       <c r="D2" s="8">
         <f t="shared" ref="D2:D15" si="0">C2/0.55</f>
-        <v>230.81818181818181</v>
+        <v>293.14545454545453</v>
       </c>
       <c r="E2" s="46">
         <v>284.02999999999997</v>
       </c>
       <c r="F2" s="9">
         <f>(E2-D2)/E2*100</f>
-        <v>18.734576693243024</v>
+        <v>-3.2093280799403425</v>
       </c>
       <c r="G2" s="48">
         <v>282.27999999999997</v>
       </c>
       <c r="H2" s="10">
         <f>(G2-D2)/G2*100</f>
-        <v>18.230770221701206</v>
+        <v>-3.8491761886972351</v>
       </c>
       <c r="I2" s="11">
         <v>261.14400000000001</v>
       </c>
       <c r="J2" s="11">
         <f>(I2-D2)/I2*100</f>
-        <v>11.612680429884735</v>
+        <v>-12.254332684440202</v>
       </c>
       <c r="K2" s="12">
         <v>247.298</v>
       </c>
       <c r="L2" s="12">
         <f>(K2-D2)/K2*100</f>
-        <v>6.663951257922907</v>
+        <v>-18.539355168846704</v>
       </c>
       <c r="M2" s="4">
         <v>175.1</v>
       </c>
       <c r="N2" s="13">
         <f>(M2-D2)/M2*100</f>
-        <v>-31.820777737396817</v>
+        <v>-67.416022013394937</v>
       </c>
       <c r="O2" s="5">
         <v>132.96</v>
       </c>
       <c r="P2" s="14">
         <f>(O2-D2)/O2*100</f>
-        <v>-73.599715567224578</v>
+        <v>-120.47642489880755</v>
       </c>
       <c r="Q2" s="6">
         <v>109</v>
       </c>
       <c r="R2" s="15">
         <f>(Q2-D2)/Q2*100</f>
-        <v>-111.75979983319434</v>
+        <v>-168.94078398665553</v>
       </c>
       <c r="S2" s="7">
         <v>396</v>
       </c>
       <c r="T2" s="44">
         <f>(S2-D2)/S2*100</f>
-        <v>41.712580348943987</v>
+        <v>25.973370064279163</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -2511,67 +2523,67 @@
         <v>15</v>
       </c>
       <c r="C3" s="36">
-        <v>136.82</v>
+        <v>165.19</v>
       </c>
       <c r="D3" s="8">
         <f t="shared" si="0"/>
-        <v>248.76363636363632</v>
+        <v>300.34545454545452</v>
       </c>
       <c r="E3" s="46">
         <v>261.19</v>
       </c>
       <c r="F3" s="9">
         <f t="shared" ref="F3:F15" si="1">(E3-D3)/E3*100</f>
-        <v>4.757595480823797</v>
+        <v>-14.991176746986683</v>
       </c>
       <c r="G3" s="48">
         <v>261.44</v>
       </c>
       <c r="H3" s="10">
         <f t="shared" ref="H3:H15" si="2">(G3-D3)/G3*100</f>
-        <v>4.8486703015466937</v>
+        <v>-14.881217313897842</v>
       </c>
       <c r="I3" s="11">
         <v>240.84</v>
       </c>
       <c r="J3" s="11">
         <f t="shared" ref="J3:J15" si="3">(I3-D3)/I3*100</f>
-        <v>-3.2900001509866801</v>
+        <v>-24.707463272485679</v>
       </c>
       <c r="K3" s="12">
         <v>246.30699999999999</v>
       </c>
       <c r="L3" s="12">
         <f t="shared" ref="L3:L15" si="4">(K3-D3)/K3*100</f>
-        <v>-0.99738796040564626</v>
+        <v>-21.939471694046265</v>
       </c>
       <c r="M3" s="4">
         <v>179.7</v>
       </c>
       <c r="N3" s="13">
         <f t="shared" ref="N3:N15" si="5">(M3-D3)/M3*100</f>
-        <v>-38.432741437749776</v>
+        <v>-67.137147771538423</v>
       </c>
       <c r="O3" s="5">
         <v>89.58</v>
       </c>
       <c r="P3" s="14">
         <f t="shared" ref="P3:P15" si="6">(O3-D3)/O3*100</f>
-        <v>-177.69997361424012</v>
+        <v>-235.281820211492</v>
       </c>
       <c r="Q3" s="6">
         <v>92</v>
       </c>
       <c r="R3" s="15">
         <f t="shared" ref="R3:R15" si="7">(Q3-D3)/Q3*100</f>
-        <v>-170.395256916996</v>
+        <v>-226.46245059288535</v>
       </c>
       <c r="S3" s="7">
         <v>267</v>
       </c>
       <c r="T3" s="44">
         <f t="shared" ref="T3:T15" si="8">(S3-D3)/S3*100</f>
-        <v>6.830098740211116</v>
+        <v>-12.488934286687083</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -2582,67 +2594,67 @@
         <v>17</v>
       </c>
       <c r="C4" s="36">
-        <v>121.71</v>
+        <v>141.15</v>
       </c>
       <c r="D4" s="8">
         <f t="shared" si="0"/>
-        <v>221.29090909090905</v>
+        <v>256.63636363636363</v>
       </c>
       <c r="E4" s="46">
         <v>270.38</v>
       </c>
       <c r="F4" s="9">
         <f t="shared" si="1"/>
-        <v>18.155592465822526</v>
+        <v>5.0830817233657708</v>
       </c>
       <c r="G4" s="48">
         <v>270.31</v>
       </c>
       <c r="H4" s="10">
         <f t="shared" si="2"/>
-        <v>18.134397879875308</v>
+        <v>5.0585018547728078</v>
       </c>
       <c r="I4" s="11">
         <v>252.50399999999999</v>
       </c>
       <c r="J4" s="11">
         <f t="shared" si="3"/>
-        <v>12.361424337472252</v>
+        <v>-1.6365537323621153</v>
       </c>
       <c r="K4" s="12">
         <v>277.21300000000002</v>
       </c>
       <c r="L4" s="12">
         <f t="shared" si="4"/>
-        <v>20.172968406637121</v>
+        <v>7.4226808856858781</v>
       </c>
       <c r="M4" s="4">
         <v>190.5</v>
       </c>
       <c r="N4" s="13">
         <f t="shared" si="5"/>
-        <v>-16.163206871868269</v>
+        <v>-34.717251252684314</v>
       </c>
       <c r="O4" s="5">
         <v>112.77</v>
       </c>
       <c r="P4" s="14">
         <f t="shared" si="6"/>
-        <v>-96.23207332704537</v>
+        <v>-127.5750320443058</v>
       </c>
       <c r="Q4" s="6">
         <v>99</v>
       </c>
       <c r="R4" s="15">
         <f t="shared" si="7"/>
-        <v>-123.52617079889802</v>
+        <v>-159.22865013774103</v>
       </c>
       <c r="S4" s="7">
         <v>335</v>
       </c>
       <c r="T4" s="44">
         <f t="shared" si="8"/>
-        <v>33.943012211668936</v>
+        <v>23.392130257801902</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -2653,67 +2665,67 @@
         <v>19</v>
       </c>
       <c r="C5" s="36">
-        <v>257.93</v>
+        <v>309.69</v>
       </c>
       <c r="D5" s="8">
         <f t="shared" si="0"/>
-        <v>468.96363636363634</v>
+        <v>563.07272727272721</v>
       </c>
       <c r="E5" s="46">
         <v>412.91</v>
       </c>
       <c r="F5" s="9">
         <f t="shared" si="1"/>
-        <v>-13.575267337588413</v>
+        <v>-36.366938866272832</v>
       </c>
       <c r="G5" s="48">
         <v>412.67</v>
       </c>
       <c r="H5" s="10">
         <f t="shared" si="2"/>
-        <v>-13.641320271315172</v>
+        <v>-36.446246946162105</v>
       </c>
       <c r="I5" s="11">
         <v>410.4</v>
       </c>
       <c r="J5" s="11">
         <f t="shared" si="3"/>
-        <v>-14.269891901470849</v>
+        <v>-37.200956937799035</v>
       </c>
       <c r="K5" s="12">
         <v>434.423</v>
       </c>
       <c r="L5" s="12">
         <f t="shared" si="4"/>
-        <v>-7.9509225716954068</v>
+        <v>-29.613930955020155</v>
       </c>
       <c r="M5" s="4">
         <v>343</v>
       </c>
       <c r="N5" s="13">
         <f t="shared" si="5"/>
-        <v>-36.724092234296307</v>
+        <v>-64.16114497747148</v>
       </c>
       <c r="O5" s="5">
         <v>250.72</v>
       </c>
       <c r="P5" s="14">
         <f t="shared" si="6"/>
-        <v>-87.046759877008753</v>
+        <v>-124.58229390265123</v>
       </c>
       <c r="Q5" s="6">
         <v>222</v>
       </c>
       <c r="R5" s="15">
         <f t="shared" si="7"/>
-        <v>-111.24488124488123</v>
+        <v>-153.63636363636363</v>
       </c>
       <c r="S5" s="7">
         <v>474</v>
       </c>
       <c r="T5" s="44">
         <f t="shared" si="8"/>
-        <v>1.0625239739163839</v>
+        <v>-18.791714614499412</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -2724,60 +2736,60 @@
         <v>21</v>
       </c>
       <c r="C6" s="36">
-        <v>57.4</v>
+        <v>55.06</v>
       </c>
       <c r="D6" s="8">
         <f t="shared" si="0"/>
-        <v>104.36363636363635</v>
+        <v>100.10909090909091</v>
       </c>
       <c r="E6" s="46">
         <v>78.66</v>
       </c>
       <c r="F6" s="9">
         <f t="shared" si="1"/>
-        <v>-32.676883248965609</v>
+        <v>-27.268104384809195</v>
       </c>
       <c r="G6" s="48">
         <v>78.03</v>
       </c>
       <c r="H6" s="10">
         <f t="shared" si="2"/>
-        <v>-33.74809222560085</v>
+        <v>-28.295643866578118</v>
       </c>
       <c r="I6" s="11">
         <v>43.847999999999999</v>
       </c>
       <c r="J6" s="11">
         <f t="shared" si="3"/>
-        <v>-138.01230697782418</v>
+        <v>-128.30936624040072</v>
       </c>
       <c r="K6" s="12">
         <v>84.33</v>
       </c>
       <c r="L6" s="12">
         <f t="shared" si="4"/>
-        <v>-23.756239017711785</v>
+        <v>-18.711124047303347</v>
       </c>
       <c r="M6" s="4">
         <v>29.2</v>
       </c>
       <c r="N6" s="13">
         <f t="shared" si="5"/>
-        <v>-257.40971357409705</v>
+        <v>-242.83935242839351</v>
       </c>
       <c r="O6" s="5">
         <v>36.770000000000003</v>
       </c>
       <c r="P6" s="14">
         <f t="shared" si="6"/>
-        <v>-183.82821964546187</v>
+        <v>-172.25752218953195</v>
       </c>
       <c r="Q6" s="6">
         <v>10.5</v>
       </c>
       <c r="R6" s="15">
         <f t="shared" si="7"/>
-        <v>-893.93939393939377</v>
+        <v>-853.41991341991343</v>
       </c>
       <c r="S6" s="7"/>
       <c r="T6" s="44" t="e">
@@ -2793,60 +2805,60 @@
         <v>23</v>
       </c>
       <c r="C7" s="36">
-        <v>83.64</v>
+        <v>66.59</v>
       </c>
       <c r="D7" s="8">
         <f t="shared" si="0"/>
-        <v>152.07272727272726</v>
+        <v>121.07272727272726</v>
       </c>
       <c r="E7" s="46">
         <v>80.25</v>
       </c>
       <c r="F7" s="9">
         <f t="shared" si="1"/>
-        <v>-89.498725573491924</v>
+        <v>-50.869442084395345</v>
       </c>
       <c r="G7" s="48">
         <v>81.17</v>
       </c>
       <c r="H7" s="10">
         <f t="shared" si="2"/>
-        <v>-87.350902147009066</v>
+        <v>-49.159452103889691</v>
       </c>
       <c r="I7" s="11">
         <v>55.08</v>
       </c>
       <c r="J7" s="11">
         <f t="shared" si="3"/>
-        <v>-176.09427609427607</v>
+        <v>-119.81250412622961</v>
       </c>
       <c r="K7" s="12">
         <v>82.099000000000004</v>
       </c>
       <c r="L7" s="12">
         <f t="shared" si="4"/>
-        <v>-85.230913010788512</v>
+        <v>-47.471622398235368</v>
       </c>
       <c r="M7" s="4">
         <v>63.5</v>
       </c>
       <c r="N7" s="13">
         <f t="shared" si="5"/>
-        <v>-139.48460987831066</v>
+        <v>-90.665712240515376</v>
       </c>
       <c r="O7" s="5">
         <v>39.5</v>
       </c>
       <c r="P7" s="14">
         <f t="shared" si="6"/>
-        <v>-284.99424626006902</v>
+        <v>-206.51323360184119</v>
       </c>
       <c r="Q7" s="6">
         <v>10.75</v>
       </c>
       <c r="R7" s="15">
         <f t="shared" si="7"/>
-        <v>-1314.630021141649</v>
+        <v>-1026.2579281183932</v>
       </c>
       <c r="S7" s="7"/>
       <c r="T7" s="44" t="e">
@@ -2862,60 +2874,60 @@
         <v>25</v>
       </c>
       <c r="C8" s="36">
-        <v>505.05</v>
+        <v>520.71</v>
       </c>
       <c r="D8" s="8">
         <f t="shared" si="0"/>
-        <v>918.27272727272725</v>
+        <v>946.74545454545455</v>
       </c>
       <c r="E8" s="46">
         <v>754.91</v>
       </c>
       <c r="F8" s="9">
         <f t="shared" si="1"/>
-        <v>-21.640026926749851</v>
+        <v>-25.41169868533396</v>
       </c>
       <c r="G8" s="48">
         <v>758.8</v>
       </c>
       <c r="H8" s="10">
         <f t="shared" si="2"/>
-        <v>-21.016437437101647</v>
+        <v>-24.768773661762602</v>
       </c>
       <c r="I8" s="50">
         <v>708.048</v>
       </c>
       <c r="J8" s="11">
         <f t="shared" si="3"/>
-        <v>-29.690745157493168</v>
+        <v>-33.712044175741553</v>
       </c>
       <c r="K8" s="12">
         <v>770.98</v>
       </c>
       <c r="L8" s="12">
         <f t="shared" si="4"/>
-        <v>-19.104610660811854</v>
+        <v>-22.797667195706055</v>
       </c>
       <c r="M8" s="16">
         <v>733.7</v>
       </c>
       <c r="N8" s="13">
         <f t="shared" si="5"/>
-        <v>-25.156430049438079</v>
+        <v>-29.037134325399279</v>
       </c>
       <c r="O8" s="17">
         <v>491.73</v>
       </c>
       <c r="P8" s="14">
         <f t="shared" si="6"/>
-        <v>-86.743279294069353</v>
+        <v>-92.533596596801999</v>
       </c>
       <c r="Q8" s="18">
         <v>385</v>
       </c>
       <c r="R8" s="15">
         <f t="shared" si="7"/>
-        <v>-138.51239669421486</v>
+        <v>-145.90791027154663</v>
       </c>
       <c r="S8" s="19"/>
       <c r="T8" s="44" t="e">
@@ -2931,60 +2943,60 @@
         <v>25</v>
       </c>
       <c r="C9" s="36">
-        <v>498.11</v>
+        <v>513.66999999999996</v>
       </c>
       <c r="D9" s="8">
         <f t="shared" si="0"/>
-        <v>905.65454545454543</v>
+        <v>933.94545454545437</v>
       </c>
       <c r="E9" s="46">
         <v>729.69</v>
       </c>
       <c r="F9" s="9">
         <f t="shared" si="1"/>
-        <v>-24.114972858960019</v>
+        <v>-27.992086303149872</v>
       </c>
       <c r="G9" s="48">
         <v>730.2</v>
       </c>
       <c r="H9" s="10">
         <f t="shared" si="2"/>
-        <v>-24.028286148253269</v>
+        <v>-27.902691666044138</v>
       </c>
       <c r="I9" s="11">
         <v>747.36</v>
       </c>
       <c r="J9" s="11">
         <f t="shared" si="3"/>
-        <v>-21.180494735408022</v>
+        <v>-24.965940717385777</v>
       </c>
       <c r="K9" s="12">
         <v>804.54399999999998</v>
       </c>
       <c r="L9" s="12">
         <f t="shared" si="4"/>
-        <v>-12.567435150165243</v>
+        <v>-16.083825688272409</v>
       </c>
       <c r="M9" s="4">
         <v>704</v>
       </c>
       <c r="N9" s="13">
         <f t="shared" si="5"/>
-        <v>-28.644111570247933</v>
+        <v>-32.662706611570222</v>
       </c>
       <c r="O9" s="5">
         <v>517.11</v>
       </c>
       <c r="P9" s="14">
         <f t="shared" si="6"/>
-        <v>-75.137697096274565</v>
+        <v>-80.608662479057529</v>
       </c>
       <c r="Q9" s="6">
         <v>409</v>
       </c>
       <c r="R9" s="15">
         <f t="shared" si="7"/>
-        <v>-121.43142920649032</v>
+        <v>-128.34852189375411</v>
       </c>
       <c r="S9" s="7"/>
       <c r="T9" s="44" t="e">
@@ -3000,60 +3012,60 @@
         <v>28</v>
       </c>
       <c r="C10" s="36">
-        <v>137.37</v>
+        <v>151.88999999999999</v>
       </c>
       <c r="D10" s="8">
         <f t="shared" si="0"/>
-        <v>249.76363636363635</v>
+        <v>276.16363636363633</v>
       </c>
       <c r="E10" s="46">
         <v>155.91999999999999</v>
       </c>
       <c r="F10" s="9">
         <f t="shared" si="1"/>
-        <v>-60.187042306077707</v>
+        <v>-77.118802182937628</v>
       </c>
       <c r="G10" s="48">
         <v>154.52000000000001</v>
       </c>
       <c r="H10" s="10">
         <f t="shared" si="2"/>
-        <v>-61.638387499117485</v>
+        <v>-78.723554467794671</v>
       </c>
       <c r="I10" s="11">
         <v>176.904</v>
       </c>
       <c r="J10" s="11">
         <f t="shared" si="3"/>
-        <v>-41.185974519307848</v>
+        <v>-56.109322775989426</v>
       </c>
       <c r="K10" s="12">
         <v>180.93700000000001</v>
       </c>
       <c r="L10" s="12">
         <f t="shared" si="4"/>
-        <v>-38.039006042786347</v>
+        <v>-52.629719937677933</v>
       </c>
       <c r="M10" s="4">
         <v>159.19999999999999</v>
       </c>
       <c r="N10" s="13">
         <f t="shared" si="5"/>
-        <v>-56.886706258565553</v>
+        <v>-73.469620831429864</v>
       </c>
       <c r="O10" s="5">
         <v>122.15</v>
       </c>
       <c r="P10" s="14">
         <f t="shared" si="6"/>
-        <v>-104.47289100584227</v>
+        <v>-126.08566218881401</v>
       </c>
       <c r="Q10" s="6">
         <v>62</v>
       </c>
       <c r="R10" s="15">
         <f t="shared" si="7"/>
-        <v>-302.84457478005862</v>
+        <v>-345.42521994134893</v>
       </c>
       <c r="S10" s="7"/>
       <c r="T10" s="44" t="e">
@@ -3069,60 +3081,60 @@
         <v>13</v>
       </c>
       <c r="C11" s="36">
-        <v>121.6</v>
+        <v>150.5</v>
       </c>
       <c r="D11" s="8">
         <f t="shared" si="0"/>
-        <v>221.09090909090907</v>
+        <v>273.63636363636363</v>
       </c>
       <c r="E11" s="46">
         <v>246.16</v>
       </c>
       <c r="F11" s="9">
         <f t="shared" si="1"/>
-        <v>10.184063580228685</v>
+        <v>-11.161993677430788</v>
       </c>
       <c r="G11" s="48">
         <v>247.81</v>
       </c>
       <c r="H11" s="10">
         <f t="shared" si="2"/>
-        <v>10.782087449695709</v>
+        <v>-10.421840779776289</v>
       </c>
       <c r="I11" s="11">
         <v>225.28800000000001</v>
       </c>
       <c r="J11" s="11">
         <f t="shared" si="3"/>
-        <v>1.8629891113112751</v>
+        <v>-21.460691930490576</v>
       </c>
       <c r="K11" s="12">
         <v>225.29400000000001</v>
       </c>
       <c r="L11" s="12">
         <f t="shared" si="4"/>
-        <v>1.8656026832010377</v>
+        <v>-21.457457205413199</v>
       </c>
       <c r="M11" s="4">
         <v>161.30000000000001</v>
       </c>
       <c r="N11" s="13">
         <f t="shared" si="5"/>
-        <v>-37.068139547990732</v>
+        <v>-69.64436679253788</v>
       </c>
       <c r="O11" s="5">
         <v>124.64</v>
       </c>
       <c r="P11" s="14">
         <f t="shared" si="6"/>
-        <v>-77.383592017738337</v>
+        <v>-119.54137005484888</v>
       </c>
       <c r="Q11" s="6">
         <v>94</v>
       </c>
       <c r="R11" s="15">
         <f t="shared" si="7"/>
-        <v>-135.20309477756282</v>
+        <v>-191.10251450676981</v>
       </c>
       <c r="S11" s="7"/>
       <c r="T11" s="44" t="e">
@@ -3138,60 +3150,60 @@
         <v>31</v>
       </c>
       <c r="C12" s="36">
-        <v>248.63</v>
+        <v>219.71</v>
       </c>
       <c r="D12" s="8">
         <f t="shared" si="0"/>
-        <v>452.0545454545454</v>
+        <v>399.47272727272724</v>
       </c>
       <c r="E12" s="46">
         <v>229.11</v>
       </c>
       <c r="F12" s="9">
         <f t="shared" si="1"/>
-        <v>-97.308954412529076</v>
+        <v>-74.358485999182591</v>
       </c>
       <c r="G12" s="48">
         <v>230.03</v>
       </c>
       <c r="H12" s="10">
         <f t="shared" si="2"/>
-        <v>-96.51982152525558</v>
+        <v>-73.661143012966676</v>
       </c>
       <c r="I12" s="11">
         <v>389.23200000000003</v>
       </c>
       <c r="J12" s="11">
         <f t="shared" si="3"/>
-        <v>-16.14012862625513</v>
+        <v>-2.6310085688553904</v>
       </c>
       <c r="K12" s="12">
         <v>652.13199999999995</v>
       </c>
       <c r="L12" s="12">
         <f t="shared" si="4"/>
-        <v>30.680514764718581</v>
+        <v>38.743578405487341</v>
       </c>
       <c r="M12" s="4">
         <v>348.7</v>
       </c>
       <c r="N12" s="13">
         <f t="shared" si="5"/>
-        <v>-29.639961415126304</v>
+        <v>-14.560575644602022</v>
       </c>
       <c r="O12" s="5">
         <v>113.53</v>
       </c>
       <c r="P12" s="14">
         <f t="shared" si="6"/>
-        <v>-298.180697132516</v>
+        <v>-251.86534596382208</v>
       </c>
       <c r="Q12" s="6">
         <v>164</v>
       </c>
       <c r="R12" s="15">
         <f t="shared" si="7"/>
-        <v>-175.64301552106429</v>
+        <v>-143.58093126385808</v>
       </c>
       <c r="S12" s="7"/>
       <c r="T12" s="44" t="e">
@@ -3207,60 +3219,60 @@
         <v>33</v>
       </c>
       <c r="C13" s="36">
-        <v>269.86</v>
+        <v>306.64</v>
       </c>
       <c r="D13" s="8">
         <f t="shared" si="0"/>
-        <v>490.65454545454543</v>
+        <v>557.5272727272727</v>
       </c>
       <c r="E13" s="46">
         <v>493.58</v>
       </c>
       <c r="F13" s="9">
         <f t="shared" si="1"/>
-        <v>0.59270119240134456</v>
+        <v>-12.955807108730646</v>
       </c>
       <c r="G13" s="48">
         <v>497.5</v>
       </c>
       <c r="H13" s="10">
         <f t="shared" si="2"/>
-        <v>1.3759707629054418</v>
+        <v>-12.065783462768383</v>
       </c>
       <c r="I13" s="11">
         <v>434.80799999999999</v>
       </c>
       <c r="J13" s="11">
         <f t="shared" si="3"/>
-        <v>-12.843955367551985</v>
+        <v>-28.223784458260358</v>
       </c>
       <c r="K13" s="12">
         <v>481.536</v>
       </c>
       <c r="L13" s="12">
         <f t="shared" si="4"/>
-        <v>-1.8936373302401954</v>
+        <v>-15.781015900633118</v>
       </c>
       <c r="M13" s="4">
         <v>400.9</v>
       </c>
       <c r="N13" s="13">
         <f t="shared" si="5"/>
-        <v>-22.388262772398466</v>
+        <v>-39.068913127281803</v>
       </c>
       <c r="O13" s="5">
         <v>265.24</v>
       </c>
       <c r="P13" s="14">
         <f t="shared" si="6"/>
-        <v>-84.985124964011987</v>
+        <v>-110.19728273536144</v>
       </c>
       <c r="Q13" s="6">
         <v>208</v>
       </c>
       <c r="R13" s="15">
         <f t="shared" si="7"/>
-        <v>-135.8916083916084</v>
+        <v>-168.04195804195803</v>
       </c>
       <c r="S13" s="7"/>
       <c r="T13" s="44" t="e">
@@ -3276,60 +3288,60 @@
         <v>25</v>
       </c>
       <c r="C14" s="36">
-        <v>510.28</v>
+        <v>526.16999999999996</v>
       </c>
       <c r="D14" s="8">
         <f t="shared" si="0"/>
-        <v>927.78181818181804</v>
+        <v>956.67272727272712</v>
       </c>
       <c r="E14" s="46">
         <v>736.31</v>
       </c>
       <c r="F14" s="9">
         <f t="shared" si="1"/>
-        <v>-26.004239814998858</v>
+        <v>-29.927982408595184</v>
       </c>
       <c r="G14" s="48">
         <v>738.33</v>
       </c>
       <c r="H14" s="10">
         <f t="shared" si="2"/>
-        <v>-25.659504311326643</v>
+        <v>-29.572511921867871</v>
       </c>
       <c r="I14" s="11">
         <v>649.94399999999996</v>
       </c>
       <c r="J14" s="11">
         <f t="shared" si="3"/>
-        <v>-42.747962621674809</v>
+        <v>-47.193100832183568</v>
       </c>
       <c r="K14" s="12">
         <v>627.39200000000005</v>
       </c>
       <c r="L14" s="12">
         <f t="shared" si="4"/>
-        <v>-47.879127910750846</v>
+        <v>-52.484049409735391</v>
       </c>
       <c r="M14" s="4">
         <v>605.70000000000005</v>
       </c>
       <c r="N14" s="13">
         <f t="shared" si="5"/>
-        <v>-53.175139207828629</v>
+        <v>-57.944977261470541</v>
       </c>
       <c r="O14" s="5">
         <v>531.75</v>
       </c>
       <c r="P14" s="14">
         <f t="shared" si="6"/>
-        <v>-74.477069709791834</v>
+        <v>-79.910244903192691</v>
       </c>
       <c r="Q14" s="6">
         <v>319</v>
       </c>
       <c r="R14" s="15">
         <f t="shared" si="7"/>
-        <v>-190.84069535480191</v>
+        <v>-199.8974066685665</v>
       </c>
       <c r="S14" s="7"/>
       <c r="T14" s="44" t="e">
@@ -3345,60 +3357,60 @@
         <v>36</v>
       </c>
       <c r="C15" s="37">
-        <v>601.62</v>
+        <v>619.85</v>
       </c>
       <c r="D15" s="38">
         <f t="shared" si="0"/>
-        <v>1093.8545454545454</v>
+        <v>1127</v>
       </c>
       <c r="E15" s="47">
         <v>872.31</v>
       </c>
       <c r="F15" s="39">
         <f t="shared" si="1"/>
-        <v>-25.397455658486713</v>
+        <v>-29.197189072692055</v>
       </c>
       <c r="G15" s="49">
         <v>868.19</v>
       </c>
       <c r="H15" s="10">
         <f t="shared" si="2"/>
-        <v>-25.992529913330642</v>
+        <v>-29.810294981513252</v>
       </c>
       <c r="I15" s="51">
         <v>820.58399999999995</v>
       </c>
       <c r="J15" s="11">
         <f t="shared" si="3"/>
-        <v>-33.301958782348358</v>
+        <v>-37.341210649976126</v>
       </c>
       <c r="K15" s="12">
         <v>811.38800000000003</v>
       </c>
       <c r="L15" s="12">
         <f t="shared" si="4"/>
-        <v>-34.812758563664403</v>
+        <v>-38.897789959920523</v>
       </c>
       <c r="M15" s="40">
         <v>752.1</v>
       </c>
       <c r="N15" s="13">
         <f t="shared" si="5"/>
-        <v>-45.440040613554757</v>
+        <v>-49.847094801223236</v>
       </c>
       <c r="O15" s="41">
         <v>555.38</v>
       </c>
       <c r="P15" s="14">
         <f t="shared" si="6"/>
-        <v>-96.956056295607567</v>
+        <v>-102.92412402319133</v>
       </c>
       <c r="Q15" s="42">
         <v>450</v>
       </c>
       <c r="R15" s="15">
         <f t="shared" si="7"/>
-        <v>-143.07878787878786</v>
+        <v>-150.44444444444446</v>
       </c>
       <c r="S15" s="43"/>
       <c r="T15" s="44" t="e">
@@ -3407,45 +3419,45 @@
       </c>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="106" t="s">
+      <c r="A16" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="106"/>
+      <c r="B16" s="108"/>
       <c r="C16" s="54"/>
       <c r="D16" s="55"/>
       <c r="F16" s="53">
         <f>AVERAGE(F2:F15)</f>
-        <v>-24.141359908952058</v>
+        <v>-29.696139562649389</v>
       </c>
       <c r="G16" s="53"/>
       <c r="H16" s="53">
         <f t="shared" ref="H16:T16" si="9">AVERAGE(H2:H15)</f>
-        <v>-24.015956061613284</v>
+        <v>-29.607130608496153</v>
       </c>
       <c r="I16" s="53"/>
       <c r="J16" s="53">
         <f t="shared" si="9"/>
-        <v>-35.922900075423492</v>
+        <v>-41.11130579304286</v>
       </c>
       <c r="K16" s="53"/>
       <c r="L16" s="53">
         <f t="shared" si="9"/>
-        <v>-15.20350007903861</v>
+        <v>-22.160055019259804</v>
       </c>
       <c r="M16" s="53"/>
       <c r="N16" s="53">
         <f t="shared" si="9"/>
-        <v>-58.459566654919236</v>
+        <v>-66.655144291393782</v>
       </c>
       <c r="O16" s="53"/>
       <c r="P16" s="53">
         <f t="shared" si="9"/>
-        <v>-128.69552827192152</v>
+        <v>-139.31090112812282</v>
       </c>
       <c r="Q16" s="53"/>
       <c r="R16" s="53">
         <f t="shared" si="9"/>
-        <v>-290.63865189140012</v>
+        <v>-290.04964263744279</v>
       </c>
       <c r="S16" s="53"/>
       <c r="T16" s="53" t="e">
@@ -3454,46 +3466,46 @@
       </c>
     </row>
     <row r="17" spans="1:20">
-      <c r="A17" s="105" t="s">
+      <c r="A17" s="107" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="105"/>
+      <c r="B17" s="107"/>
       <c r="C17" s="45"/>
       <c r="D17" s="45"/>
       <c r="E17" s="52"/>
       <c r="F17" s="53" cm="1">
         <f t="array" ref="F17">AVERAGE(ABS(F2:F15))</f>
-        <v>31.630578396454826</v>
+        <v>30.422294094558783</v>
       </c>
       <c r="G17" s="53"/>
       <c r="H17" s="53" cm="1">
         <f t="array" ref="H17">AVERAGE(ABS(H2:H15))</f>
-        <v>31.640512721002484</v>
+        <v>30.329773730606547</v>
       </c>
       <c r="I17" s="53"/>
       <c r="J17" s="53" cm="1">
         <f t="array" ref="J17">AVERAGE(ABS(J2:J15))</f>
-        <v>39.613913486661815</v>
+        <v>41.11130579304286</v>
       </c>
       <c r="K17" s="53"/>
       <c r="L17" s="53" cm="1">
         <f t="array" ref="L17">AVERAGE(ABS(L2:L15))</f>
-        <v>23.686791095107132</v>
+        <v>28.755234917998838</v>
       </c>
       <c r="M17" s="53"/>
       <c r="N17" s="53" cm="1">
         <f t="array" ref="N17">AVERAGE(ABS(N2:N15))</f>
-        <v>58.459566654919236</v>
+        <v>66.655144291393782</v>
       </c>
       <c r="O17" s="53"/>
       <c r="P17" s="53" cm="1">
         <f t="array" ref="P17">AVERAGE(ABS(P2:P15))</f>
-        <v>128.69552827192152</v>
+        <v>139.31090112812282</v>
       </c>
       <c r="Q17" s="53"/>
       <c r="R17" s="53" cm="1">
         <f t="array" ref="R17">AVERAGE(ABS(R2:R15))</f>
-        <v>290.63865189140012</v>
+        <v>290.04964263744279</v>
       </c>
       <c r="S17" s="53"/>
       <c r="T17" s="53" t="e" cm="1">
@@ -3501,11 +3513,49 @@
         <v>#DIV/0!</v>
       </c>
     </row>
+    <row r="23" spans="1:20">
+      <c r="C23" s="109"/>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="C24" s="109"/>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="C25" s="109"/>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="C26" s="109"/>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="C27" s="109"/>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="C28" s="109"/>
+    </row>
     <row r="29" spans="1:20">
+      <c r="C29" s="109"/>
       <c r="J29" s="60"/>
     </row>
+    <row r="30" spans="1:20">
+      <c r="C30" s="109"/>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="C31" s="109"/>
+    </row>
     <row r="32" spans="1:20">
+      <c r="C32" s="109"/>
       <c r="E32" s="60"/>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" s="109"/>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" s="109"/>
+    </row>
+    <row r="35" spans="3:3">
+      <c r="C35" s="109"/>
+    </row>
+    <row r="36" spans="3:3">
+      <c r="C36" s="109"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
Update guests' volume estimation using ChimeraX to define vdW radius of atoms
</commit_message>
<xml_diff>
--- a/results/quantitative-analysis.xlsx
+++ b/results/quantitative-analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gyorgy Szaloki\Papers\Cavity calculations\Benchmarking\Structures for benchmarking\QUANTITATIVE ANALYSIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7543670-3C34-44CA-998E-BD6F43F9A73E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F864CA71-932A-4633-B7BB-4346757AD65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -807,7 +807,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1100,6 +1100,7 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1127,7 +1128,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1510,7 +1516,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1566,43 +1572,43 @@
       </c>
       <c r="C2" s="80">
         <f>Calculations!C2</f>
-        <v>161.22999999999999</v>
+        <v>137.38999999999999</v>
       </c>
       <c r="D2" s="80">
         <f>Calculations!D2</f>
-        <v>293.14545454545453</v>
+        <v>249.79999999999995</v>
       </c>
       <c r="E2" s="81" t="str">
         <f>ROUND(Calculations!E2,0)&amp;" ("&amp;ROUND(Calculations!F2,1)&amp;"%)"</f>
-        <v>284 (-3.2%)</v>
+        <v>284 (12.1%)</v>
       </c>
       <c r="F2" s="58" t="str">
         <f>ROUND(Calculations!G2,0)&amp;" ("&amp;ROUND(Calculations!H2,1)&amp;"%)"</f>
-        <v>282 (-3.8%)</v>
+        <v>282 (11.5%)</v>
       </c>
       <c r="G2" s="58" t="str">
         <f>ROUND(Calculations!I2,0)&amp;" ("&amp;ROUND(Calculations!J2,1)&amp;"%)"</f>
-        <v>261 (-12.3%)</v>
+        <v>261 (4.3%)</v>
       </c>
       <c r="H2" s="58" t="str">
         <f>ROUND(Calculations!K2,0)&amp;" ("&amp;ROUND(Calculations!L2,1)&amp;"%)"</f>
-        <v>247 (-18.5%)</v>
+        <v>247 (-1%)</v>
       </c>
       <c r="I2" s="58" t="str">
         <f>ROUND(Calculations!M2,0)&amp;" ("&amp;ROUND(Calculations!N2,1)&amp;"%)"</f>
-        <v>175 (-67.4%)</v>
+        <v>175 (-42.7%)</v>
       </c>
       <c r="J2" s="58" t="str">
         <f>ROUND(Calculations!O2,0)&amp;" ("&amp;ROUND(Calculations!P2,1)&amp;"%)"</f>
-        <v>133 (-120.5%)</v>
+        <v>133 (-87.9%)</v>
       </c>
       <c r="K2" s="58" t="str">
         <f>ROUND(Calculations!Q2,0)&amp;" ("&amp;ROUND(Calculations!R2,1)&amp;"%)"</f>
-        <v>109 (-168.9%)</v>
+        <v>109 (-129.2%)</v>
       </c>
       <c r="L2" s="59" t="str">
         <f>ROUND(Calculations!S2,0)&amp;" ("&amp;ROUND(Calculations!T2,1)&amp;"%)"</f>
-        <v>396 (26%)</v>
+        <v>396 (36.9%)</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1614,43 +1620,43 @@
       </c>
       <c r="C3" s="80">
         <f>Calculations!C3</f>
-        <v>165.19</v>
+        <v>146.03</v>
       </c>
       <c r="D3" s="80">
         <f>Calculations!D3</f>
-        <v>300.34545454545452</v>
+        <v>265.5090909090909</v>
       </c>
       <c r="E3" s="81" t="str">
         <f>ROUND(Calculations!E3,0)&amp;" ("&amp;ROUND(Calculations!F3,1)&amp;"%)"</f>
-        <v>261 (-15%)</v>
+        <v>261 (-1.7%)</v>
       </c>
       <c r="F3" s="58" t="str">
         <f>ROUND(Calculations!G3,0)&amp;" ("&amp;ROUND(Calculations!H3,1)&amp;"%)"</f>
-        <v>261 (-14.9%)</v>
+        <v>261 (-1.6%)</v>
       </c>
       <c r="G3" s="58" t="str">
         <f>ROUND(Calculations!I3,0)&amp;" ("&amp;ROUND(Calculations!J3,1)&amp;"%)"</f>
-        <v>241 (-24.7%)</v>
+        <v>241 (-10.2%)</v>
       </c>
       <c r="H3" s="58" t="str">
         <f>ROUND(Calculations!K3,0)&amp;" ("&amp;ROUND(Calculations!L3,1)&amp;"%)"</f>
-        <v>246 (-21.9%)</v>
+        <v>246 (-7.8%)</v>
       </c>
       <c r="I3" s="58" t="str">
         <f>ROUND(Calculations!M3,0)&amp;" ("&amp;ROUND(Calculations!N3,1)&amp;"%)"</f>
-        <v>180 (-67.1%)</v>
+        <v>180 (-47.8%)</v>
       </c>
       <c r="J3" s="58" t="str">
         <f>ROUND(Calculations!O3,0)&amp;" ("&amp;ROUND(Calculations!P3,1)&amp;"%)"</f>
-        <v>90 (-235.3%)</v>
+        <v>90 (-196.4%)</v>
       </c>
       <c r="K3" s="58" t="str">
         <f>ROUND(Calculations!Q3,0)&amp;" ("&amp;ROUND(Calculations!R3,1)&amp;"%)"</f>
-        <v>92 (-226.5%)</v>
+        <v>92 (-188.6%)</v>
       </c>
       <c r="L3" s="59" t="str">
         <f>ROUND(Calculations!S3,0)&amp;" ("&amp;ROUND(Calculations!T3,1)&amp;"%)"</f>
-        <v>267 (-12.5%)</v>
+        <v>267 (0.6%)</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1662,43 +1668,43 @@
       </c>
       <c r="C4" s="80">
         <f>Calculations!C4</f>
-        <v>141.15</v>
+        <v>129.1</v>
       </c>
       <c r="D4" s="80">
         <f>Calculations!D4</f>
-        <v>256.63636363636363</v>
+        <v>234.72727272727269</v>
       </c>
       <c r="E4" s="81" t="str">
         <f>ROUND(Calculations!E4,0)&amp;" ("&amp;ROUND(Calculations!F4,1)&amp;"%)"</f>
-        <v>270 (5.1%)</v>
+        <v>270 (13.2%)</v>
       </c>
       <c r="F4" s="58" t="str">
         <f>ROUND(Calculations!G4,0)&amp;" ("&amp;ROUND(Calculations!H4,1)&amp;"%)"</f>
-        <v>270 (5.1%)</v>
+        <v>270 (13.2%)</v>
       </c>
       <c r="G4" s="58" t="str">
         <f>ROUND(Calculations!I4,0)&amp;" ("&amp;ROUND(Calculations!J4,1)&amp;"%)"</f>
-        <v>253 (-1.6%)</v>
+        <v>253 (7%)</v>
       </c>
       <c r="H4" s="58" t="str">
         <f>ROUND(Calculations!K4,0)&amp;" ("&amp;ROUND(Calculations!L4,1)&amp;"%)"</f>
-        <v>277 (7.4%)</v>
+        <v>277 (15.3%)</v>
       </c>
       <c r="I4" s="58" t="str">
         <f>ROUND(Calculations!M4,0)&amp;" ("&amp;ROUND(Calculations!N4,1)&amp;"%)"</f>
-        <v>191 (-34.7%)</v>
+        <v>191 (-23.2%)</v>
       </c>
       <c r="J4" s="58" t="str">
         <f>ROUND(Calculations!O4,0)&amp;" ("&amp;ROUND(Calculations!P4,1)&amp;"%)"</f>
-        <v>113 (-127.6%)</v>
+        <v>113 (-108.1%)</v>
       </c>
       <c r="K4" s="58" t="str">
         <f>ROUND(Calculations!Q4,0)&amp;" ("&amp;ROUND(Calculations!R4,1)&amp;"%)"</f>
-        <v>99 (-159.2%)</v>
+        <v>99 (-137.1%)</v>
       </c>
       <c r="L4" s="59" t="str">
         <f>ROUND(Calculations!S4,0)&amp;" ("&amp;ROUND(Calculations!T4,1)&amp;"%)"</f>
-        <v>335 (23.4%)</v>
+        <v>335 (29.9%)</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1710,43 +1716,43 @@
       </c>
       <c r="C5" s="80">
         <f>Calculations!C5</f>
-        <v>309.69</v>
+        <v>271.23</v>
       </c>
       <c r="D5" s="80">
         <f>Calculations!D5</f>
-        <v>563.07272727272721</v>
+        <v>493.14545454545453</v>
       </c>
       <c r="E5" s="81" t="str">
         <f>ROUND(Calculations!E5,0)&amp;" ("&amp;ROUND(Calculations!F5,1)&amp;"%)"</f>
-        <v>413 (-36.4%)</v>
+        <v>413 (-19.4%)</v>
       </c>
       <c r="F5" s="58" t="str">
         <f>ROUND(Calculations!G5,0)&amp;" ("&amp;ROUND(Calculations!H5,1)&amp;"%)"</f>
-        <v>413 (-36.4%)</v>
+        <v>413 (-19.5%)</v>
       </c>
       <c r="G5" s="58" t="str">
         <f>ROUND(Calculations!I5,0)&amp;" ("&amp;ROUND(Calculations!J5,1)&amp;"%)"</f>
-        <v>410 (-37.2%)</v>
+        <v>410 (-20.2%)</v>
       </c>
       <c r="H5" s="58" t="str">
         <f>ROUND(Calculations!K5,0)&amp;" ("&amp;ROUND(Calculations!L5,1)&amp;"%)"</f>
-        <v>434 (-29.6%)</v>
+        <v>434 (-13.5%)</v>
       </c>
       <c r="I5" s="58" t="str">
         <f>ROUND(Calculations!M5,0)&amp;" ("&amp;ROUND(Calculations!N5,1)&amp;"%)"</f>
-        <v>343 (-64.2%)</v>
+        <v>343 (-43.8%)</v>
       </c>
       <c r="J5" s="58" t="str">
         <f>ROUND(Calculations!O5,0)&amp;" ("&amp;ROUND(Calculations!P5,1)&amp;"%)"</f>
-        <v>251 (-124.6%)</v>
+        <v>251 (-96.7%)</v>
       </c>
       <c r="K5" s="58" t="str">
         <f>ROUND(Calculations!Q5,0)&amp;" ("&amp;ROUND(Calculations!R5,1)&amp;"%)"</f>
-        <v>222 (-153.6%)</v>
+        <v>222 (-122.1%)</v>
       </c>
       <c r="L5" s="59" t="str">
         <f>ROUND(Calculations!S5,0)&amp;" ("&amp;ROUND(Calculations!T5,1)&amp;"%)"</f>
-        <v>474 (-18.8%)</v>
+        <v>474 (-4%)</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1758,39 +1764,39 @@
       </c>
       <c r="C6" s="80">
         <f>Calculations!C6</f>
-        <v>55.06</v>
+        <v>40.74</v>
       </c>
       <c r="D6" s="80">
         <f>Calculations!D6</f>
-        <v>100.10909090909091</v>
+        <v>74.072727272727263</v>
       </c>
       <c r="E6" s="81" t="str">
         <f>ROUND(Calculations!E6,0)&amp;" ("&amp;ROUND(Calculations!F6,1)&amp;"%)"</f>
-        <v>79 (-27.3%)</v>
+        <v>79 (5.8%)</v>
       </c>
       <c r="F6" s="58" t="str">
         <f>ROUND(Calculations!G6,0)&amp;" ("&amp;ROUND(Calculations!H6,1)&amp;"%)"</f>
-        <v>78 (-28.3%)</v>
+        <v>78 (5.1%)</v>
       </c>
       <c r="G6" s="58" t="str">
         <f>ROUND(Calculations!I6,0)&amp;" ("&amp;ROUND(Calculations!J6,1)&amp;"%)"</f>
-        <v>44 (-128.3%)</v>
+        <v>44 (-68.9%)</v>
       </c>
       <c r="H6" s="58" t="str">
         <f>ROUND(Calculations!K6,0)&amp;" ("&amp;ROUND(Calculations!L6,1)&amp;"%)"</f>
-        <v>84 (-18.7%)</v>
+        <v>84 (12.2%)</v>
       </c>
       <c r="I6" s="58" t="str">
         <f>ROUND(Calculations!M6,0)&amp;" ("&amp;ROUND(Calculations!N6,1)&amp;"%)"</f>
-        <v>29 (-242.8%)</v>
+        <v>29 (-153.7%)</v>
       </c>
       <c r="J6" s="58" t="str">
         <f>ROUND(Calculations!O6,0)&amp;" ("&amp;ROUND(Calculations!P6,1)&amp;"%)"</f>
-        <v>37 (-172.3%)</v>
+        <v>37 (-101.4%)</v>
       </c>
       <c r="K6" s="58" t="str">
         <f>ROUND(Calculations!Q6,0)&amp;" ("&amp;ROUND(Calculations!R6,1)&amp;"%)"</f>
-        <v>11 (-853.4%)</v>
+        <v>11 (-605.5%)</v>
       </c>
       <c r="L6" s="59" t="e">
         <f>ROUND(Calculations!S6,0)&amp;" ("&amp;ROUND(Calculations!T6,1)&amp;"%)"</f>
@@ -1806,39 +1812,39 @@
       </c>
       <c r="C7" s="80">
         <f>Calculations!C7</f>
-        <v>66.59</v>
+        <v>65.87</v>
       </c>
       <c r="D7" s="80">
         <f>Calculations!D7</f>
-        <v>121.07272727272726</v>
+        <v>119.76363636363637</v>
       </c>
       <c r="E7" s="81" t="str">
         <f>ROUND(Calculations!E7,0)&amp;" ("&amp;ROUND(Calculations!F7,1)&amp;"%)"</f>
-        <v>80 (-50.9%)</v>
+        <v>80 (-49.2%)</v>
       </c>
       <c r="F7" s="58" t="str">
         <f>ROUND(Calculations!G7,0)&amp;" ("&amp;ROUND(Calculations!H7,1)&amp;"%)"</f>
-        <v>81 (-49.2%)</v>
+        <v>81 (-47.5%)</v>
       </c>
       <c r="G7" s="58" t="str">
         <f>ROUND(Calculations!I7,0)&amp;" ("&amp;ROUND(Calculations!J7,1)&amp;"%)"</f>
-        <v>55 (-119.8%)</v>
+        <v>55 (-117.4%)</v>
       </c>
       <c r="H7" s="58" t="str">
         <f>ROUND(Calculations!K7,0)&amp;" ("&amp;ROUND(Calculations!L7,1)&amp;"%)"</f>
-        <v>82 (-47.5%)</v>
+        <v>82 (-45.9%)</v>
       </c>
       <c r="I7" s="58" t="str">
         <f>ROUND(Calculations!M7,0)&amp;" ("&amp;ROUND(Calculations!N7,1)&amp;"%)"</f>
-        <v>64 (-90.7%)</v>
+        <v>64 (-88.6%)</v>
       </c>
       <c r="J7" s="58" t="str">
         <f>ROUND(Calculations!O7,0)&amp;" ("&amp;ROUND(Calculations!P7,1)&amp;"%)"</f>
-        <v>40 (-206.5%)</v>
+        <v>40 (-203.2%)</v>
       </c>
       <c r="K7" s="58" t="str">
         <f>ROUND(Calculations!Q7,0)&amp;" ("&amp;ROUND(Calculations!R7,1)&amp;"%)"</f>
-        <v>11 (-1026.3%)</v>
+        <v>11 (-1014.1%)</v>
       </c>
       <c r="L7" s="59" t="e">
         <f>ROUND(Calculations!S7,0)&amp;" ("&amp;ROUND(Calculations!T7,1)&amp;"%)"</f>
@@ -1854,39 +1860,39 @@
       </c>
       <c r="C8" s="80">
         <f>Calculations!C8</f>
-        <v>520.71</v>
+        <v>487.72</v>
       </c>
       <c r="D8" s="80">
         <f>Calculations!D8</f>
-        <v>946.74545454545455</v>
+        <v>886.76363636363635</v>
       </c>
       <c r="E8" s="81" t="str">
         <f>ROUND(Calculations!E8,0)&amp;" ("&amp;ROUND(Calculations!F8,1)&amp;"%)"</f>
-        <v>755 (-25.4%)</v>
+        <v>755 (-17.5%)</v>
       </c>
       <c r="F8" s="58" t="str">
         <f>ROUND(Calculations!G8,0)&amp;" ("&amp;ROUND(Calculations!H8,1)&amp;"%)"</f>
-        <v>759 (-24.8%)</v>
+        <v>759 (-16.9%)</v>
       </c>
       <c r="G8" s="58" t="str">
         <f>ROUND(Calculations!I8,0)&amp;" ("&amp;ROUND(Calculations!J8,1)&amp;"%)"</f>
-        <v>708 (-33.7%)</v>
+        <v>708 (-25.2%)</v>
       </c>
       <c r="H8" s="58" t="str">
         <f>ROUND(Calculations!K8,0)&amp;" ("&amp;ROUND(Calculations!L8,1)&amp;"%)"</f>
-        <v>771 (-22.8%)</v>
+        <v>771 (-15%)</v>
       </c>
       <c r="I8" s="58" t="str">
         <f>ROUND(Calculations!M8,0)&amp;" ("&amp;ROUND(Calculations!N8,1)&amp;"%)"</f>
-        <v>734 (-29%)</v>
+        <v>734 (-20.9%)</v>
       </c>
       <c r="J8" s="58" t="str">
         <f>ROUND(Calculations!O8,0)&amp;" ("&amp;ROUND(Calculations!P8,1)&amp;"%)"</f>
-        <v>492 (-92.5%)</v>
+        <v>492 (-80.3%)</v>
       </c>
       <c r="K8" s="58" t="str">
         <f>ROUND(Calculations!Q8,0)&amp;" ("&amp;ROUND(Calculations!R8,1)&amp;"%)"</f>
-        <v>385 (-145.9%)</v>
+        <v>385 (-130.3%)</v>
       </c>
       <c r="L8" s="59" t="e">
         <f>ROUND(Calculations!S8,0)&amp;" ("&amp;ROUND(Calculations!T8,1)&amp;"%)"</f>
@@ -1902,39 +1908,39 @@
       </c>
       <c r="C9" s="80">
         <f>Calculations!C9</f>
-        <v>513.66999999999996</v>
+        <v>480.87</v>
       </c>
       <c r="D9" s="80">
         <f>Calculations!D9</f>
-        <v>933.94545454545437</v>
+        <v>874.30909090909086</v>
       </c>
       <c r="E9" s="81" t="str">
         <f>ROUND(Calculations!E9,0)&amp;" ("&amp;ROUND(Calculations!F9,1)&amp;"%)"</f>
-        <v>730 (-28%)</v>
+        <v>730 (-19.8%)</v>
       </c>
       <c r="F9" s="58" t="str">
         <f>ROUND(Calculations!G9,0)&amp;" ("&amp;ROUND(Calculations!H9,1)&amp;"%)"</f>
-        <v>730 (-27.9%)</v>
+        <v>730 (-19.7%)</v>
       </c>
       <c r="G9" s="58" t="str">
         <f>ROUND(Calculations!I9,0)&amp;" ("&amp;ROUND(Calculations!J9,1)&amp;"%)"</f>
-        <v>747 (-25%)</v>
+        <v>747 (-17%)</v>
       </c>
       <c r="H9" s="58" t="str">
         <f>ROUND(Calculations!K9,0)&amp;" ("&amp;ROUND(Calculations!L9,1)&amp;"%)"</f>
-        <v>805 (-16.1%)</v>
+        <v>805 (-8.7%)</v>
       </c>
       <c r="I9" s="58" t="str">
         <f>ROUND(Calculations!M9,0)&amp;" ("&amp;ROUND(Calculations!N9,1)&amp;"%)"</f>
-        <v>704 (-32.7%)</v>
+        <v>704 (-24.2%)</v>
       </c>
       <c r="J9" s="58" t="str">
         <f>ROUND(Calculations!O9,0)&amp;" ("&amp;ROUND(Calculations!P9,1)&amp;"%)"</f>
-        <v>517 (-80.6%)</v>
+        <v>517 (-69.1%)</v>
       </c>
       <c r="K9" s="58" t="str">
         <f>ROUND(Calculations!Q9,0)&amp;" ("&amp;ROUND(Calculations!R9,1)&amp;"%)"</f>
-        <v>409 (-128.3%)</v>
+        <v>409 (-113.8%)</v>
       </c>
       <c r="L9" s="59" t="e">
         <f>ROUND(Calculations!S9,0)&amp;" ("&amp;ROUND(Calculations!T9,1)&amp;"%)"</f>
@@ -1950,39 +1956,39 @@
       </c>
       <c r="C10" s="80">
         <f>Calculations!C10</f>
-        <v>151.88999999999999</v>
+        <v>135.84</v>
       </c>
       <c r="D10" s="80">
         <f>Calculations!D10</f>
-        <v>276.16363636363633</v>
+        <v>246.98181818181817</v>
       </c>
       <c r="E10" s="81" t="str">
         <f>ROUND(Calculations!E10,0)&amp;" ("&amp;ROUND(Calculations!F10,1)&amp;"%)"</f>
-        <v>156 (-77.1%)</v>
+        <v>156 (-58.4%)</v>
       </c>
       <c r="F10" s="58" t="str">
         <f>ROUND(Calculations!G10,0)&amp;" ("&amp;ROUND(Calculations!H10,1)&amp;"%)"</f>
-        <v>155 (-78.7%)</v>
+        <v>155 (-59.8%)</v>
       </c>
       <c r="G10" s="58" t="str">
         <f>ROUND(Calculations!I10,0)&amp;" ("&amp;ROUND(Calculations!J10,1)&amp;"%)"</f>
-        <v>177 (-56.1%)</v>
+        <v>177 (-39.6%)</v>
       </c>
       <c r="H10" s="58" t="str">
         <f>ROUND(Calculations!K10,0)&amp;" ("&amp;ROUND(Calculations!L10,1)&amp;"%)"</f>
-        <v>181 (-52.6%)</v>
+        <v>181 (-36.5%)</v>
       </c>
       <c r="I10" s="58" t="str">
         <f>ROUND(Calculations!M10,0)&amp;" ("&amp;ROUND(Calculations!N10,1)&amp;"%)"</f>
-        <v>159 (-73.5%)</v>
+        <v>159 (-55.1%)</v>
       </c>
       <c r="J10" s="58" t="str">
         <f>ROUND(Calculations!O10,0)&amp;" ("&amp;ROUND(Calculations!P10,1)&amp;"%)"</f>
-        <v>122 (-126.1%)</v>
+        <v>122 (-102.2%)</v>
       </c>
       <c r="K10" s="58" t="str">
         <f>ROUND(Calculations!Q10,0)&amp;" ("&amp;ROUND(Calculations!R10,1)&amp;"%)"</f>
-        <v>62 (-345.4%)</v>
+        <v>62 (-298.4%)</v>
       </c>
       <c r="L10" s="59" t="e">
         <f>ROUND(Calculations!S10,0)&amp;" ("&amp;ROUND(Calculations!T10,1)&amp;"%)"</f>
@@ -1998,39 +2004,39 @@
       </c>
       <c r="C11" s="80">
         <f>Calculations!C11</f>
-        <v>150.5</v>
+        <v>130.58000000000001</v>
       </c>
       <c r="D11" s="80">
         <f>Calculations!D11</f>
-        <v>273.63636363636363</v>
+        <v>237.41818181818184</v>
       </c>
       <c r="E11" s="81" t="str">
         <f>ROUND(Calculations!E11,0)&amp;" ("&amp;ROUND(Calculations!F11,1)&amp;"%)"</f>
-        <v>246 (-11.2%)</v>
+        <v>246 (3.6%)</v>
       </c>
       <c r="F11" s="58" t="str">
         <f>ROUND(Calculations!G11,0)&amp;" ("&amp;ROUND(Calculations!H11,1)&amp;"%)"</f>
-        <v>248 (-10.4%)</v>
+        <v>248 (4.2%)</v>
       </c>
       <c r="G11" s="58" t="str">
         <f>ROUND(Calculations!I11,0)&amp;" ("&amp;ROUND(Calculations!J11,1)&amp;"%)"</f>
-        <v>225 (-21.5%)</v>
+        <v>225 (-5.4%)</v>
       </c>
       <c r="H11" s="58" t="str">
         <f>ROUND(Calculations!K11,0)&amp;" ("&amp;ROUND(Calculations!L11,1)&amp;"%)"</f>
-        <v>225 (-21.5%)</v>
+        <v>225 (-5.4%)</v>
       </c>
       <c r="I11" s="58" t="str">
         <f>ROUND(Calculations!M11,0)&amp;" ("&amp;ROUND(Calculations!N11,1)&amp;"%)"</f>
-        <v>161 (-69.6%)</v>
+        <v>161 (-47.2%)</v>
       </c>
       <c r="J11" s="58" t="str">
         <f>ROUND(Calculations!O11,0)&amp;" ("&amp;ROUND(Calculations!P11,1)&amp;"%)"</f>
-        <v>125 (-119.5%)</v>
+        <v>125 (-90.5%)</v>
       </c>
       <c r="K11" s="58" t="str">
         <f>ROUND(Calculations!Q11,0)&amp;" ("&amp;ROUND(Calculations!R11,1)&amp;"%)"</f>
-        <v>94 (-191.1%)</v>
+        <v>94 (-152.6%)</v>
       </c>
       <c r="L11" s="59" t="e">
         <f>ROUND(Calculations!S11,0)&amp;" ("&amp;ROUND(Calculations!T11,1)&amp;"%)"</f>
@@ -2046,39 +2052,39 @@
       </c>
       <c r="C12" s="80">
         <f>Calculations!C12</f>
-        <v>219.71</v>
+        <v>209.55</v>
       </c>
       <c r="D12" s="80">
         <f>Calculations!D12</f>
-        <v>399.47272727272724</v>
+        <v>381</v>
       </c>
       <c r="E12" s="81" t="str">
         <f>ROUND(Calculations!E12,0)&amp;" ("&amp;ROUND(Calculations!F12,1)&amp;"%)"</f>
-        <v>229 (-74.4%)</v>
+        <v>229 (-66.3%)</v>
       </c>
       <c r="F12" s="58" t="str">
         <f>ROUND(Calculations!G12,0)&amp;" ("&amp;ROUND(Calculations!H12,1)&amp;"%)"</f>
-        <v>230 (-73.7%)</v>
+        <v>230 (-65.6%)</v>
       </c>
       <c r="G12" s="58" t="str">
         <f>ROUND(Calculations!I12,0)&amp;" ("&amp;ROUND(Calculations!J12,1)&amp;"%)"</f>
-        <v>389 (-2.6%)</v>
+        <v>389 (2.1%)</v>
       </c>
       <c r="H12" s="58" t="str">
         <f>ROUND(Calculations!K12,0)&amp;" ("&amp;ROUND(Calculations!L12,1)&amp;"%)"</f>
-        <v>652 (38.7%)</v>
+        <v>652 (41.6%)</v>
       </c>
       <c r="I12" s="58" t="str">
         <f>ROUND(Calculations!M12,0)&amp;" ("&amp;ROUND(Calculations!N12,1)&amp;"%)"</f>
-        <v>349 (-14.6%)</v>
+        <v>349 (-9.3%)</v>
       </c>
       <c r="J12" s="58" t="str">
         <f>ROUND(Calculations!O12,0)&amp;" ("&amp;ROUND(Calculations!P12,1)&amp;"%)"</f>
-        <v>114 (-251.9%)</v>
+        <v>114 (-235.6%)</v>
       </c>
       <c r="K12" s="58" t="str">
         <f>ROUND(Calculations!Q12,0)&amp;" ("&amp;ROUND(Calculations!R12,1)&amp;"%)"</f>
-        <v>164 (-143.6%)</v>
+        <v>164 (-132.3%)</v>
       </c>
       <c r="L12" s="59" t="e">
         <f>ROUND(Calculations!S12,0)&amp;" ("&amp;ROUND(Calculations!T12,1)&amp;"%)"</f>
@@ -2094,39 +2100,39 @@
       </c>
       <c r="C13" s="80">
         <f>Calculations!C13</f>
-        <v>306.64</v>
+        <v>285.27999999999997</v>
       </c>
       <c r="D13" s="80">
         <f>Calculations!D13</f>
-        <v>557.5272727272727</v>
+        <v>518.69090909090903</v>
       </c>
       <c r="E13" s="81" t="str">
         <f>ROUND(Calculations!E13,0)&amp;" ("&amp;ROUND(Calculations!F13,1)&amp;"%)"</f>
-        <v>494 (-13%)</v>
+        <v>494 (-5.1%)</v>
       </c>
       <c r="F13" s="58" t="str">
         <f>ROUND(Calculations!G13,0)&amp;" ("&amp;ROUND(Calculations!H13,1)&amp;"%)"</f>
-        <v>498 (-12.1%)</v>
+        <v>498 (-4.3%)</v>
       </c>
       <c r="G13" s="58" t="str">
         <f>ROUND(Calculations!I13,0)&amp;" ("&amp;ROUND(Calculations!J13,1)&amp;"%)"</f>
-        <v>435 (-28.2%)</v>
+        <v>435 (-19.3%)</v>
       </c>
       <c r="H13" s="58" t="str">
         <f>ROUND(Calculations!K13,0)&amp;" ("&amp;ROUND(Calculations!L13,1)&amp;"%)"</f>
-        <v>482 (-15.8%)</v>
+        <v>482 (-7.7%)</v>
       </c>
       <c r="I13" s="58" t="str">
         <f>ROUND(Calculations!M13,0)&amp;" ("&amp;ROUND(Calculations!N13,1)&amp;"%)"</f>
-        <v>401 (-39.1%)</v>
+        <v>401 (-29.4%)</v>
       </c>
       <c r="J13" s="58" t="str">
         <f>ROUND(Calculations!O13,0)&amp;" ("&amp;ROUND(Calculations!P13,1)&amp;"%)"</f>
-        <v>265 (-110.2%)</v>
+        <v>265 (-95.6%)</v>
       </c>
       <c r="K13" s="58" t="str">
         <f>ROUND(Calculations!Q13,0)&amp;" ("&amp;ROUND(Calculations!R13,1)&amp;"%)"</f>
-        <v>208 (-168%)</v>
+        <v>208 (-149.4%)</v>
       </c>
       <c r="L13" s="59" t="e">
         <f>ROUND(Calculations!S13,0)&amp;" ("&amp;ROUND(Calculations!T13,1)&amp;"%)"</f>
@@ -2142,39 +2148,39 @@
       </c>
       <c r="C14" s="80">
         <f>Calculations!C14</f>
-        <v>526.16999999999996</v>
+        <v>492.76</v>
       </c>
       <c r="D14" s="80">
         <f>Calculations!D14</f>
-        <v>956.67272727272712</v>
+        <v>895.92727272727268</v>
       </c>
       <c r="E14" s="81" t="str">
         <f>ROUND(Calculations!E14,0)&amp;" ("&amp;ROUND(Calculations!F14,1)&amp;"%)"</f>
-        <v>736 (-29.9%)</v>
+        <v>736 (-21.7%)</v>
       </c>
       <c r="F14" s="58" t="str">
         <f>ROUND(Calculations!G14,0)&amp;" ("&amp;ROUND(Calculations!H14,1)&amp;"%)"</f>
-        <v>738 (-29.6%)</v>
+        <v>738 (-21.3%)</v>
       </c>
       <c r="G14" s="58" t="str">
         <f>ROUND(Calculations!I14,0)&amp;" ("&amp;ROUND(Calculations!J14,1)&amp;"%)"</f>
-        <v>650 (-47.2%)</v>
+        <v>650 (-37.8%)</v>
       </c>
       <c r="H14" s="58" t="str">
         <f>ROUND(Calculations!K14,0)&amp;" ("&amp;ROUND(Calculations!L14,1)&amp;"%)"</f>
-        <v>627 (-52.5%)</v>
+        <v>627 (-42.8%)</v>
       </c>
       <c r="I14" s="58" t="str">
         <f>ROUND(Calculations!M14,0)&amp;" ("&amp;ROUND(Calculations!N14,1)&amp;"%)"</f>
-        <v>606 (-57.9%)</v>
+        <v>606 (-47.9%)</v>
       </c>
       <c r="J14" s="58" t="str">
         <f>ROUND(Calculations!O14,0)&amp;" ("&amp;ROUND(Calculations!P14,1)&amp;"%)"</f>
-        <v>532 (-79.9%)</v>
+        <v>532 (-68.5%)</v>
       </c>
       <c r="K14" s="58" t="str">
         <f>ROUND(Calculations!Q14,0)&amp;" ("&amp;ROUND(Calculations!R14,1)&amp;"%)"</f>
-        <v>319 (-199.9%)</v>
+        <v>319 (-180.9%)</v>
       </c>
       <c r="L14" s="59" t="e">
         <f>ROUND(Calculations!S14,0)&amp;" ("&amp;ROUND(Calculations!T14,1)&amp;"%)"</f>
@@ -2190,39 +2196,39 @@
       </c>
       <c r="C15" s="80">
         <f>Calculations!C15</f>
-        <v>619.85</v>
+        <v>581.73</v>
       </c>
       <c r="D15" s="80">
         <f>Calculations!D15</f>
-        <v>1127</v>
+        <v>1057.6909090909091</v>
       </c>
       <c r="E15" s="82" t="str">
         <f>ROUND(Calculations!E15,0)&amp;" ("&amp;ROUND(Calculations!F15,1)&amp;"%)"</f>
-        <v>872 (-29.2%)</v>
+        <v>872 (-21.3%)</v>
       </c>
       <c r="F15" s="83" t="str">
         <f>ROUND(Calculations!G15,0)&amp;" ("&amp;ROUND(Calculations!H15,1)&amp;"%)"</f>
-        <v>868 (-29.8%)</v>
+        <v>868 (-21.8%)</v>
       </c>
       <c r="G15" s="83" t="str">
         <f>ROUND(Calculations!I15,0)&amp;" ("&amp;ROUND(Calculations!J15,1)&amp;"%)"</f>
-        <v>821 (-37.3%)</v>
+        <v>821 (-28.9%)</v>
       </c>
       <c r="H15" s="83" t="str">
         <f>ROUND(Calculations!K15,0)&amp;" ("&amp;ROUND(Calculations!L15,1)&amp;"%)"</f>
-        <v>811 (-38.9%)</v>
+        <v>811 (-30.4%)</v>
       </c>
       <c r="I15" s="83" t="str">
         <f>ROUND(Calculations!M15,0)&amp;" ("&amp;ROUND(Calculations!N15,1)&amp;"%)"</f>
-        <v>752 (-49.8%)</v>
+        <v>752 (-40.6%)</v>
       </c>
       <c r="J15" s="83" t="str">
         <f>ROUND(Calculations!O15,0)&amp;" ("&amp;ROUND(Calculations!P15,1)&amp;"%)"</f>
-        <v>555 (-102.9%)</v>
+        <v>555 (-90.4%)</v>
       </c>
       <c r="K15" s="83" t="str">
         <f>ROUND(Calculations!Q15,0)&amp;" ("&amp;ROUND(Calculations!R15,1)&amp;"%)"</f>
-        <v>450 (-150.4%)</v>
+        <v>450 (-135%)</v>
       </c>
       <c r="L15" s="84" t="e">
         <f>ROUND(Calculations!S15,0)&amp;" ("&amp;ROUND(Calculations!T15,1)&amp;"%)"</f>
@@ -2244,31 +2250,31 @@
       </c>
       <c r="E16" s="96" t="str">
         <f>ROUND(Calculations!F16,1)&amp;"%"</f>
-        <v>-29.7%</v>
+        <v>-17.6%</v>
       </c>
       <c r="F16" s="86" t="str">
         <f>ROUND(Calculations!H16,1)&amp;"%"</f>
-        <v>-29.6%</v>
+        <v>-17.4%</v>
       </c>
       <c r="G16" s="97" t="str">
         <f>ROUND(Calculations!J16,1)&amp;"%"</f>
-        <v>-41.1%</v>
+        <v>-26.9%</v>
       </c>
       <c r="H16" s="97" t="str">
         <f>ROUND(Calculations!L16,1)&amp;"%"</f>
-        <v>-22.2%</v>
+        <v>-10.4%</v>
       </c>
       <c r="I16" s="97" t="str">
         <f>ROUND(Calculations!N16,1)&amp;"%"</f>
-        <v>-66.7%</v>
+        <v>-48.2%</v>
       </c>
       <c r="J16" s="97" t="str">
         <f>ROUND(Calculations!P16,1)&amp;"%"</f>
-        <v>-139.3%</v>
+        <v>-116.1%</v>
       </c>
       <c r="K16" s="97" t="str">
         <f>ROUND(Calculations!R16,1)&amp;"%"</f>
-        <v>-290%</v>
+        <v>-249.2%</v>
       </c>
       <c r="L16" s="87" t="e">
         <f>ROUND(Calculations!T16,1)&amp;"%"</f>
@@ -2290,31 +2296,31 @@
       </c>
       <c r="E17" s="98" t="str">
         <f>ROUND(Calculations!F17,1)&amp;"%"</f>
-        <v>30.4%</v>
+        <v>22.5%</v>
       </c>
       <c r="F17" s="88" t="str">
         <f>ROUND(Calculations!H17,1)&amp;"%"</f>
-        <v>30.3%</v>
+        <v>22.3%</v>
       </c>
       <c r="G17" s="99" t="str">
         <f>ROUND(Calculations!J17,1)&amp;"%"</f>
-        <v>41.1%</v>
+        <v>28.8%</v>
       </c>
       <c r="H17" s="99" t="str">
         <f>ROUND(Calculations!L17,1)&amp;"%"</f>
-        <v>28.8%</v>
+        <v>20.3%</v>
       </c>
       <c r="I17" s="99" t="str">
         <f>ROUND(Calculations!N17,1)&amp;"%"</f>
-        <v>66.7%</v>
+        <v>48.2%</v>
       </c>
       <c r="J17" s="99" t="str">
         <f>ROUND(Calculations!P17,1)&amp;"%"</f>
-        <v>139.3%</v>
+        <v>116.1%</v>
       </c>
       <c r="K17" s="99" t="str">
         <f>ROUND(Calculations!R17,1)&amp;"%"</f>
-        <v>290%</v>
+        <v>249.2%</v>
       </c>
       <c r="L17" s="89" t="e">
         <f>ROUND(Calculations!T17,1)&amp;"%"</f>
@@ -2322,29 +2328,29 @@
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="102" t="s">
+      <c r="A20" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="103"/>
-      <c r="C20" s="104"/>
+      <c r="B20" s="104"/>
+      <c r="C20" s="105"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="105" t="s">
+      <c r="B21" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="106"/>
+      <c r="C21" s="107"/>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="100" t="s">
+      <c r="B22" s="101" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="101"/>
+      <c r="C22" s="102"/>
     </row>
     <row r="27" spans="1:12">
       <c r="D27" s="95"/>
@@ -2367,7 +2373,7 @@
   <dimension ref="A1:T36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C15"/>
+      <selection activeCell="C32" sqref="C19:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -2452,67 +2458,67 @@
         <v>13</v>
       </c>
       <c r="C2" s="36">
-        <v>161.22999999999999</v>
+        <v>137.38999999999999</v>
       </c>
       <c r="D2" s="8">
         <f t="shared" ref="D2:D15" si="0">C2/0.55</f>
-        <v>293.14545454545453</v>
+        <v>249.79999999999995</v>
       </c>
       <c r="E2" s="46">
         <v>284.02999999999997</v>
       </c>
       <c r="F2" s="9">
         <f>(E2-D2)/E2*100</f>
-        <v>-3.2093280799403425</v>
+        <v>12.051543851001663</v>
       </c>
       <c r="G2" s="48">
         <v>282.27999999999997</v>
       </c>
       <c r="H2" s="10">
         <f>(G2-D2)/G2*100</f>
-        <v>-3.8491761886972351</v>
+        <v>11.506305795663888</v>
       </c>
       <c r="I2" s="11">
         <v>261.14400000000001</v>
       </c>
       <c r="J2" s="11">
         <f>(I2-D2)/I2*100</f>
-        <v>-12.254332684440202</v>
+        <v>4.3439634837484498</v>
       </c>
       <c r="K2" s="12">
         <v>247.298</v>
       </c>
       <c r="L2" s="12">
         <f>(K2-D2)/K2*100</f>
-        <v>-18.539355168846704</v>
+        <v>-1.0117348300430868</v>
       </c>
       <c r="M2" s="4">
         <v>175.1</v>
       </c>
       <c r="N2" s="13">
         <f>(M2-D2)/M2*100</f>
-        <v>-67.416022013394937</v>
+        <v>-42.661336379211853</v>
       </c>
       <c r="O2" s="5">
         <v>132.96</v>
       </c>
       <c r="P2" s="14">
         <f>(O2-D2)/O2*100</f>
-        <v>-120.47642489880755</v>
+        <v>-87.876052948255065</v>
       </c>
       <c r="Q2" s="6">
         <v>109</v>
       </c>
       <c r="R2" s="15">
         <f>(Q2-D2)/Q2*100</f>
-        <v>-168.94078398665553</v>
+        <v>-129.17431192660547</v>
       </c>
       <c r="S2" s="7">
         <v>396</v>
       </c>
       <c r="T2" s="44">
         <f>(S2-D2)/S2*100</f>
-        <v>25.973370064279163</v>
+        <v>36.919191919191931</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -2523,67 +2529,67 @@
         <v>15</v>
       </c>
       <c r="C3" s="36">
-        <v>165.19</v>
+        <v>146.03</v>
       </c>
       <c r="D3" s="8">
         <f t="shared" si="0"/>
-        <v>300.34545454545452</v>
+        <v>265.5090909090909</v>
       </c>
       <c r="E3" s="46">
         <v>261.19</v>
       </c>
       <c r="F3" s="9">
         <f t="shared" ref="F3:F15" si="1">(E3-D3)/E3*100</f>
-        <v>-14.991176746986683</v>
+        <v>-1.6536203181939979</v>
       </c>
       <c r="G3" s="48">
         <v>261.44</v>
       </c>
       <c r="H3" s="10">
         <f t="shared" ref="H3:H15" si="2">(G3-D3)/G3*100</f>
-        <v>-14.881217313897842</v>
+        <v>-1.556414821408699</v>
       </c>
       <c r="I3" s="11">
         <v>240.84</v>
       </c>
       <c r="J3" s="11">
         <f t="shared" ref="J3:J15" si="3">(I3-D3)/I3*100</f>
-        <v>-24.707463272485679</v>
+        <v>-10.242937597197683</v>
       </c>
       <c r="K3" s="12">
         <v>246.30699999999999</v>
       </c>
       <c r="L3" s="12">
         <f t="shared" ref="L3:L15" si="4">(K3-D3)/K3*100</f>
-        <v>-21.939471694046265</v>
+        <v>-7.795998858778237</v>
       </c>
       <c r="M3" s="4">
         <v>179.7</v>
       </c>
       <c r="N3" s="13">
         <f t="shared" ref="N3:N15" si="5">(M3-D3)/M3*100</f>
-        <v>-67.137147771538423</v>
+        <v>-47.751302676177474</v>
       </c>
       <c r="O3" s="5">
         <v>89.58</v>
       </c>
       <c r="P3" s="14">
         <f t="shared" ref="P3:P15" si="6">(O3-D3)/O3*100</f>
-        <v>-235.281820211492</v>
+        <v>-196.39326960157504</v>
       </c>
       <c r="Q3" s="6">
         <v>92</v>
       </c>
       <c r="R3" s="15">
         <f t="shared" ref="R3:R15" si="7">(Q3-D3)/Q3*100</f>
-        <v>-226.46245059288535</v>
+        <v>-188.59683794466403</v>
       </c>
       <c r="S3" s="7">
         <v>267</v>
       </c>
       <c r="T3" s="44">
         <f t="shared" ref="T3:T15" si="8">(S3-D3)/S3*100</f>
-        <v>-12.488934286687083</v>
+        <v>0.55839291794348289</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -2594,67 +2600,67 @@
         <v>17</v>
       </c>
       <c r="C4" s="36">
-        <v>141.15</v>
+        <v>129.1</v>
       </c>
       <c r="D4" s="8">
         <f t="shared" si="0"/>
-        <v>256.63636363636363</v>
+        <v>234.72727272727269</v>
       </c>
       <c r="E4" s="46">
         <v>270.38</v>
       </c>
       <c r="F4" s="9">
         <f t="shared" si="1"/>
-        <v>5.0830817233657708</v>
+        <v>13.186155511771325</v>
       </c>
       <c r="G4" s="48">
         <v>270.31</v>
       </c>
       <c r="H4" s="10">
         <f t="shared" si="2"/>
-        <v>5.0585018547728078</v>
+        <v>13.163674030826575</v>
       </c>
       <c r="I4" s="11">
         <v>252.50399999999999</v>
       </c>
       <c r="J4" s="11">
         <f t="shared" si="3"/>
-        <v>-1.6365537323621153</v>
+        <v>7.0401765012543569</v>
       </c>
       <c r="K4" s="12">
         <v>277.21300000000002</v>
       </c>
       <c r="L4" s="12">
         <f t="shared" si="4"/>
-        <v>7.4226808856858781</v>
+        <v>15.326022687510083</v>
       </c>
       <c r="M4" s="4">
         <v>190.5</v>
       </c>
       <c r="N4" s="13">
         <f t="shared" si="5"/>
-        <v>-34.717251252684314</v>
+        <v>-23.216416129801935</v>
       </c>
       <c r="O4" s="5">
         <v>112.77</v>
       </c>
       <c r="P4" s="14">
         <f t="shared" si="6"/>
-        <v>-127.5750320443058</v>
+        <v>-108.14691205752655</v>
       </c>
       <c r="Q4" s="6">
         <v>99</v>
       </c>
       <c r="R4" s="15">
         <f t="shared" si="7"/>
-        <v>-159.22865013774103</v>
+        <v>-137.09825528007343</v>
       </c>
       <c r="S4" s="7">
         <v>335</v>
       </c>
       <c r="T4" s="44">
         <f t="shared" si="8"/>
-        <v>23.392130257801902</v>
+        <v>29.932157394843973</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -2665,67 +2671,67 @@
         <v>19</v>
       </c>
       <c r="C5" s="36">
-        <v>309.69</v>
+        <v>271.23</v>
       </c>
       <c r="D5" s="8">
         <f t="shared" si="0"/>
-        <v>563.07272727272721</v>
+        <v>493.14545454545453</v>
       </c>
       <c r="E5" s="46">
         <v>412.91</v>
       </c>
       <c r="F5" s="9">
         <f t="shared" si="1"/>
-        <v>-36.366938866272832</v>
+        <v>-19.431705346311425</v>
       </c>
       <c r="G5" s="48">
         <v>412.67</v>
       </c>
       <c r="H5" s="10">
         <f t="shared" si="2"/>
-        <v>-36.446246946162105</v>
+        <v>-19.501164258476386</v>
       </c>
       <c r="I5" s="11">
         <v>410.4</v>
       </c>
       <c r="J5" s="11">
         <f t="shared" si="3"/>
-        <v>-37.200956937799035</v>
+        <v>-20.162147793726742</v>
       </c>
       <c r="K5" s="12">
         <v>434.423</v>
       </c>
       <c r="L5" s="12">
         <f t="shared" si="4"/>
-        <v>-29.613930955020155</v>
+        <v>-13.51734474129006</v>
       </c>
       <c r="M5" s="4">
         <v>343</v>
       </c>
       <c r="N5" s="13">
         <f t="shared" si="5"/>
-        <v>-64.16114497747148</v>
+        <v>-43.774184998674784</v>
       </c>
       <c r="O5" s="5">
         <v>250.72</v>
       </c>
       <c r="P5" s="14">
         <f t="shared" si="6"/>
-        <v>-124.58229390265123</v>
+        <v>-96.691709694262343</v>
       </c>
       <c r="Q5" s="6">
         <v>222</v>
       </c>
       <c r="R5" s="15">
         <f t="shared" si="7"/>
-        <v>-153.63636363636363</v>
+        <v>-122.13759213759212</v>
       </c>
       <c r="S5" s="7">
         <v>474</v>
       </c>
       <c r="T5" s="44">
         <f t="shared" si="8"/>
-        <v>-18.791714614499412</v>
+        <v>-4.0391254315304908</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -2736,60 +2742,60 @@
         <v>21</v>
       </c>
       <c r="C6" s="36">
-        <v>55.06</v>
+        <v>40.74</v>
       </c>
       <c r="D6" s="8">
         <f t="shared" si="0"/>
-        <v>100.10909090909091</v>
+        <v>74.072727272727263</v>
       </c>
       <c r="E6" s="46">
         <v>78.66</v>
       </c>
       <c r="F6" s="9">
         <f t="shared" si="1"/>
-        <v>-27.268104384809195</v>
+        <v>5.8317731086609887</v>
       </c>
       <c r="G6" s="48">
         <v>78.03</v>
       </c>
       <c r="H6" s="10">
         <f t="shared" si="2"/>
-        <v>-28.295643866578118</v>
+        <v>5.071476005732074</v>
       </c>
       <c r="I6" s="11">
         <v>43.847999999999999</v>
       </c>
       <c r="J6" s="11">
         <f t="shared" si="3"/>
-        <v>-128.30936624040072</v>
+        <v>-68.930686172065464</v>
       </c>
       <c r="K6" s="12">
         <v>84.33</v>
       </c>
       <c r="L6" s="12">
         <f t="shared" si="4"/>
-        <v>-18.711124047303347</v>
+        <v>12.163254745965535</v>
       </c>
       <c r="M6" s="4">
         <v>29.2</v>
       </c>
       <c r="N6" s="13">
         <f t="shared" si="5"/>
-        <v>-242.83935242839351</v>
+        <v>-153.67372353673721</v>
       </c>
       <c r="O6" s="5">
         <v>36.770000000000003</v>
       </c>
       <c r="P6" s="14">
         <f t="shared" si="6"/>
-        <v>-172.25752218953195</v>
+        <v>-101.44880955324247</v>
       </c>
       <c r="Q6" s="6">
         <v>10.5</v>
       </c>
       <c r="R6" s="15">
         <f t="shared" si="7"/>
-        <v>-853.41991341991343</v>
+        <v>-605.45454545454538</v>
       </c>
       <c r="S6" s="7"/>
       <c r="T6" s="44" t="e">
@@ -2805,60 +2811,60 @@
         <v>23</v>
       </c>
       <c r="C7" s="36">
-        <v>66.59</v>
+        <v>65.87</v>
       </c>
       <c r="D7" s="8">
         <f t="shared" si="0"/>
-        <v>121.07272727272726</v>
+        <v>119.76363636363637</v>
       </c>
       <c r="E7" s="46">
         <v>80.25</v>
       </c>
       <c r="F7" s="9">
         <f t="shared" si="1"/>
-        <v>-50.869442084395345</v>
+        <v>-49.238176154064007</v>
       </c>
       <c r="G7" s="48">
         <v>81.17</v>
       </c>
       <c r="H7" s="10">
         <f t="shared" si="2"/>
-        <v>-49.159452103889691</v>
+        <v>-47.546675327875278</v>
       </c>
       <c r="I7" s="11">
         <v>55.08</v>
       </c>
       <c r="J7" s="11">
         <f t="shared" si="3"/>
-        <v>-119.81250412622961</v>
+        <v>-117.43579586716844</v>
       </c>
       <c r="K7" s="12">
         <v>82.099000000000004</v>
       </c>
       <c r="L7" s="12">
         <f t="shared" si="4"/>
-        <v>-47.471622398235368</v>
+        <v>-45.877095170021995</v>
       </c>
       <c r="M7" s="4">
         <v>63.5</v>
       </c>
       <c r="N7" s="13">
         <f t="shared" si="5"/>
-        <v>-90.665712240515376</v>
+        <v>-88.60415175375806</v>
       </c>
       <c r="O7" s="5">
         <v>39.5</v>
       </c>
       <c r="P7" s="14">
         <f t="shared" si="6"/>
-        <v>-206.51323360184119</v>
+        <v>-203.19907940161107</v>
       </c>
       <c r="Q7" s="6">
         <v>10.75</v>
       </c>
       <c r="R7" s="15">
         <f t="shared" si="7"/>
-        <v>-1026.2579281183932</v>
+        <v>-1014.0803382663847</v>
       </c>
       <c r="S7" s="7"/>
       <c r="T7" s="44" t="e">
@@ -2874,60 +2880,60 @@
         <v>25</v>
       </c>
       <c r="C8" s="36">
-        <v>520.71</v>
+        <v>487.72</v>
       </c>
       <c r="D8" s="8">
         <f t="shared" si="0"/>
-        <v>946.74545454545455</v>
+        <v>886.76363636363635</v>
       </c>
       <c r="E8" s="46">
         <v>754.91</v>
       </c>
       <c r="F8" s="9">
         <f t="shared" si="1"/>
-        <v>-25.41169868533396</v>
+        <v>-17.466139852914438</v>
       </c>
       <c r="G8" s="48">
         <v>758.8</v>
       </c>
       <c r="H8" s="10">
         <f t="shared" si="2"/>
-        <v>-24.768773661762602</v>
+        <v>-16.863947860257827</v>
       </c>
       <c r="I8" s="50">
         <v>708.048</v>
       </c>
       <c r="J8" s="11">
         <f t="shared" si="3"/>
-        <v>-33.712044175741553</v>
+        <v>-25.240610292471182</v>
       </c>
       <c r="K8" s="12">
         <v>770.98</v>
       </c>
       <c r="L8" s="12">
         <f t="shared" si="4"/>
-        <v>-22.797667195706055</v>
+        <v>-15.017722426474919</v>
       </c>
       <c r="M8" s="16">
         <v>733.7</v>
       </c>
       <c r="N8" s="13">
         <f t="shared" si="5"/>
-        <v>-29.037134325399279</v>
+        <v>-20.86188310803275</v>
       </c>
       <c r="O8" s="17">
         <v>491.73</v>
       </c>
       <c r="P8" s="14">
         <f t="shared" si="6"/>
-        <v>-92.533596596801999</v>
+        <v>-80.335476046536982</v>
       </c>
       <c r="Q8" s="18">
         <v>385</v>
       </c>
       <c r="R8" s="15">
         <f t="shared" si="7"/>
-        <v>-145.90791027154663</v>
+        <v>-130.32821723730814</v>
       </c>
       <c r="S8" s="19"/>
       <c r="T8" s="44" t="e">
@@ -2943,60 +2949,60 @@
         <v>25</v>
       </c>
       <c r="C9" s="36">
-        <v>513.66999999999996</v>
+        <v>480.87</v>
       </c>
       <c r="D9" s="8">
         <f t="shared" si="0"/>
-        <v>933.94545454545437</v>
+        <v>874.30909090909086</v>
       </c>
       <c r="E9" s="46">
         <v>729.69</v>
       </c>
       <c r="F9" s="9">
         <f t="shared" si="1"/>
-        <v>-27.992086303149872</v>
+        <v>-19.819250765268919</v>
       </c>
       <c r="G9" s="48">
         <v>730.2</v>
       </c>
       <c r="H9" s="10">
         <f t="shared" si="2"/>
-        <v>-27.902691666044138</v>
+        <v>-19.73556435347724</v>
       </c>
       <c r="I9" s="11">
         <v>747.36</v>
       </c>
       <c r="J9" s="11">
         <f t="shared" si="3"/>
-        <v>-24.965940717385777</v>
+        <v>-16.986337362059896</v>
       </c>
       <c r="K9" s="12">
         <v>804.54399999999998</v>
       </c>
       <c r="L9" s="12">
         <f t="shared" si="4"/>
-        <v>-16.083825688272409</v>
+        <v>-8.6713829087148593</v>
       </c>
       <c r="M9" s="4">
         <v>704</v>
       </c>
       <c r="N9" s="13">
         <f t="shared" si="5"/>
-        <v>-32.662706611570222</v>
+        <v>-24.191632231404949</v>
       </c>
       <c r="O9" s="5">
         <v>517.11</v>
       </c>
       <c r="P9" s="14">
         <f t="shared" si="6"/>
-        <v>-80.608662479057529</v>
+        <v>-69.076036222291364</v>
       </c>
       <c r="Q9" s="6">
         <v>409</v>
       </c>
       <c r="R9" s="15">
         <f t="shared" si="7"/>
-        <v>-128.34852189375411</v>
+        <v>-113.76750388975327</v>
       </c>
       <c r="S9" s="7"/>
       <c r="T9" s="44" t="e">
@@ -3012,60 +3018,60 @@
         <v>28</v>
       </c>
       <c r="C10" s="36">
-        <v>151.88999999999999</v>
+        <v>135.84</v>
       </c>
       <c r="D10" s="8">
         <f t="shared" si="0"/>
-        <v>276.16363636363633</v>
+        <v>246.98181818181817</v>
       </c>
       <c r="E10" s="46">
         <v>155.91999999999999</v>
       </c>
       <c r="F10" s="9">
         <f t="shared" si="1"/>
-        <v>-77.118802182937628</v>
+        <v>-58.402910583516032</v>
       </c>
       <c r="G10" s="48">
         <v>154.52000000000001</v>
       </c>
       <c r="H10" s="10">
         <f t="shared" si="2"/>
-        <v>-78.723554467794671</v>
+        <v>-59.838090979690747</v>
       </c>
       <c r="I10" s="11">
         <v>176.904</v>
       </c>
       <c r="J10" s="11">
         <f t="shared" si="3"/>
-        <v>-56.109322775989426</v>
+        <v>-39.613472946806276</v>
       </c>
       <c r="K10" s="12">
         <v>180.93700000000001</v>
       </c>
       <c r="L10" s="12">
         <f t="shared" si="4"/>
-        <v>-52.629719937677933</v>
+        <v>-36.501554785266784</v>
       </c>
       <c r="M10" s="4">
         <v>159.19999999999999</v>
       </c>
       <c r="N10" s="13">
         <f t="shared" si="5"/>
-        <v>-73.469620831429864</v>
+        <v>-55.139333028780271</v>
       </c>
       <c r="O10" s="5">
         <v>122.15</v>
       </c>
       <c r="P10" s="14">
         <f t="shared" si="6"/>
-        <v>-126.08566218881401</v>
+        <v>-102.1955122241655</v>
       </c>
       <c r="Q10" s="6">
         <v>62</v>
       </c>
       <c r="R10" s="15">
         <f t="shared" si="7"/>
-        <v>-345.42521994134893</v>
+        <v>-298.35777126099703</v>
       </c>
       <c r="S10" s="7"/>
       <c r="T10" s="44" t="e">
@@ -3081,60 +3087,60 @@
         <v>13</v>
       </c>
       <c r="C11" s="36">
-        <v>150.5</v>
+        <v>130.58000000000001</v>
       </c>
       <c r="D11" s="8">
         <f t="shared" si="0"/>
-        <v>273.63636363636363</v>
+        <v>237.41818181818184</v>
       </c>
       <c r="E11" s="46">
         <v>246.16</v>
       </c>
       <c r="F11" s="9">
         <f t="shared" si="1"/>
-        <v>-11.161993677430788</v>
+        <v>3.5512748544922652</v>
       </c>
       <c r="G11" s="48">
         <v>247.81</v>
       </c>
       <c r="H11" s="10">
         <f t="shared" si="2"/>
-        <v>-10.421840779776289</v>
+        <v>4.1934619998459173</v>
       </c>
       <c r="I11" s="11">
         <v>225.28800000000001</v>
       </c>
       <c r="J11" s="11">
         <f t="shared" si="3"/>
-        <v>-21.460691930490576</v>
+        <v>-5.3843000151725011</v>
       </c>
       <c r="K11" s="12">
         <v>225.29400000000001</v>
       </c>
       <c r="L11" s="12">
         <f t="shared" si="4"/>
-        <v>-21.457457205413199</v>
+        <v>-5.3814934344375898</v>
       </c>
       <c r="M11" s="4">
         <v>161.30000000000001</v>
       </c>
       <c r="N11" s="13">
         <f t="shared" si="5"/>
-        <v>-69.64436679253788</v>
+        <v>-47.190441300794674</v>
       </c>
       <c r="O11" s="5">
         <v>124.64</v>
       </c>
       <c r="P11" s="14">
         <f t="shared" si="6"/>
-        <v>-119.54137005484888</v>
+        <v>-90.483136888785168</v>
       </c>
       <c r="Q11" s="6">
         <v>94</v>
       </c>
       <c r="R11" s="15">
         <f t="shared" si="7"/>
-        <v>-191.10251450676981</v>
+        <v>-152.5725338491296</v>
       </c>
       <c r="S11" s="7"/>
       <c r="T11" s="44" t="e">
@@ -3150,60 +3156,60 @@
         <v>31</v>
       </c>
       <c r="C12" s="36">
-        <v>219.71</v>
+        <v>209.55</v>
       </c>
       <c r="D12" s="8">
         <f t="shared" si="0"/>
-        <v>399.47272727272724</v>
+        <v>381</v>
       </c>
       <c r="E12" s="46">
         <v>229.11</v>
       </c>
       <c r="F12" s="9">
         <f t="shared" si="1"/>
-        <v>-74.358485999182591</v>
+        <v>-66.295665837370692</v>
       </c>
       <c r="G12" s="48">
         <v>230.03</v>
       </c>
       <c r="H12" s="10">
         <f t="shared" si="2"/>
-        <v>-73.661143012966676</v>
+        <v>-65.630569925661874</v>
       </c>
       <c r="I12" s="11">
         <v>389.23200000000003</v>
       </c>
       <c r="J12" s="11">
         <f t="shared" si="3"/>
-        <v>-2.6310085688553904</v>
+        <v>2.1149340239240422</v>
       </c>
       <c r="K12" s="12">
         <v>652.13199999999995</v>
       </c>
       <c r="L12" s="12">
         <f t="shared" si="4"/>
-        <v>38.743578405487341</v>
+        <v>41.576245300031275</v>
       </c>
       <c r="M12" s="4">
         <v>348.7</v>
       </c>
       <c r="N12" s="13">
         <f t="shared" si="5"/>
-        <v>-14.560575644602022</v>
+        <v>-9.2629767708632098</v>
       </c>
       <c r="O12" s="5">
         <v>113.53</v>
       </c>
       <c r="P12" s="14">
         <f t="shared" si="6"/>
-        <v>-251.86534596382208</v>
+        <v>-235.59411609266277</v>
       </c>
       <c r="Q12" s="6">
         <v>164</v>
       </c>
       <c r="R12" s="15">
         <f t="shared" si="7"/>
-        <v>-143.58093126385808</v>
+        <v>-132.3170731707317</v>
       </c>
       <c r="S12" s="7"/>
       <c r="T12" s="44" t="e">
@@ -3219,60 +3225,60 @@
         <v>33</v>
       </c>
       <c r="C13" s="36">
-        <v>306.64</v>
+        <v>285.27999999999997</v>
       </c>
       <c r="D13" s="8">
         <f t="shared" si="0"/>
-        <v>557.5272727272727</v>
+        <v>518.69090909090903</v>
       </c>
       <c r="E13" s="46">
         <v>493.58</v>
       </c>
       <c r="F13" s="9">
         <f t="shared" si="1"/>
-        <v>-12.955807108730646</v>
+        <v>-5.0875053873554537</v>
       </c>
       <c r="G13" s="48">
         <v>497.5</v>
       </c>
       <c r="H13" s="10">
         <f t="shared" si="2"/>
-        <v>-12.065783462768383</v>
+        <v>-4.259479214253072</v>
       </c>
       <c r="I13" s="11">
         <v>434.80799999999999</v>
       </c>
       <c r="J13" s="11">
         <f t="shared" si="3"/>
-        <v>-28.223784458260358</v>
+        <v>-19.291942441470496</v>
       </c>
       <c r="K13" s="12">
         <v>481.536</v>
       </c>
       <c r="L13" s="12">
         <f t="shared" si="4"/>
-        <v>-15.781015900633118</v>
+        <v>-7.7159151321830626</v>
       </c>
       <c r="M13" s="4">
         <v>400.9</v>
       </c>
       <c r="N13" s="13">
         <f t="shared" si="5"/>
-        <v>-39.068913127281803</v>
+        <v>-29.381618630807949</v>
       </c>
       <c r="O13" s="5">
         <v>265.24</v>
       </c>
       <c r="P13" s="14">
         <f t="shared" si="6"/>
-        <v>-110.19728273536144</v>
+        <v>-95.555311827367291</v>
       </c>
       <c r="Q13" s="6">
         <v>208</v>
       </c>
       <c r="R13" s="15">
         <f t="shared" si="7"/>
-        <v>-168.04195804195803</v>
+        <v>-149.37062937062936</v>
       </c>
       <c r="S13" s="7"/>
       <c r="T13" s="44" t="e">
@@ -3288,60 +3294,60 @@
         <v>25</v>
       </c>
       <c r="C14" s="36">
-        <v>526.16999999999996</v>
+        <v>492.76</v>
       </c>
       <c r="D14" s="8">
         <f t="shared" si="0"/>
-        <v>956.67272727272712</v>
+        <v>895.92727272727268</v>
       </c>
       <c r="E14" s="46">
         <v>736.31</v>
       </c>
       <c r="F14" s="9">
         <f t="shared" si="1"/>
-        <v>-29.927982408595184</v>
+        <v>-21.677998767811484</v>
       </c>
       <c r="G14" s="48">
         <v>738.33</v>
       </c>
       <c r="H14" s="10">
         <f t="shared" si="2"/>
-        <v>-29.572511921867871</v>
+        <v>-21.345099444323356</v>
       </c>
       <c r="I14" s="11">
         <v>649.94399999999996</v>
       </c>
       <c r="J14" s="11">
         <f t="shared" si="3"/>
-        <v>-47.193100832183568</v>
+        <v>-37.846841070503416</v>
       </c>
       <c r="K14" s="12">
         <v>627.39200000000005</v>
       </c>
       <c r="L14" s="12">
         <f t="shared" si="4"/>
-        <v>-52.484049409735391</v>
+        <v>-42.801832463160608</v>
       </c>
       <c r="M14" s="4">
         <v>605.70000000000005</v>
       </c>
       <c r="N14" s="13">
         <f t="shared" si="5"/>
-        <v>-57.944977261470541</v>
+        <v>-47.916010025965434</v>
       </c>
       <c r="O14" s="5">
         <v>531.75</v>
       </c>
       <c r="P14" s="14">
         <f t="shared" si="6"/>
-        <v>-79.910244903192691</v>
+        <v>-68.486558105740045</v>
       </c>
       <c r="Q14" s="6">
         <v>319</v>
       </c>
       <c r="R14" s="15">
         <f t="shared" si="7"/>
-        <v>-199.8974066685665</v>
+        <v>-180.85494442861213</v>
       </c>
       <c r="S14" s="7"/>
       <c r="T14" s="44" t="e">
@@ -3357,60 +3363,60 @@
         <v>36</v>
       </c>
       <c r="C15" s="37">
-        <v>619.85</v>
+        <v>581.73</v>
       </c>
       <c r="D15" s="38">
         <f t="shared" si="0"/>
-        <v>1127</v>
+        <v>1057.6909090909091</v>
       </c>
       <c r="E15" s="47">
         <v>872.31</v>
       </c>
       <c r="F15" s="39">
         <f t="shared" si="1"/>
-        <v>-29.197189072692055</v>
+        <v>-21.251723480289026</v>
       </c>
       <c r="G15" s="49">
         <v>868.19</v>
       </c>
       <c r="H15" s="10">
         <f t="shared" si="2"/>
-        <v>-29.810294981513252</v>
+        <v>-21.82712414228557</v>
       </c>
       <c r="I15" s="51">
         <v>820.58399999999995</v>
       </c>
       <c r="J15" s="11">
         <f t="shared" si="3"/>
-        <v>-37.341210649976126</v>
+        <v>-28.894897913060603</v>
       </c>
       <c r="K15" s="12">
         <v>811.38800000000003</v>
       </c>
       <c r="L15" s="12">
         <f t="shared" si="4"/>
-        <v>-38.897789959920523</v>
+        <v>-30.355749541638417</v>
       </c>
       <c r="M15" s="40">
         <v>752.1</v>
       </c>
       <c r="N15" s="13">
         <f t="shared" si="5"/>
-        <v>-49.847094801223236</v>
+        <v>-40.631685825144146</v>
       </c>
       <c r="O15" s="41">
         <v>555.38</v>
       </c>
       <c r="P15" s="14">
         <f t="shared" si="6"/>
-        <v>-102.92412402319133</v>
+        <v>-90.444544112303134</v>
       </c>
       <c r="Q15" s="42">
         <v>450</v>
       </c>
       <c r="R15" s="15">
         <f t="shared" si="7"/>
-        <v>-150.44444444444446</v>
+        <v>-135.04242424242426</v>
       </c>
       <c r="S15" s="43"/>
       <c r="T15" s="44" t="e">
@@ -3419,45 +3425,45 @@
       </c>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="108" t="s">
+      <c r="A16" s="109" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="108"/>
+      <c r="B16" s="109"/>
       <c r="C16" s="54"/>
       <c r="D16" s="55"/>
       <c r="F16" s="53">
         <f>AVERAGE(F2:F15)</f>
-        <v>-29.696139562649389</v>
+        <v>-17.550282083369233</v>
       </c>
       <c r="G16" s="53"/>
       <c r="H16" s="53">
         <f t="shared" ref="H16:T16" si="9">AVERAGE(H2:H15)</f>
-        <v>-29.607130608496153</v>
+        <v>-17.440658035402972</v>
       </c>
       <c r="I16" s="53"/>
       <c r="J16" s="53">
         <f t="shared" si="9"/>
-        <v>-41.11130579304286</v>
+        <v>-26.89506396162685</v>
       </c>
       <c r="K16" s="53"/>
       <c r="L16" s="53">
         <f t="shared" si="9"/>
-        <v>-22.160055019259804</v>
+        <v>-10.398735825607336</v>
       </c>
       <c r="M16" s="53"/>
       <c r="N16" s="53">
         <f t="shared" si="9"/>
-        <v>-66.655144291393782</v>
+        <v>-48.161192599725332</v>
       </c>
       <c r="O16" s="53"/>
       <c r="P16" s="53">
         <f t="shared" si="9"/>
-        <v>-139.31090112812282</v>
+        <v>-116.13760891259462</v>
       </c>
       <c r="Q16" s="53"/>
       <c r="R16" s="53">
         <f t="shared" si="9"/>
-        <v>-290.04964263744279</v>
+        <v>-249.22521274710371</v>
       </c>
       <c r="S16" s="53"/>
       <c r="T16" s="53" t="e">
@@ -3466,46 +3472,46 @@
       </c>
     </row>
     <row r="17" spans="1:20">
-      <c r="A17" s="107" t="s">
+      <c r="A17" s="108" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="107"/>
+      <c r="B17" s="108"/>
       <c r="C17" s="45"/>
       <c r="D17" s="45"/>
       <c r="E17" s="52"/>
       <c r="F17" s="53" cm="1">
         <f t="array" ref="F17">AVERAGE(ABS(F2:F15))</f>
-        <v>30.422294094558783</v>
+        <v>22.496103129930123</v>
       </c>
       <c r="G17" s="53"/>
       <c r="H17" s="53" cm="1">
         <f t="array" ref="H17">AVERAGE(ABS(H2:H15))</f>
-        <v>30.329773730606547</v>
+        <v>22.288503439984179</v>
       </c>
       <c r="I17" s="53"/>
       <c r="J17" s="53" cm="1">
         <f t="array" ref="J17">AVERAGE(ABS(J2:J15))</f>
-        <v>41.11130579304286</v>
+        <v>28.823503105759261</v>
       </c>
       <c r="K17" s="53"/>
       <c r="L17" s="53" cm="1">
         <f t="array" ref="L17">AVERAGE(ABS(L2:L15))</f>
-        <v>28.755234917998838</v>
+        <v>20.265239073251177</v>
       </c>
       <c r="M17" s="53"/>
       <c r="N17" s="53" cm="1">
         <f t="array" ref="N17">AVERAGE(ABS(N2:N15))</f>
-        <v>66.655144291393782</v>
+        <v>48.161192599725332</v>
       </c>
       <c r="O17" s="53"/>
       <c r="P17" s="53" cm="1">
         <f t="array" ref="P17">AVERAGE(ABS(P2:P15))</f>
-        <v>139.31090112812282</v>
+        <v>116.13760891259462</v>
       </c>
       <c r="Q17" s="53"/>
       <c r="R17" s="53" cm="1">
         <f t="array" ref="R17">AVERAGE(ABS(R2:R15))</f>
-        <v>290.04964263744279</v>
+        <v>249.22521274710371</v>
       </c>
       <c r="S17" s="53"/>
       <c r="T17" s="53" t="e" cm="1">
@@ -3513,49 +3519,88 @@
         <v>#DIV/0!</v>
       </c>
     </row>
+    <row r="19" spans="1:20">
+      <c r="C19" s="111"/>
+      <c r="D19" s="100"/>
+      <c r="E19" s="110"/>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="C20" s="111"/>
+      <c r="D20" s="100"/>
+      <c r="E20" s="110"/>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="C21" s="111"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="110"/>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="C22" s="111"/>
+      <c r="D22" s="100"/>
+      <c r="E22" s="110"/>
+    </row>
     <row r="23" spans="1:20">
-      <c r="C23" s="109"/>
+      <c r="C23" s="111"/>
+      <c r="D23" s="100"/>
+      <c r="E23" s="110"/>
     </row>
     <row r="24" spans="1:20">
-      <c r="C24" s="109"/>
+      <c r="C24" s="111"/>
+      <c r="D24" s="100"/>
+      <c r="E24" s="110"/>
     </row>
     <row r="25" spans="1:20">
-      <c r="C25" s="109"/>
+      <c r="C25" s="111"/>
+      <c r="D25" s="100"/>
+      <c r="E25" s="110"/>
     </row>
     <row r="26" spans="1:20">
-      <c r="C26" s="109"/>
+      <c r="C26" s="111"/>
+      <c r="D26" s="100"/>
+      <c r="E26" s="110"/>
     </row>
     <row r="27" spans="1:20">
-      <c r="C27" s="109"/>
+      <c r="C27" s="111"/>
+      <c r="D27" s="100"/>
+      <c r="E27" s="110"/>
     </row>
     <row r="28" spans="1:20">
-      <c r="C28" s="109"/>
+      <c r="C28" s="111"/>
+      <c r="D28" s="100"/>
+      <c r="E28" s="110"/>
     </row>
     <row r="29" spans="1:20">
-      <c r="C29" s="109"/>
+      <c r="C29" s="111"/>
+      <c r="D29" s="100"/>
+      <c r="E29" s="110"/>
       <c r="J29" s="60"/>
     </row>
     <row r="30" spans="1:20">
-      <c r="C30" s="109"/>
+      <c r="C30" s="111"/>
+      <c r="D30" s="100"/>
+      <c r="E30" s="110"/>
     </row>
     <row r="31" spans="1:20">
-      <c r="C31" s="109"/>
+      <c r="C31" s="111"/>
+      <c r="D31" s="100"/>
+      <c r="E31" s="110"/>
     </row>
     <row r="32" spans="1:20">
-      <c r="C32" s="109"/>
-      <c r="E32" s="60"/>
+      <c r="C32" s="111"/>
+      <c r="D32" s="100"/>
+      <c r="E32" s="110"/>
     </row>
     <row r="33" spans="3:3">
-      <c r="C33" s="109"/>
+      <c r="C33" s="100"/>
     </row>
     <row r="34" spans="3:3">
-      <c r="C34" s="109"/>
+      <c r="C34" s="100"/>
     </row>
     <row r="35" spans="3:3">
-      <c r="C35" s="109"/>
+      <c r="C35" s="100"/>
     </row>
     <row r="36" spans="3:3">
-      <c r="C36" s="109"/>
+      <c r="C36" s="100"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
Update KVFinder project benchmarking results
</commit_message>
<xml_diff>
--- a/results/quantitative-analysis.xlsx
+++ b/results/quantitative-analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gyorgy Szaloki\Papers\Cavity calculations\Benchmarking\Structures for benchmarking\QUANTITATIVE ANALYSIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F864CA71-932A-4633-B7BB-4346757AD65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4F624E5-5F5C-4570-A19E-7787D4848DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -329,7 +329,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -338,126 +338,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
@@ -803,163 +683,99 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -974,152 +790,155 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1128,11 +947,197 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1526,837 +1531,837 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="70" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="71" t="s">
+      <c r="F1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="72" t="s">
+      <c r="G1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="73" t="s">
+      <c r="H1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="74" t="s">
+      <c r="I1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="75" t="s">
+      <c r="J1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="76" t="s">
+      <c r="K1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="77" t="s">
+      <c r="L1" s="29" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="80">
+      <c r="C2" s="32">
         <f>Calculations!C2</f>
         <v>137.38999999999999</v>
       </c>
-      <c r="D2" s="80">
+      <c r="D2" s="32">
         <f>Calculations!D2</f>
         <v>249.79999999999995</v>
       </c>
-      <c r="E2" s="81" t="str">
+      <c r="E2" s="33" t="str">
         <f>ROUND(Calculations!E2,0)&amp;" ("&amp;ROUND(Calculations!F2,1)&amp;"%)"</f>
         <v>284 (12.1%)</v>
       </c>
-      <c r="F2" s="58" t="str">
+      <c r="F2" s="10" t="str">
         <f>ROUND(Calculations!G2,0)&amp;" ("&amp;ROUND(Calculations!H2,1)&amp;"%)"</f>
         <v>282 (11.5%)</v>
       </c>
-      <c r="G2" s="58" t="str">
+      <c r="G2" s="10" t="str">
         <f>ROUND(Calculations!I2,0)&amp;" ("&amp;ROUND(Calculations!J2,1)&amp;"%)"</f>
         <v>261 (4.3%)</v>
       </c>
-      <c r="H2" s="58" t="str">
+      <c r="H2" s="10" t="str">
         <f>ROUND(Calculations!K2,0)&amp;" ("&amp;ROUND(Calculations!L2,1)&amp;"%)"</f>
         <v>247 (-1%)</v>
       </c>
-      <c r="I2" s="58" t="str">
+      <c r="I2" s="10" t="str">
         <f>ROUND(Calculations!M2,0)&amp;" ("&amp;ROUND(Calculations!N2,1)&amp;"%)"</f>
         <v>175 (-42.7%)</v>
       </c>
-      <c r="J2" s="58" t="str">
+      <c r="J2" s="10" t="str">
         <f>ROUND(Calculations!O2,0)&amp;" ("&amp;ROUND(Calculations!P2,1)&amp;"%)"</f>
         <v>133 (-87.9%)</v>
       </c>
-      <c r="K2" s="58" t="str">
+      <c r="K2" s="10" t="str">
         <f>ROUND(Calculations!Q2,0)&amp;" ("&amp;ROUND(Calculations!R2,1)&amp;"%)"</f>
         <v>109 (-129.2%)</v>
       </c>
-      <c r="L2" s="59" t="str">
+      <c r="L2" s="11" t="str">
         <f>ROUND(Calculations!S2,0)&amp;" ("&amp;ROUND(Calculations!T2,1)&amp;"%)"</f>
         <v>396 (36.9%)</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="80">
+      <c r="C3" s="32">
         <f>Calculations!C3</f>
         <v>146.03</v>
       </c>
-      <c r="D3" s="80">
+      <c r="D3" s="32">
         <f>Calculations!D3</f>
         <v>265.5090909090909</v>
       </c>
-      <c r="E3" s="81" t="str">
+      <c r="E3" s="33" t="str">
         <f>ROUND(Calculations!E3,0)&amp;" ("&amp;ROUND(Calculations!F3,1)&amp;"%)"</f>
         <v>261 (-1.7%)</v>
       </c>
-      <c r="F3" s="58" t="str">
+      <c r="F3" s="10" t="str">
         <f>ROUND(Calculations!G3,0)&amp;" ("&amp;ROUND(Calculations!H3,1)&amp;"%)"</f>
         <v>261 (-1.6%)</v>
       </c>
-      <c r="G3" s="58" t="str">
+      <c r="G3" s="10" t="str">
         <f>ROUND(Calculations!I3,0)&amp;" ("&amp;ROUND(Calculations!J3,1)&amp;"%)"</f>
         <v>241 (-10.2%)</v>
       </c>
-      <c r="H3" s="58" t="str">
+      <c r="H3" s="10" t="str">
         <f>ROUND(Calculations!K3,0)&amp;" ("&amp;ROUND(Calculations!L3,1)&amp;"%)"</f>
         <v>246 (-7.8%)</v>
       </c>
-      <c r="I3" s="58" t="str">
+      <c r="I3" s="10" t="str">
         <f>ROUND(Calculations!M3,0)&amp;" ("&amp;ROUND(Calculations!N3,1)&amp;"%)"</f>
         <v>180 (-47.8%)</v>
       </c>
-      <c r="J3" s="58" t="str">
+      <c r="J3" s="10" t="str">
         <f>ROUND(Calculations!O3,0)&amp;" ("&amp;ROUND(Calculations!P3,1)&amp;"%)"</f>
         <v>90 (-196.4%)</v>
       </c>
-      <c r="K3" s="58" t="str">
+      <c r="K3" s="10" t="str">
         <f>ROUND(Calculations!Q3,0)&amp;" ("&amp;ROUND(Calculations!R3,1)&amp;"%)"</f>
         <v>92 (-188.6%)</v>
       </c>
-      <c r="L3" s="59" t="str">
+      <c r="L3" s="11" t="str">
         <f>ROUND(Calculations!S3,0)&amp;" ("&amp;ROUND(Calculations!T3,1)&amp;"%)"</f>
-        <v>267 (0.6%)</v>
+        <v>267 (0.4%)</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="80">
+      <c r="C4" s="32">
         <f>Calculations!C4</f>
         <v>129.1</v>
       </c>
-      <c r="D4" s="80">
+      <c r="D4" s="32">
         <f>Calculations!D4</f>
         <v>234.72727272727269</v>
       </c>
-      <c r="E4" s="81" t="str">
+      <c r="E4" s="33" t="str">
         <f>ROUND(Calculations!E4,0)&amp;" ("&amp;ROUND(Calculations!F4,1)&amp;"%)"</f>
         <v>270 (13.2%)</v>
       </c>
-      <c r="F4" s="58" t="str">
+      <c r="F4" s="10" t="str">
         <f>ROUND(Calculations!G4,0)&amp;" ("&amp;ROUND(Calculations!H4,1)&amp;"%)"</f>
         <v>270 (13.2%)</v>
       </c>
-      <c r="G4" s="58" t="str">
+      <c r="G4" s="10" t="str">
         <f>ROUND(Calculations!I4,0)&amp;" ("&amp;ROUND(Calculations!J4,1)&amp;"%)"</f>
         <v>253 (7%)</v>
       </c>
-      <c r="H4" s="58" t="str">
+      <c r="H4" s="10" t="str">
         <f>ROUND(Calculations!K4,0)&amp;" ("&amp;ROUND(Calculations!L4,1)&amp;"%)"</f>
         <v>277 (15.3%)</v>
       </c>
-      <c r="I4" s="58" t="str">
+      <c r="I4" s="10" t="str">
         <f>ROUND(Calculations!M4,0)&amp;" ("&amp;ROUND(Calculations!N4,1)&amp;"%)"</f>
         <v>191 (-23.2%)</v>
       </c>
-      <c r="J4" s="58" t="str">
+      <c r="J4" s="10" t="str">
         <f>ROUND(Calculations!O4,0)&amp;" ("&amp;ROUND(Calculations!P4,1)&amp;"%)"</f>
         <v>113 (-108.1%)</v>
       </c>
-      <c r="K4" s="58" t="str">
+      <c r="K4" s="10" t="str">
         <f>ROUND(Calculations!Q4,0)&amp;" ("&amp;ROUND(Calculations!R4,1)&amp;"%)"</f>
         <v>99 (-137.1%)</v>
       </c>
-      <c r="L4" s="59" t="str">
+      <c r="L4" s="11" t="str">
         <f>ROUND(Calculations!S4,0)&amp;" ("&amp;ROUND(Calculations!T4,1)&amp;"%)"</f>
-        <v>335 (29.9%)</v>
+        <v>335 (30%)</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="80">
+      <c r="C5" s="32">
         <f>Calculations!C5</f>
         <v>271.23</v>
       </c>
-      <c r="D5" s="80">
+      <c r="D5" s="32">
         <f>Calculations!D5</f>
         <v>493.14545454545453</v>
       </c>
-      <c r="E5" s="81" t="str">
+      <c r="E5" s="33" t="str">
         <f>ROUND(Calculations!E5,0)&amp;" ("&amp;ROUND(Calculations!F5,1)&amp;"%)"</f>
-        <v>413 (-19.4%)</v>
-      </c>
-      <c r="F5" s="58" t="str">
+        <v>438 (-12.7%)</v>
+      </c>
+      <c r="F5" s="10" t="str">
         <f>ROUND(Calculations!G5,0)&amp;" ("&amp;ROUND(Calculations!H5,1)&amp;"%)"</f>
-        <v>413 (-19.5%)</v>
-      </c>
-      <c r="G5" s="58" t="str">
+        <v>436 (-13.2%)</v>
+      </c>
+      <c r="G5" s="10" t="str">
         <f>ROUND(Calculations!I5,0)&amp;" ("&amp;ROUND(Calculations!J5,1)&amp;"%)"</f>
         <v>410 (-20.2%)</v>
       </c>
-      <c r="H5" s="58" t="str">
+      <c r="H5" s="10" t="str">
         <f>ROUND(Calculations!K5,0)&amp;" ("&amp;ROUND(Calculations!L5,1)&amp;"%)"</f>
         <v>434 (-13.5%)</v>
       </c>
-      <c r="I5" s="58" t="str">
+      <c r="I5" s="10" t="str">
         <f>ROUND(Calculations!M5,0)&amp;" ("&amp;ROUND(Calculations!N5,1)&amp;"%)"</f>
         <v>343 (-43.8%)</v>
       </c>
-      <c r="J5" s="58" t="str">
+      <c r="J5" s="10" t="str">
         <f>ROUND(Calculations!O5,0)&amp;" ("&amp;ROUND(Calculations!P5,1)&amp;"%)"</f>
         <v>251 (-96.7%)</v>
       </c>
-      <c r="K5" s="58" t="str">
+      <c r="K5" s="10" t="str">
         <f>ROUND(Calculations!Q5,0)&amp;" ("&amp;ROUND(Calculations!R5,1)&amp;"%)"</f>
         <v>222 (-122.1%)</v>
       </c>
-      <c r="L5" s="59" t="str">
+      <c r="L5" s="11" t="str">
         <f>ROUND(Calculations!S5,0)&amp;" ("&amp;ROUND(Calculations!T5,1)&amp;"%)"</f>
-        <v>474 (-4%)</v>
+        <v>474 (-4.1%)</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="80">
+      <c r="C6" s="32">
         <f>Calculations!C6</f>
         <v>40.74</v>
       </c>
-      <c r="D6" s="80">
+      <c r="D6" s="32">
         <f>Calculations!D6</f>
         <v>74.072727272727263</v>
       </c>
-      <c r="E6" s="81" t="str">
+      <c r="E6" s="33" t="str">
         <f>ROUND(Calculations!E6,0)&amp;" ("&amp;ROUND(Calculations!F6,1)&amp;"%)"</f>
         <v>79 (5.8%)</v>
       </c>
-      <c r="F6" s="58" t="str">
+      <c r="F6" s="10" t="str">
         <f>ROUND(Calculations!G6,0)&amp;" ("&amp;ROUND(Calculations!H6,1)&amp;"%)"</f>
         <v>78 (5.1%)</v>
       </c>
-      <c r="G6" s="58" t="str">
+      <c r="G6" s="10" t="str">
         <f>ROUND(Calculations!I6,0)&amp;" ("&amp;ROUND(Calculations!J6,1)&amp;"%)"</f>
         <v>44 (-68.9%)</v>
       </c>
-      <c r="H6" s="58" t="str">
+      <c r="H6" s="10" t="str">
         <f>ROUND(Calculations!K6,0)&amp;" ("&amp;ROUND(Calculations!L6,1)&amp;"%)"</f>
         <v>84 (12.2%)</v>
       </c>
-      <c r="I6" s="58" t="str">
+      <c r="I6" s="10" t="str">
         <f>ROUND(Calculations!M6,0)&amp;" ("&amp;ROUND(Calculations!N6,1)&amp;"%)"</f>
         <v>29 (-153.7%)</v>
       </c>
-      <c r="J6" s="58" t="str">
+      <c r="J6" s="10" t="str">
         <f>ROUND(Calculations!O6,0)&amp;" ("&amp;ROUND(Calculations!P6,1)&amp;"%)"</f>
         <v>37 (-101.4%)</v>
       </c>
-      <c r="K6" s="58" t="str">
+      <c r="K6" s="10" t="str">
         <f>ROUND(Calculations!Q6,0)&amp;" ("&amp;ROUND(Calculations!R6,1)&amp;"%)"</f>
         <v>11 (-605.5%)</v>
       </c>
-      <c r="L6" s="59" t="e">
+      <c r="L6" s="11" t="str">
         <f>ROUND(Calculations!S6,0)&amp;" ("&amp;ROUND(Calculations!T6,1)&amp;"%)"</f>
-        <v>#DIV/0!</v>
+        <v>65 (-13.3%)</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="80">
+      <c r="C7" s="32">
         <f>Calculations!C7</f>
         <v>65.87</v>
       </c>
-      <c r="D7" s="80">
+      <c r="D7" s="32">
         <f>Calculations!D7</f>
         <v>119.76363636363637</v>
       </c>
-      <c r="E7" s="81" t="str">
+      <c r="E7" s="33" t="str">
         <f>ROUND(Calculations!E7,0)&amp;" ("&amp;ROUND(Calculations!F7,1)&amp;"%)"</f>
         <v>80 (-49.2%)</v>
       </c>
-      <c r="F7" s="58" t="str">
+      <c r="F7" s="10" t="str">
         <f>ROUND(Calculations!G7,0)&amp;" ("&amp;ROUND(Calculations!H7,1)&amp;"%)"</f>
         <v>81 (-47.5%)</v>
       </c>
-      <c r="G7" s="58" t="str">
+      <c r="G7" s="10" t="str">
         <f>ROUND(Calculations!I7,0)&amp;" ("&amp;ROUND(Calculations!J7,1)&amp;"%)"</f>
         <v>55 (-117.4%)</v>
       </c>
-      <c r="H7" s="58" t="str">
+      <c r="H7" s="10" t="str">
         <f>ROUND(Calculations!K7,0)&amp;" ("&amp;ROUND(Calculations!L7,1)&amp;"%)"</f>
         <v>82 (-45.9%)</v>
       </c>
-      <c r="I7" s="58" t="str">
+      <c r="I7" s="10" t="str">
         <f>ROUND(Calculations!M7,0)&amp;" ("&amp;ROUND(Calculations!N7,1)&amp;"%)"</f>
         <v>64 (-88.6%)</v>
       </c>
-      <c r="J7" s="58" t="str">
+      <c r="J7" s="10" t="str">
         <f>ROUND(Calculations!O7,0)&amp;" ("&amp;ROUND(Calculations!P7,1)&amp;"%)"</f>
         <v>40 (-203.2%)</v>
       </c>
-      <c r="K7" s="58" t="str">
+      <c r="K7" s="10" t="str">
         <f>ROUND(Calculations!Q7,0)&amp;" ("&amp;ROUND(Calculations!R7,1)&amp;"%)"</f>
         <v>11 (-1014.1%)</v>
       </c>
-      <c r="L7" s="59" t="e">
+      <c r="L7" s="11" t="str">
         <f>ROUND(Calculations!S7,0)&amp;" ("&amp;ROUND(Calculations!T7,1)&amp;"%)"</f>
-        <v>#DIV/0!</v>
+        <v>79 (-51.4%)</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="80">
+      <c r="C8" s="32">
         <f>Calculations!C8</f>
         <v>487.72</v>
       </c>
-      <c r="D8" s="80">
+      <c r="D8" s="32">
         <f>Calculations!D8</f>
         <v>886.76363636363635</v>
       </c>
-      <c r="E8" s="81" t="str">
+      <c r="E8" s="33" t="str">
         <f>ROUND(Calculations!E8,0)&amp;" ("&amp;ROUND(Calculations!F8,1)&amp;"%)"</f>
         <v>755 (-17.5%)</v>
       </c>
-      <c r="F8" s="58" t="str">
+      <c r="F8" s="10" t="str">
         <f>ROUND(Calculations!G8,0)&amp;" ("&amp;ROUND(Calculations!H8,1)&amp;"%)"</f>
         <v>759 (-16.9%)</v>
       </c>
-      <c r="G8" s="58" t="str">
+      <c r="G8" s="10" t="str">
         <f>ROUND(Calculations!I8,0)&amp;" ("&amp;ROUND(Calculations!J8,1)&amp;"%)"</f>
         <v>708 (-25.2%)</v>
       </c>
-      <c r="H8" s="58" t="str">
+      <c r="H8" s="10" t="str">
         <f>ROUND(Calculations!K8,0)&amp;" ("&amp;ROUND(Calculations!L8,1)&amp;"%)"</f>
         <v>771 (-15%)</v>
       </c>
-      <c r="I8" s="58" t="str">
+      <c r="I8" s="10" t="str">
         <f>ROUND(Calculations!M8,0)&amp;" ("&amp;ROUND(Calculations!N8,1)&amp;"%)"</f>
         <v>734 (-20.9%)</v>
       </c>
-      <c r="J8" s="58" t="str">
+      <c r="J8" s="10" t="str">
         <f>ROUND(Calculations!O8,0)&amp;" ("&amp;ROUND(Calculations!P8,1)&amp;"%)"</f>
         <v>492 (-80.3%)</v>
       </c>
-      <c r="K8" s="58" t="str">
+      <c r="K8" s="10" t="str">
         <f>ROUND(Calculations!Q8,0)&amp;" ("&amp;ROUND(Calculations!R8,1)&amp;"%)"</f>
         <v>385 (-130.3%)</v>
       </c>
-      <c r="L8" s="59" t="e">
+      <c r="L8" s="11" t="str">
         <f>ROUND(Calculations!S8,0)&amp;" ("&amp;ROUND(Calculations!T8,1)&amp;"%)"</f>
-        <v>#DIV/0!</v>
+        <v>778 (-14%)</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="80">
+      <c r="C9" s="32">
         <f>Calculations!C9</f>
         <v>480.87</v>
       </c>
-      <c r="D9" s="80">
+      <c r="D9" s="32">
         <f>Calculations!D9</f>
         <v>874.30909090909086</v>
       </c>
-      <c r="E9" s="81" t="str">
+      <c r="E9" s="33" t="str">
         <f>ROUND(Calculations!E9,0)&amp;" ("&amp;ROUND(Calculations!F9,1)&amp;"%)"</f>
         <v>730 (-19.8%)</v>
       </c>
-      <c r="F9" s="58" t="str">
+      <c r="F9" s="10" t="str">
         <f>ROUND(Calculations!G9,0)&amp;" ("&amp;ROUND(Calculations!H9,1)&amp;"%)"</f>
         <v>730 (-19.7%)</v>
       </c>
-      <c r="G9" s="58" t="str">
+      <c r="G9" s="10" t="str">
         <f>ROUND(Calculations!I9,0)&amp;" ("&amp;ROUND(Calculations!J9,1)&amp;"%)"</f>
         <v>747 (-17%)</v>
       </c>
-      <c r="H9" s="58" t="str">
+      <c r="H9" s="10" t="str">
         <f>ROUND(Calculations!K9,0)&amp;" ("&amp;ROUND(Calculations!L9,1)&amp;"%)"</f>
         <v>805 (-8.7%)</v>
       </c>
-      <c r="I9" s="58" t="str">
+      <c r="I9" s="10" t="str">
         <f>ROUND(Calculations!M9,0)&amp;" ("&amp;ROUND(Calculations!N9,1)&amp;"%)"</f>
         <v>704 (-24.2%)</v>
       </c>
-      <c r="J9" s="58" t="str">
+      <c r="J9" s="10" t="str">
         <f>ROUND(Calculations!O9,0)&amp;" ("&amp;ROUND(Calculations!P9,1)&amp;"%)"</f>
         <v>517 (-69.1%)</v>
       </c>
-      <c r="K9" s="58" t="str">
+      <c r="K9" s="10" t="str">
         <f>ROUND(Calculations!Q9,0)&amp;" ("&amp;ROUND(Calculations!R9,1)&amp;"%)"</f>
         <v>409 (-113.8%)</v>
       </c>
-      <c r="L9" s="59" t="e">
+      <c r="L9" s="11" t="str">
         <f>ROUND(Calculations!S9,0)&amp;" ("&amp;ROUND(Calculations!T9,1)&amp;"%)"</f>
-        <v>#DIV/0!</v>
+        <v>682 (-28.3%)</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="80">
+      <c r="C10" s="32">
         <f>Calculations!C10</f>
         <v>135.84</v>
       </c>
-      <c r="D10" s="80">
+      <c r="D10" s="32">
         <f>Calculations!D10</f>
         <v>246.98181818181817</v>
       </c>
-      <c r="E10" s="81" t="str">
+      <c r="E10" s="33" t="str">
         <f>ROUND(Calculations!E10,0)&amp;" ("&amp;ROUND(Calculations!F10,1)&amp;"%)"</f>
         <v>156 (-58.4%)</v>
       </c>
-      <c r="F10" s="58" t="str">
+      <c r="F10" s="10" t="str">
         <f>ROUND(Calculations!G10,0)&amp;" ("&amp;ROUND(Calculations!H10,1)&amp;"%)"</f>
         <v>155 (-59.8%)</v>
       </c>
-      <c r="G10" s="58" t="str">
+      <c r="G10" s="10" t="str">
         <f>ROUND(Calculations!I10,0)&amp;" ("&amp;ROUND(Calculations!J10,1)&amp;"%)"</f>
         <v>177 (-39.6%)</v>
       </c>
-      <c r="H10" s="58" t="str">
+      <c r="H10" s="10" t="str">
         <f>ROUND(Calculations!K10,0)&amp;" ("&amp;ROUND(Calculations!L10,1)&amp;"%)"</f>
         <v>181 (-36.5%)</v>
       </c>
-      <c r="I10" s="58" t="str">
+      <c r="I10" s="10" t="str">
         <f>ROUND(Calculations!M10,0)&amp;" ("&amp;ROUND(Calculations!N10,1)&amp;"%)"</f>
         <v>159 (-55.1%)</v>
       </c>
-      <c r="J10" s="58" t="str">
+      <c r="J10" s="10" t="str">
         <f>ROUND(Calculations!O10,0)&amp;" ("&amp;ROUND(Calculations!P10,1)&amp;"%)"</f>
         <v>122 (-102.2%)</v>
       </c>
-      <c r="K10" s="58" t="str">
+      <c r="K10" s="10" t="str">
         <f>ROUND(Calculations!Q10,0)&amp;" ("&amp;ROUND(Calculations!R10,1)&amp;"%)"</f>
         <v>62 (-298.4%)</v>
       </c>
-      <c r="L10" s="59" t="e">
+      <c r="L10" s="11" t="str">
         <f>ROUND(Calculations!S10,0)&amp;" ("&amp;ROUND(Calculations!T10,1)&amp;"%)"</f>
-        <v>#DIV/0!</v>
+        <v>173 (-42.5%)</v>
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="80">
+      <c r="C11" s="32">
         <f>Calculations!C11</f>
         <v>130.58000000000001</v>
       </c>
-      <c r="D11" s="80">
+      <c r="D11" s="32">
         <f>Calculations!D11</f>
         <v>237.41818181818184</v>
       </c>
-      <c r="E11" s="81" t="str">
+      <c r="E11" s="33" t="str">
         <f>ROUND(Calculations!E11,0)&amp;" ("&amp;ROUND(Calculations!F11,1)&amp;"%)"</f>
         <v>246 (3.6%)</v>
       </c>
-      <c r="F11" s="58" t="str">
+      <c r="F11" s="10" t="str">
         <f>ROUND(Calculations!G11,0)&amp;" ("&amp;ROUND(Calculations!H11,1)&amp;"%)"</f>
         <v>248 (4.2%)</v>
       </c>
-      <c r="G11" s="58" t="str">
+      <c r="G11" s="10" t="str">
         <f>ROUND(Calculations!I11,0)&amp;" ("&amp;ROUND(Calculations!J11,1)&amp;"%)"</f>
         <v>225 (-5.4%)</v>
       </c>
-      <c r="H11" s="58" t="str">
+      <c r="H11" s="10" t="str">
         <f>ROUND(Calculations!K11,0)&amp;" ("&amp;ROUND(Calculations!L11,1)&amp;"%)"</f>
         <v>225 (-5.4%)</v>
       </c>
-      <c r="I11" s="58" t="str">
+      <c r="I11" s="10" t="str">
         <f>ROUND(Calculations!M11,0)&amp;" ("&amp;ROUND(Calculations!N11,1)&amp;"%)"</f>
         <v>161 (-47.2%)</v>
       </c>
-      <c r="J11" s="58" t="str">
+      <c r="J11" s="10" t="str">
         <f>ROUND(Calculations!O11,0)&amp;" ("&amp;ROUND(Calculations!P11,1)&amp;"%)"</f>
         <v>125 (-90.5%)</v>
       </c>
-      <c r="K11" s="58" t="str">
+      <c r="K11" s="10" t="str">
         <f>ROUND(Calculations!Q11,0)&amp;" ("&amp;ROUND(Calculations!R11,1)&amp;"%)"</f>
         <v>94 (-152.6%)</v>
       </c>
-      <c r="L11" s="59" t="e">
+      <c r="L11" s="11" t="str">
         <f>ROUND(Calculations!S11,0)&amp;" ("&amp;ROUND(Calculations!T11,1)&amp;"%)"</f>
-        <v>#DIV/0!</v>
+        <v>351 (32.3%)</v>
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="80">
+      <c r="C12" s="32">
         <f>Calculations!C12</f>
         <v>209.55</v>
       </c>
-      <c r="D12" s="80">
+      <c r="D12" s="32">
         <f>Calculations!D12</f>
         <v>381</v>
       </c>
-      <c r="E12" s="81" t="str">
+      <c r="E12" s="33" t="str">
         <f>ROUND(Calculations!E12,0)&amp;" ("&amp;ROUND(Calculations!F12,1)&amp;"%)"</f>
-        <v>229 (-66.3%)</v>
-      </c>
-      <c r="F12" s="58" t="str">
+        <v>317 (-20.1%)</v>
+      </c>
+      <c r="F12" s="10" t="str">
         <f>ROUND(Calculations!G12,0)&amp;" ("&amp;ROUND(Calculations!H12,1)&amp;"%)"</f>
-        <v>230 (-65.6%)</v>
-      </c>
-      <c r="G12" s="58" t="str">
+        <v>317 (-20%)</v>
+      </c>
+      <c r="G12" s="10" t="str">
         <f>ROUND(Calculations!I12,0)&amp;" ("&amp;ROUND(Calculations!J12,1)&amp;"%)"</f>
         <v>389 (2.1%)</v>
       </c>
-      <c r="H12" s="58" t="str">
+      <c r="H12" s="10" t="str">
         <f>ROUND(Calculations!K12,0)&amp;" ("&amp;ROUND(Calculations!L12,1)&amp;"%)"</f>
         <v>652 (41.6%)</v>
       </c>
-      <c r="I12" s="58" t="str">
+      <c r="I12" s="10" t="str">
         <f>ROUND(Calculations!M12,0)&amp;" ("&amp;ROUND(Calculations!N12,1)&amp;"%)"</f>
         <v>349 (-9.3%)</v>
       </c>
-      <c r="J12" s="58" t="str">
+      <c r="J12" s="10" t="str">
         <f>ROUND(Calculations!O12,0)&amp;" ("&amp;ROUND(Calculations!P12,1)&amp;"%)"</f>
         <v>114 (-235.6%)</v>
       </c>
-      <c r="K12" s="58" t="str">
+      <c r="K12" s="10" t="str">
         <f>ROUND(Calculations!Q12,0)&amp;" ("&amp;ROUND(Calculations!R12,1)&amp;"%)"</f>
         <v>164 (-132.3%)</v>
       </c>
-      <c r="L12" s="59" t="e">
+      <c r="L12" s="11" t="str">
         <f>ROUND(Calculations!S12,0)&amp;" ("&amp;ROUND(Calculations!T12,1)&amp;"%)"</f>
-        <v>#DIV/0!</v>
+        <v>227 (-68%)</v>
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="64" t="s">
+      <c r="A13" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="80">
+      <c r="C13" s="32">
         <f>Calculations!C13</f>
         <v>285.27999999999997</v>
       </c>
-      <c r="D13" s="80">
+      <c r="D13" s="32">
         <f>Calculations!D13</f>
         <v>518.69090909090903</v>
       </c>
-      <c r="E13" s="81" t="str">
+      <c r="E13" s="33" t="str">
         <f>ROUND(Calculations!E13,0)&amp;" ("&amp;ROUND(Calculations!F13,1)&amp;"%)"</f>
         <v>494 (-5.1%)</v>
       </c>
-      <c r="F13" s="58" t="str">
+      <c r="F13" s="10" t="str">
         <f>ROUND(Calculations!G13,0)&amp;" ("&amp;ROUND(Calculations!H13,1)&amp;"%)"</f>
         <v>498 (-4.3%)</v>
       </c>
-      <c r="G13" s="58" t="str">
+      <c r="G13" s="10" t="str">
         <f>ROUND(Calculations!I13,0)&amp;" ("&amp;ROUND(Calculations!J13,1)&amp;"%)"</f>
         <v>435 (-19.3%)</v>
       </c>
-      <c r="H13" s="58" t="str">
+      <c r="H13" s="10" t="str">
         <f>ROUND(Calculations!K13,0)&amp;" ("&amp;ROUND(Calculations!L13,1)&amp;"%)"</f>
         <v>482 (-7.7%)</v>
       </c>
-      <c r="I13" s="58" t="str">
+      <c r="I13" s="10" t="str">
         <f>ROUND(Calculations!M13,0)&amp;" ("&amp;ROUND(Calculations!N13,1)&amp;"%)"</f>
         <v>401 (-29.4%)</v>
       </c>
-      <c r="J13" s="58" t="str">
+      <c r="J13" s="10" t="str">
         <f>ROUND(Calculations!O13,0)&amp;" ("&amp;ROUND(Calculations!P13,1)&amp;"%)"</f>
         <v>265 (-95.6%)</v>
       </c>
-      <c r="K13" s="58" t="str">
+      <c r="K13" s="10" t="str">
         <f>ROUND(Calculations!Q13,0)&amp;" ("&amp;ROUND(Calculations!R13,1)&amp;"%)"</f>
         <v>208 (-149.4%)</v>
       </c>
-      <c r="L13" s="59" t="e">
+      <c r="L13" s="11" t="str">
         <f>ROUND(Calculations!S13,0)&amp;" ("&amp;ROUND(Calculations!T13,1)&amp;"%)"</f>
-        <v>#DIV/0!</v>
+        <v>457 (-13.6%)</v>
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="64" t="s">
+      <c r="A14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="80">
+      <c r="C14" s="32">
         <f>Calculations!C14</f>
         <v>492.76</v>
       </c>
-      <c r="D14" s="80">
+      <c r="D14" s="32">
         <f>Calculations!D14</f>
         <v>895.92727272727268</v>
       </c>
-      <c r="E14" s="81" t="str">
+      <c r="E14" s="33" t="str">
         <f>ROUND(Calculations!E14,0)&amp;" ("&amp;ROUND(Calculations!F14,1)&amp;"%)"</f>
         <v>736 (-21.7%)</v>
       </c>
-      <c r="F14" s="58" t="str">
+      <c r="F14" s="10" t="str">
         <f>ROUND(Calculations!G14,0)&amp;" ("&amp;ROUND(Calculations!H14,1)&amp;"%)"</f>
         <v>738 (-21.3%)</v>
       </c>
-      <c r="G14" s="58" t="str">
+      <c r="G14" s="10" t="str">
         <f>ROUND(Calculations!I14,0)&amp;" ("&amp;ROUND(Calculations!J14,1)&amp;"%)"</f>
         <v>650 (-37.8%)</v>
       </c>
-      <c r="H14" s="58" t="str">
+      <c r="H14" s="10" t="str">
         <f>ROUND(Calculations!K14,0)&amp;" ("&amp;ROUND(Calculations!L14,1)&amp;"%)"</f>
         <v>627 (-42.8%)</v>
       </c>
-      <c r="I14" s="58" t="str">
+      <c r="I14" s="10" t="str">
         <f>ROUND(Calculations!M14,0)&amp;" ("&amp;ROUND(Calculations!N14,1)&amp;"%)"</f>
         <v>606 (-47.9%)</v>
       </c>
-      <c r="J14" s="58" t="str">
+      <c r="J14" s="10" t="str">
         <f>ROUND(Calculations!O14,0)&amp;" ("&amp;ROUND(Calculations!P14,1)&amp;"%)"</f>
         <v>532 (-68.5%)</v>
       </c>
-      <c r="K14" s="58" t="str">
+      <c r="K14" s="10" t="str">
         <f>ROUND(Calculations!Q14,0)&amp;" ("&amp;ROUND(Calculations!R14,1)&amp;"%)"</f>
         <v>319 (-180.9%)</v>
       </c>
-      <c r="L14" s="59" t="e">
+      <c r="L14" s="11" t="str">
         <f>ROUND(Calculations!S14,0)&amp;" ("&amp;ROUND(Calculations!T14,1)&amp;"%)"</f>
-        <v>#DIV/0!</v>
+        <v>742 (-20.7%)</v>
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="65" t="s">
+      <c r="A15" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="92" t="s">
+      <c r="B15" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="80">
+      <c r="C15" s="32">
         <f>Calculations!C15</f>
         <v>581.73</v>
       </c>
-      <c r="D15" s="80">
+      <c r="D15" s="32">
         <f>Calculations!D15</f>
         <v>1057.6909090909091</v>
       </c>
-      <c r="E15" s="82" t="str">
+      <c r="E15" s="34" t="str">
         <f>ROUND(Calculations!E15,0)&amp;" ("&amp;ROUND(Calculations!F15,1)&amp;"%)"</f>
         <v>872 (-21.3%)</v>
       </c>
-      <c r="F15" s="83" t="str">
+      <c r="F15" s="35" t="str">
         <f>ROUND(Calculations!G15,0)&amp;" ("&amp;ROUND(Calculations!H15,1)&amp;"%)"</f>
         <v>868 (-21.8%)</v>
       </c>
-      <c r="G15" s="83" t="str">
+      <c r="G15" s="35" t="str">
         <f>ROUND(Calculations!I15,0)&amp;" ("&amp;ROUND(Calculations!J15,1)&amp;"%)"</f>
         <v>821 (-28.9%)</v>
       </c>
-      <c r="H15" s="83" t="str">
+      <c r="H15" s="35" t="str">
         <f>ROUND(Calculations!K15,0)&amp;" ("&amp;ROUND(Calculations!L15,1)&amp;"%)"</f>
         <v>811 (-30.4%)</v>
       </c>
-      <c r="I15" s="83" t="str">
+      <c r="I15" s="35" t="str">
         <f>ROUND(Calculations!M15,0)&amp;" ("&amp;ROUND(Calculations!N15,1)&amp;"%)"</f>
         <v>752 (-40.6%)</v>
       </c>
-      <c r="J15" s="83" t="str">
+      <c r="J15" s="35" t="str">
         <f>ROUND(Calculations!O15,0)&amp;" ("&amp;ROUND(Calculations!P15,1)&amp;"%)"</f>
         <v>555 (-90.4%)</v>
       </c>
-      <c r="K15" s="83" t="str">
+      <c r="K15" s="35" t="str">
         <f>ROUND(Calculations!Q15,0)&amp;" ("&amp;ROUND(Calculations!R15,1)&amp;"%)"</f>
         <v>450 (-135%)</v>
       </c>
-      <c r="L15" s="84" t="e">
+      <c r="L15" s="36" t="str">
         <f>ROUND(Calculations!S15,0)&amp;" ("&amp;ROUND(Calculations!T15,1)&amp;"%)"</f>
-        <v>#DIV/0!</v>
+        <v>1031 (-2.5%)</v>
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="90" t="s">
+      <c r="A16" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="85" t="s">
+      <c r="B16" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="93" t="s">
+      <c r="C16" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="94" t="s">
+      <c r="D16" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="96" t="str">
+      <c r="E16" s="48" t="str">
         <f>ROUND(Calculations!F16,1)&amp;"%"</f>
-        <v>-17.6%</v>
-      </c>
-      <c r="F16" s="86" t="str">
+        <v>-13.8%</v>
+      </c>
+      <c r="F16" s="38" t="str">
         <f>ROUND(Calculations!H16,1)&amp;"%"</f>
-        <v>-17.4%</v>
-      </c>
-      <c r="G16" s="97" t="str">
+        <v>-13.7%</v>
+      </c>
+      <c r="G16" s="49" t="str">
         <f>ROUND(Calculations!J16,1)&amp;"%"</f>
         <v>-26.9%</v>
       </c>
-      <c r="H16" s="97" t="str">
+      <c r="H16" s="49" t="str">
         <f>ROUND(Calculations!L16,1)&amp;"%"</f>
         <v>-10.4%</v>
       </c>
-      <c r="I16" s="97" t="str">
+      <c r="I16" s="49" t="str">
         <f>ROUND(Calculations!N16,1)&amp;"%"</f>
         <v>-48.2%</v>
       </c>
-      <c r="J16" s="97" t="str">
+      <c r="J16" s="49" t="str">
         <f>ROUND(Calculations!P16,1)&amp;"%"</f>
         <v>-116.1%</v>
       </c>
-      <c r="K16" s="97" t="str">
+      <c r="K16" s="49" t="str">
         <f>ROUND(Calculations!R16,1)&amp;"%"</f>
         <v>-249.2%</v>
       </c>
-      <c r="L16" s="87" t="e">
+      <c r="L16" s="39" t="str">
         <f>ROUND(Calculations!T16,1)&amp;"%"</f>
-        <v>#DIV/0!</v>
+        <v>-11.3%</v>
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="91" t="s">
+      <c r="A17" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="62" t="s">
+      <c r="C17" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="63" t="s">
+      <c r="D17" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="98" t="str">
+      <c r="E17" s="50" t="str">
         <f>ROUND(Calculations!F17,1)&amp;"%"</f>
-        <v>22.5%</v>
-      </c>
-      <c r="F17" s="88" t="str">
+        <v>18.7%</v>
+      </c>
+      <c r="F17" s="40" t="str">
         <f>ROUND(Calculations!H17,1)&amp;"%"</f>
-        <v>22.3%</v>
-      </c>
-      <c r="G17" s="99" t="str">
+        <v>18.6%</v>
+      </c>
+      <c r="G17" s="51" t="str">
         <f>ROUND(Calculations!J17,1)&amp;"%"</f>
         <v>28.8%</v>
       </c>
-      <c r="H17" s="99" t="str">
+      <c r="H17" s="51" t="str">
         <f>ROUND(Calculations!L17,1)&amp;"%"</f>
         <v>20.3%</v>
       </c>
-      <c r="I17" s="99" t="str">
+      <c r="I17" s="51" t="str">
         <f>ROUND(Calculations!N17,1)&amp;"%"</f>
         <v>48.2%</v>
       </c>
-      <c r="J17" s="99" t="str">
+      <c r="J17" s="51" t="str">
         <f>ROUND(Calculations!P17,1)&amp;"%"</f>
         <v>116.1%</v>
       </c>
-      <c r="K17" s="99" t="str">
+      <c r="K17" s="51" t="str">
         <f>ROUND(Calculations!R17,1)&amp;"%"</f>
         <v>249.2%</v>
       </c>
-      <c r="L17" s="89" t="e">
+      <c r="L17" s="41" t="str">
         <f>ROUND(Calculations!T17,1)&amp;"%"</f>
-        <v>#DIV/0!</v>
+        <v>25.6%</v>
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="103" t="s">
+      <c r="A20" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="104"/>
-      <c r="C20" s="105"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="58"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="57" t="s">
+      <c r="A21" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="106" t="s">
+      <c r="B21" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="107"/>
+      <c r="C21" s="60"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="56" t="s">
+      <c r="A22" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="101" t="s">
+      <c r="B22" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="102"/>
+      <c r="C22" s="55"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="D27" s="95"/>
+      <c r="D27" s="47"/>
     </row>
     <row r="34" spans="7:7">
-      <c r="G34" s="95"/>
+      <c r="G34" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2373,7 +2378,7 @@
   <dimension ref="A1:T36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C19:C32"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -2389,22 +2394,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="49.5" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="103" t="s">
         <v>44</v>
       </c>
       <c r="G1" s="23" t="s">
@@ -2416,1191 +2421,1212 @@
       <c r="I1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="104" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="M1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="29" t="s">
+      <c r="N1" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="O1" s="30" t="s">
+      <c r="O1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="31" t="s">
+      <c r="P1" s="107" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="32" t="s">
+      <c r="Q1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="33" t="s">
+      <c r="R1" s="108" t="s">
         <v>49</v>
       </c>
-      <c r="S1" s="34" t="s">
+      <c r="S1" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="35" t="s">
+      <c r="T1" s="110" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="36">
+      <c r="C2" s="111">
         <v>137.38999999999999</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="112">
         <f t="shared" ref="D2:D15" si="0">C2/0.55</f>
         <v>249.79999999999995</v>
       </c>
-      <c r="E2" s="46">
+      <c r="E2" s="113">
         <v>284.02999999999997</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="114">
         <f>(E2-D2)/E2*100</f>
         <v>12.051543851001663</v>
       </c>
-      <c r="G2" s="48">
+      <c r="G2" s="115">
         <v>282.27999999999997</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="116">
         <f>(G2-D2)/G2*100</f>
         <v>11.506305795663888</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="117">
         <v>261.14400000000001</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="117">
         <f>(I2-D2)/I2*100</f>
         <v>4.3439634837484498</v>
       </c>
-      <c r="K2" s="12">
+      <c r="K2" s="118">
         <v>247.298</v>
       </c>
-      <c r="L2" s="12">
+      <c r="L2" s="118">
         <f>(K2-D2)/K2*100</f>
         <v>-1.0117348300430868</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="119">
         <v>175.1</v>
       </c>
-      <c r="N2" s="13">
+      <c r="N2" s="120">
         <f>(M2-D2)/M2*100</f>
         <v>-42.661336379211853</v>
       </c>
-      <c r="O2" s="5">
+      <c r="O2" s="121">
         <v>132.96</v>
       </c>
-      <c r="P2" s="14">
+      <c r="P2" s="122">
         <f>(O2-D2)/O2*100</f>
         <v>-87.876052948255065</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="Q2" s="123">
         <v>109</v>
       </c>
-      <c r="R2" s="15">
+      <c r="R2" s="124">
         <f>(Q2-D2)/Q2*100</f>
         <v>-129.17431192660547</v>
       </c>
-      <c r="S2" s="7">
-        <v>396</v>
-      </c>
-      <c r="T2" s="44">
+      <c r="S2" s="125">
+        <v>395.7</v>
+      </c>
+      <c r="T2" s="126">
         <f>(S2-D2)/S2*100</f>
-        <v>36.919191919191931</v>
+        <v>36.871367197371754</v>
       </c>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="36">
+      <c r="C3" s="67">
         <v>146.03</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="99">
         <f t="shared" si="0"/>
         <v>265.5090909090909</v>
       </c>
-      <c r="E3" s="46">
+      <c r="E3" s="83">
         <v>261.19</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="68">
         <f t="shared" ref="F3:F15" si="1">(E3-D3)/E3*100</f>
         <v>-1.6536203181939979</v>
       </c>
-      <c r="G3" s="48">
+      <c r="G3" s="69">
         <v>261.44</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="70">
         <f t="shared" ref="H3:H15" si="2">(G3-D3)/G3*100</f>
         <v>-1.556414821408699</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="71">
         <v>240.84</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="71">
         <f t="shared" ref="J3:J15" si="3">(I3-D3)/I3*100</f>
         <v>-10.242937597197683</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="72">
         <v>246.30699999999999</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="72">
         <f t="shared" ref="L3:L15" si="4">(K3-D3)/K3*100</f>
         <v>-7.795998858778237</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3" s="63">
         <v>179.7</v>
       </c>
-      <c r="N3" s="13">
+      <c r="N3" s="73">
         <f t="shared" ref="N3:N15" si="5">(M3-D3)/M3*100</f>
         <v>-47.751302676177474</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3" s="64">
         <v>89.58</v>
       </c>
-      <c r="P3" s="14">
+      <c r="P3" s="74">
         <f t="shared" ref="P3:P15" si="6">(O3-D3)/O3*100</f>
         <v>-196.39326960157504</v>
       </c>
-      <c r="Q3" s="6">
+      <c r="Q3" s="65">
         <v>92</v>
       </c>
-      <c r="R3" s="15">
+      <c r="R3" s="75">
         <f t="shared" ref="R3:R15" si="7">(Q3-D3)/Q3*100</f>
         <v>-188.59683794466403</v>
       </c>
-      <c r="S3" s="7">
-        <v>267</v>
-      </c>
-      <c r="T3" s="44">
+      <c r="S3" s="66">
+        <v>266.60000000000002</v>
+      </c>
+      <c r="T3" s="84">
         <f t="shared" ref="T3:T15" si="8">(S3-D3)/S3*100</f>
-        <v>0.55839291794348289</v>
+        <v>0.40919320739276888</v>
       </c>
     </row>
     <row r="4" spans="1:20">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="36">
+      <c r="C4" s="67">
         <v>129.1</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="99">
         <f t="shared" si="0"/>
         <v>234.72727272727269</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="83">
         <v>270.38</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="68">
         <f t="shared" si="1"/>
         <v>13.186155511771325</v>
       </c>
-      <c r="G4" s="48">
+      <c r="G4" s="69">
         <v>270.31</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="70">
         <f t="shared" si="2"/>
         <v>13.163674030826575</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="71">
         <v>252.50399999999999</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="71">
         <f t="shared" si="3"/>
         <v>7.0401765012543569</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="72">
         <v>277.21300000000002</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="72">
         <f t="shared" si="4"/>
         <v>15.326022687510083</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="63">
         <v>190.5</v>
       </c>
-      <c r="N4" s="13">
+      <c r="N4" s="73">
         <f t="shared" si="5"/>
         <v>-23.216416129801935</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O4" s="64">
         <v>112.77</v>
       </c>
-      <c r="P4" s="14">
+      <c r="P4" s="74">
         <f t="shared" si="6"/>
         <v>-108.14691205752655</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="Q4" s="65">
         <v>99</v>
       </c>
-      <c r="R4" s="15">
+      <c r="R4" s="75">
         <f t="shared" si="7"/>
         <v>-137.09825528007343</v>
       </c>
-      <c r="S4" s="7">
-        <v>335</v>
-      </c>
-      <c r="T4" s="44">
+      <c r="S4" s="66">
+        <v>335.1</v>
+      </c>
+      <c r="T4" s="84">
         <f t="shared" si="8"/>
-        <v>29.932157394843973</v>
+        <v>29.953066927104544</v>
       </c>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="67">
         <v>271.23</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="99">
         <f t="shared" si="0"/>
         <v>493.14545454545453</v>
       </c>
-      <c r="E5" s="46">
-        <v>412.91</v>
-      </c>
-      <c r="F5" s="9">
+      <c r="E5" s="83">
+        <v>437.61</v>
+      </c>
+      <c r="F5" s="68">
         <f t="shared" si="1"/>
-        <v>-19.431705346311425</v>
-      </c>
-      <c r="G5" s="48">
-        <v>412.67</v>
-      </c>
-      <c r="H5" s="10">
+        <v>-12.690627395501592</v>
+      </c>
+      <c r="G5" s="69">
+        <v>435.67</v>
+      </c>
+      <c r="H5" s="70">
         <f t="shared" si="2"/>
-        <v>-19.501164258476386</v>
-      </c>
-      <c r="I5" s="11">
+        <v>-13.192428798277254</v>
+      </c>
+      <c r="I5" s="71">
         <v>410.4</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="71">
         <f t="shared" si="3"/>
         <v>-20.162147793726742</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="72">
         <v>434.423</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="72">
         <f t="shared" si="4"/>
         <v>-13.51734474129006</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="63">
         <v>343</v>
       </c>
-      <c r="N5" s="13">
+      <c r="N5" s="73">
         <f t="shared" si="5"/>
         <v>-43.774184998674784</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="64">
         <v>250.72</v>
       </c>
-      <c r="P5" s="14">
+      <c r="P5" s="74">
         <f t="shared" si="6"/>
         <v>-96.691709694262343</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="65">
         <v>222</v>
       </c>
-      <c r="R5" s="15">
+      <c r="R5" s="75">
         <f t="shared" si="7"/>
         <v>-122.13759213759212</v>
       </c>
-      <c r="S5" s="7">
-        <v>474</v>
-      </c>
-      <c r="T5" s="44">
+      <c r="S5" s="66">
+        <v>473.8</v>
+      </c>
+      <c r="T5" s="84">
         <f t="shared" si="8"/>
-        <v>-4.0391254315304908</v>
+        <v>-4.0830423270271243</v>
       </c>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="67">
         <v>40.74</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="99">
         <f t="shared" si="0"/>
         <v>74.072727272727263</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="83">
         <v>78.66</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="68">
         <f t="shared" si="1"/>
         <v>5.8317731086609887</v>
       </c>
-      <c r="G6" s="48">
+      <c r="G6" s="69">
         <v>78.03</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="70">
         <f t="shared" si="2"/>
         <v>5.071476005732074</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="71">
         <v>43.847999999999999</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="71">
         <f t="shared" si="3"/>
         <v>-68.930686172065464</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="72">
         <v>84.33</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="72">
         <f t="shared" si="4"/>
         <v>12.163254745965535</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="63">
         <v>29.2</v>
       </c>
-      <c r="N6" s="13">
+      <c r="N6" s="73">
         <f t="shared" si="5"/>
         <v>-153.67372353673721</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="64">
         <v>36.770000000000003</v>
       </c>
-      <c r="P6" s="14">
+      <c r="P6" s="74">
         <f t="shared" si="6"/>
         <v>-101.44880955324247</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="Q6" s="65">
         <v>10.5</v>
       </c>
-      <c r="R6" s="15">
+      <c r="R6" s="75">
         <f t="shared" si="7"/>
         <v>-605.45454545454538</v>
       </c>
-      <c r="S6" s="7"/>
-      <c r="T6" s="44" t="e">
+      <c r="S6" s="66">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="T6" s="84">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>-13.261050875729751</v>
       </c>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="67">
         <v>65.87</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="99">
         <f t="shared" si="0"/>
         <v>119.76363636363637</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="83">
         <v>80.25</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="68">
         <f t="shared" si="1"/>
         <v>-49.238176154064007</v>
       </c>
-      <c r="G7" s="48">
+      <c r="G7" s="69">
         <v>81.17</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="70">
         <f t="shared" si="2"/>
         <v>-47.546675327875278</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="71">
         <v>55.08</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="71">
         <f t="shared" si="3"/>
         <v>-117.43579586716844</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="72">
         <v>82.099000000000004</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="72">
         <f t="shared" si="4"/>
         <v>-45.877095170021995</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="63">
         <v>63.5</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="73">
         <f t="shared" si="5"/>
         <v>-88.60415175375806</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="64">
         <v>39.5</v>
       </c>
-      <c r="P7" s="14">
+      <c r="P7" s="74">
         <f t="shared" si="6"/>
         <v>-203.19907940161107</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7" s="65">
         <v>10.75</v>
       </c>
-      <c r="R7" s="15">
+      <c r="R7" s="75">
         <f t="shared" si="7"/>
         <v>-1014.0803382663847</v>
       </c>
-      <c r="S7" s="7"/>
-      <c r="T7" s="44" t="e">
+      <c r="S7" s="66">
+        <v>79.099999999999994</v>
+      </c>
+      <c r="T7" s="84">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" s="3" customFormat="1">
-      <c r="A8" s="3" t="s">
+        <v>-51.407884151246996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" s="2" customFormat="1">
+      <c r="A8" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="36">
+      <c r="C8" s="67">
         <v>487.72</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="99">
         <f t="shared" si="0"/>
         <v>886.76363636363635</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="83">
         <v>754.91</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="68">
         <f t="shared" si="1"/>
         <v>-17.466139852914438</v>
       </c>
-      <c r="G8" s="48">
+      <c r="G8" s="69">
         <v>758.8</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="70">
         <f t="shared" si="2"/>
         <v>-16.863947860257827</v>
       </c>
-      <c r="I8" s="50">
+      <c r="I8" s="76">
         <v>708.048</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="71">
         <f t="shared" si="3"/>
         <v>-25.240610292471182</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="72">
         <v>770.98</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="72">
         <f t="shared" si="4"/>
         <v>-15.017722426474919</v>
       </c>
-      <c r="M8" s="16">
+      <c r="M8" s="77">
         <v>733.7</v>
       </c>
-      <c r="N8" s="13">
+      <c r="N8" s="73">
         <f t="shared" si="5"/>
         <v>-20.86188310803275</v>
       </c>
-      <c r="O8" s="17">
+      <c r="O8" s="78">
         <v>491.73</v>
       </c>
-      <c r="P8" s="14">
+      <c r="P8" s="74">
         <f t="shared" si="6"/>
         <v>-80.335476046536982</v>
       </c>
-      <c r="Q8" s="18">
+      <c r="Q8" s="79">
         <v>385</v>
       </c>
-      <c r="R8" s="15">
+      <c r="R8" s="75">
         <f t="shared" si="7"/>
         <v>-130.32821723730814</v>
       </c>
-      <c r="S8" s="19"/>
-      <c r="T8" s="44" t="e">
+      <c r="S8" s="80">
+        <v>777.9</v>
+      </c>
+      <c r="T8" s="84">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>-13.994554102537135</v>
       </c>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="36">
+      <c r="C9" s="67">
         <v>480.87</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="99">
         <f t="shared" si="0"/>
         <v>874.30909090909086</v>
       </c>
-      <c r="E9" s="46">
+      <c r="E9" s="83">
         <v>729.69</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="68">
         <f t="shared" si="1"/>
         <v>-19.819250765268919</v>
       </c>
-      <c r="G9" s="48">
+      <c r="G9" s="69">
         <v>730.2</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="70">
         <f t="shared" si="2"/>
         <v>-19.73556435347724</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="71">
         <v>747.36</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="71">
         <f t="shared" si="3"/>
         <v>-16.986337362059896</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="72">
         <v>804.54399999999998</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="72">
         <f t="shared" si="4"/>
         <v>-8.6713829087148593</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9" s="63">
         <v>704</v>
       </c>
-      <c r="N9" s="13">
+      <c r="N9" s="73">
         <f t="shared" si="5"/>
         <v>-24.191632231404949</v>
       </c>
-      <c r="O9" s="5">
+      <c r="O9" s="64">
         <v>517.11</v>
       </c>
-      <c r="P9" s="14">
+      <c r="P9" s="74">
         <f t="shared" si="6"/>
         <v>-69.076036222291364</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="Q9" s="65">
         <v>409</v>
       </c>
-      <c r="R9" s="15">
+      <c r="R9" s="75">
         <f t="shared" si="7"/>
         <v>-113.76750388975327</v>
       </c>
-      <c r="S9" s="7"/>
-      <c r="T9" s="44" t="e">
+      <c r="S9" s="66">
+        <v>681.5</v>
+      </c>
+      <c r="T9" s="84">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>-28.291869539118249</v>
       </c>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="36">
+      <c r="C10" s="67">
         <v>135.84</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="99">
         <f t="shared" si="0"/>
         <v>246.98181818181817</v>
       </c>
-      <c r="E10" s="46">
+      <c r="E10" s="83">
         <v>155.91999999999999</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="68">
         <f t="shared" si="1"/>
         <v>-58.402910583516032</v>
       </c>
-      <c r="G10" s="48">
+      <c r="G10" s="69">
         <v>154.52000000000001</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="70">
         <f t="shared" si="2"/>
         <v>-59.838090979690747</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="71">
         <v>176.904</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="71">
         <f t="shared" si="3"/>
         <v>-39.613472946806276</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="72">
         <v>180.93700000000001</v>
       </c>
-      <c r="L10" s="12">
+      <c r="L10" s="72">
         <f t="shared" si="4"/>
         <v>-36.501554785266784</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10" s="63">
         <v>159.19999999999999</v>
       </c>
-      <c r="N10" s="13">
+      <c r="N10" s="73">
         <f t="shared" si="5"/>
         <v>-55.139333028780271</v>
       </c>
-      <c r="O10" s="5">
+      <c r="O10" s="64">
         <v>122.15</v>
       </c>
-      <c r="P10" s="14">
+      <c r="P10" s="74">
         <f t="shared" si="6"/>
         <v>-102.1955122241655</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="Q10" s="65">
         <v>62</v>
       </c>
-      <c r="R10" s="15">
+      <c r="R10" s="75">
         <f t="shared" si="7"/>
         <v>-298.35777126099703</v>
       </c>
-      <c r="S10" s="7"/>
-      <c r="T10" s="44" t="e">
+      <c r="S10" s="66">
+        <v>173.3</v>
+      </c>
+      <c r="T10" s="84">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>-42.516917589046827</v>
       </c>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="36">
+      <c r="C11" s="67">
         <v>130.58000000000001</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="99">
         <f t="shared" si="0"/>
         <v>237.41818181818184</v>
       </c>
-      <c r="E11" s="46">
+      <c r="E11" s="83">
         <v>246.16</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="68">
         <f t="shared" si="1"/>
         <v>3.5512748544922652</v>
       </c>
-      <c r="G11" s="48">
+      <c r="G11" s="69">
         <v>247.81</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="70">
         <f t="shared" si="2"/>
         <v>4.1934619998459173</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="71">
         <v>225.28800000000001</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="71">
         <f t="shared" si="3"/>
         <v>-5.3843000151725011</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="72">
         <v>225.29400000000001</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="72">
         <f t="shared" si="4"/>
         <v>-5.3814934344375898</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11" s="63">
         <v>161.30000000000001</v>
       </c>
-      <c r="N11" s="13">
+      <c r="N11" s="73">
         <f t="shared" si="5"/>
         <v>-47.190441300794674</v>
       </c>
-      <c r="O11" s="5">
+      <c r="O11" s="64">
         <v>124.64</v>
       </c>
-      <c r="P11" s="14">
+      <c r="P11" s="74">
         <f t="shared" si="6"/>
         <v>-90.483136888785168</v>
       </c>
-      <c r="Q11" s="6">
+      <c r="Q11" s="65">
         <v>94</v>
       </c>
-      <c r="R11" s="15">
+      <c r="R11" s="75">
         <f t="shared" si="7"/>
         <v>-152.5725338491296</v>
       </c>
-      <c r="S11" s="7"/>
-      <c r="T11" s="44" t="e">
+      <c r="S11" s="66">
+        <v>350.6</v>
+      </c>
+      <c r="T11" s="84">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>32.282321215578484</v>
       </c>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="36">
+      <c r="C12" s="67">
         <v>209.55</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="99">
         <f t="shared" si="0"/>
         <v>381</v>
       </c>
-      <c r="E12" s="46">
-        <v>229.11</v>
-      </c>
-      <c r="F12" s="9">
+      <c r="E12" s="83">
+        <v>317.2</v>
+      </c>
+      <c r="F12" s="68">
         <f t="shared" si="1"/>
-        <v>-66.295665837370692</v>
-      </c>
-      <c r="G12" s="48">
-        <v>230.03</v>
-      </c>
-      <c r="H12" s="10">
+        <v>-20.113493064312742</v>
+      </c>
+      <c r="G12" s="69">
+        <v>317.41000000000003</v>
+      </c>
+      <c r="H12" s="70">
         <f t="shared" si="2"/>
-        <v>-65.630569925661874</v>
-      </c>
-      <c r="I12" s="11">
+        <v>-20.034025393024784</v>
+      </c>
+      <c r="I12" s="71">
         <v>389.23200000000003</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="71">
         <f t="shared" si="3"/>
         <v>2.1149340239240422</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="72">
         <v>652.13199999999995</v>
       </c>
-      <c r="L12" s="12">
+      <c r="L12" s="72">
         <f t="shared" si="4"/>
         <v>41.576245300031275</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12" s="63">
         <v>348.7</v>
       </c>
-      <c r="N12" s="13">
+      <c r="N12" s="73">
         <f t="shared" si="5"/>
         <v>-9.2629767708632098</v>
       </c>
-      <c r="O12" s="5">
+      <c r="O12" s="64">
         <v>113.53</v>
       </c>
-      <c r="P12" s="14">
+      <c r="P12" s="74">
         <f t="shared" si="6"/>
         <v>-235.59411609266277</v>
       </c>
-      <c r="Q12" s="6">
+      <c r="Q12" s="65">
         <v>164</v>
       </c>
-      <c r="R12" s="15">
+      <c r="R12" s="75">
         <f t="shared" si="7"/>
         <v>-132.3170731707317</v>
       </c>
-      <c r="S12" s="7"/>
-      <c r="T12" s="44" t="e">
+      <c r="S12" s="66">
+        <v>226.8</v>
+      </c>
+      <c r="T12" s="84">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>-67.989417989417973</v>
       </c>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="36">
+      <c r="C13" s="67">
         <v>285.27999999999997</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="99">
         <f t="shared" si="0"/>
         <v>518.69090909090903</v>
       </c>
-      <c r="E13" s="46">
+      <c r="E13" s="83">
         <v>493.58</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="68">
         <f t="shared" si="1"/>
         <v>-5.0875053873554537</v>
       </c>
-      <c r="G13" s="48">
+      <c r="G13" s="69">
         <v>497.5</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="70">
         <f t="shared" si="2"/>
         <v>-4.259479214253072</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="71">
         <v>434.80799999999999</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="71">
         <f t="shared" si="3"/>
         <v>-19.291942441470496</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="72">
         <v>481.536</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L13" s="72">
         <f t="shared" si="4"/>
         <v>-7.7159151321830626</v>
       </c>
-      <c r="M13" s="4">
+      <c r="M13" s="63">
         <v>400.9</v>
       </c>
-      <c r="N13" s="13">
+      <c r="N13" s="73">
         <f t="shared" si="5"/>
         <v>-29.381618630807949</v>
       </c>
-      <c r="O13" s="5">
+      <c r="O13" s="64">
         <v>265.24</v>
       </c>
-      <c r="P13" s="14">
+      <c r="P13" s="74">
         <f t="shared" si="6"/>
         <v>-95.555311827367291</v>
       </c>
-      <c r="Q13" s="6">
+      <c r="Q13" s="65">
         <v>208</v>
       </c>
-      <c r="R13" s="15">
+      <c r="R13" s="75">
         <f t="shared" si="7"/>
         <v>-149.37062937062936</v>
       </c>
-      <c r="S13" s="7"/>
-      <c r="T13" s="44" t="e">
+      <c r="S13" s="66">
+        <v>456.7</v>
+      </c>
+      <c r="T13" s="84">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>-13.573660847582451</v>
       </c>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="36">
+      <c r="C14" s="67">
         <v>492.76</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="99">
         <f t="shared" si="0"/>
         <v>895.92727272727268</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="83">
         <v>736.31</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="68">
         <f t="shared" si="1"/>
         <v>-21.677998767811484</v>
       </c>
-      <c r="G14" s="48">
+      <c r="G14" s="69">
         <v>738.33</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="70">
         <f t="shared" si="2"/>
         <v>-21.345099444323356</v>
       </c>
-      <c r="I14" s="11">
+      <c r="I14" s="71">
         <v>649.94399999999996</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J14" s="71">
         <f t="shared" si="3"/>
         <v>-37.846841070503416</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K14" s="72">
         <v>627.39200000000005</v>
       </c>
-      <c r="L14" s="12">
+      <c r="L14" s="72">
         <f t="shared" si="4"/>
         <v>-42.801832463160608</v>
       </c>
-      <c r="M14" s="4">
+      <c r="M14" s="63">
         <v>605.70000000000005</v>
       </c>
-      <c r="N14" s="13">
+      <c r="N14" s="73">
         <f t="shared" si="5"/>
         <v>-47.916010025965434</v>
       </c>
-      <c r="O14" s="5">
+      <c r="O14" s="64">
         <v>531.75</v>
       </c>
-      <c r="P14" s="14">
+      <c r="P14" s="74">
         <f t="shared" si="6"/>
         <v>-68.486558105740045</v>
       </c>
-      <c r="Q14" s="6">
+      <c r="Q14" s="65">
         <v>319</v>
       </c>
-      <c r="R14" s="15">
+      <c r="R14" s="75">
         <f t="shared" si="7"/>
         <v>-180.85494442861213</v>
       </c>
-      <c r="S14" s="7"/>
-      <c r="T14" s="44" t="e">
+      <c r="S14" s="66">
+        <v>742.3</v>
+      </c>
+      <c r="T14" s="84">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>-20.69611649296413</v>
       </c>
     </row>
     <row r="15" spans="1:20">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="37">
+      <c r="C15" s="82">
         <v>581.73</v>
       </c>
-      <c r="D15" s="38">
+      <c r="D15" s="100">
         <f t="shared" si="0"/>
         <v>1057.6909090909091</v>
       </c>
-      <c r="E15" s="47">
+      <c r="E15" s="85">
         <v>872.31</v>
       </c>
-      <c r="F15" s="39">
+      <c r="F15" s="86">
         <f t="shared" si="1"/>
         <v>-21.251723480289026</v>
       </c>
-      <c r="G15" s="49">
+      <c r="G15" s="87">
         <v>868.19</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15" s="88">
         <f t="shared" si="2"/>
         <v>-21.82712414228557</v>
       </c>
-      <c r="I15" s="51">
+      <c r="I15" s="89">
         <v>820.58399999999995</v>
       </c>
-      <c r="J15" s="11">
+      <c r="J15" s="89">
         <f t="shared" si="3"/>
         <v>-28.894897913060603</v>
       </c>
-      <c r="K15" s="12">
+      <c r="K15" s="90">
         <v>811.38800000000003</v>
       </c>
-      <c r="L15" s="12">
+      <c r="L15" s="90">
         <f t="shared" si="4"/>
         <v>-30.355749541638417</v>
       </c>
-      <c r="M15" s="40">
+      <c r="M15" s="91">
         <v>752.1</v>
       </c>
-      <c r="N15" s="13">
+      <c r="N15" s="92">
         <f t="shared" si="5"/>
         <v>-40.631685825144146</v>
       </c>
-      <c r="O15" s="41">
+      <c r="O15" s="93">
         <v>555.38</v>
       </c>
-      <c r="P15" s="14">
+      <c r="P15" s="94">
         <f t="shared" si="6"/>
         <v>-90.444544112303134</v>
       </c>
-      <c r="Q15" s="42">
+      <c r="Q15" s="95">
         <v>450</v>
       </c>
-      <c r="R15" s="15">
+      <c r="R15" s="96">
         <f t="shared" si="7"/>
         <v>-135.04242424242426</v>
       </c>
-      <c r="S15" s="43"/>
-      <c r="T15" s="44" t="e">
+      <c r="S15" s="97">
+        <v>1031.4000000000001</v>
+      </c>
+      <c r="T15" s="98">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>-2.5490507165899796</v>
       </c>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="109" t="s">
+      <c r="A16" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="109"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="55"/>
-      <c r="F16" s="53">
+      <c r="B16" s="62"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
+      <c r="F16" s="5">
         <f>AVERAGE(F2:F15)</f>
-        <v>-17.550282083369233</v>
-      </c>
-      <c r="G16" s="53"/>
-      <c r="H16" s="53">
+        <v>-13.770049888807248</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5">
         <f t="shared" ref="H16:T16" si="9">AVERAGE(H2:H15)</f>
-        <v>-17.440658035402972</v>
-      </c>
-      <c r="I16" s="53"/>
-      <c r="J16" s="53">
+        <v>-13.733138035914667</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5">
         <f t="shared" si="9"/>
         <v>-26.89506396162685</v>
       </c>
-      <c r="K16" s="53"/>
-      <c r="L16" s="53">
+      <c r="K16" s="5"/>
+      <c r="L16" s="5">
         <f t="shared" si="9"/>
         <v>-10.398735825607336</v>
       </c>
-      <c r="M16" s="53"/>
-      <c r="N16" s="53">
+      <c r="M16" s="5"/>
+      <c r="N16" s="5">
         <f t="shared" si="9"/>
         <v>-48.161192599725332</v>
       </c>
-      <c r="O16" s="53"/>
-      <c r="P16" s="53">
+      <c r="O16" s="5"/>
+      <c r="P16" s="5">
         <f t="shared" si="9"/>
         <v>-116.13760891259462</v>
       </c>
-      <c r="Q16" s="53"/>
-      <c r="R16" s="53">
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5">
         <f t="shared" si="9"/>
         <v>-249.22521274710371</v>
       </c>
-      <c r="S16" s="53"/>
-      <c r="T16" s="53" t="e">
+      <c r="S16" s="5"/>
+      <c r="T16" s="5">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>-11.346258291700934</v>
       </c>
     </row>
     <row r="17" spans="1:20">
-      <c r="A17" s="108" t="s">
+      <c r="A17" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="108"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="53" cm="1">
+      <c r="B17" s="61"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="5" cm="1">
         <f t="array" ref="F17">AVERAGE(ABS(F2:F15))</f>
-        <v>22.496103129930123</v>
-      </c>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53" cm="1">
+        <v>18.715870935368141</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5" cm="1">
         <f t="array" ref="H17">AVERAGE(ABS(H2:H15))</f>
-        <v>22.288503439984179</v>
-      </c>
-      <c r="I17" s="53"/>
-      <c r="J17" s="53" cm="1">
+        <v>18.580983440495878</v>
+      </c>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5" cm="1">
         <f t="array" ref="J17">AVERAGE(ABS(J2:J15))</f>
         <v>28.823503105759261</v>
       </c>
-      <c r="K17" s="53"/>
-      <c r="L17" s="53" cm="1">
+      <c r="K17" s="5"/>
+      <c r="L17" s="5" cm="1">
         <f t="array" ref="L17">AVERAGE(ABS(L2:L15))</f>
         <v>20.265239073251177</v>
       </c>
-      <c r="M17" s="53"/>
-      <c r="N17" s="53" cm="1">
+      <c r="M17" s="5"/>
+      <c r="N17" s="5" cm="1">
         <f t="array" ref="N17">AVERAGE(ABS(N2:N15))</f>
         <v>48.161192599725332</v>
       </c>
-      <c r="O17" s="53"/>
-      <c r="P17" s="53" cm="1">
+      <c r="O17" s="5"/>
+      <c r="P17" s="5" cm="1">
         <f t="array" ref="P17">AVERAGE(ABS(P2:P15))</f>
         <v>116.13760891259462</v>
       </c>
-      <c r="Q17" s="53"/>
-      <c r="R17" s="53" cm="1">
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5" cm="1">
         <f t="array" ref="R17">AVERAGE(ABS(R2:R15))</f>
         <v>249.22521274710371</v>
       </c>
-      <c r="S17" s="53"/>
-      <c r="T17" s="53" t="e" cm="1">
+      <c r="S17" s="5"/>
+      <c r="T17" s="5" cm="1">
         <f t="array" ref="T17">AVERAGE(ABS(T2:T15))</f>
-        <v>#DIV/0!</v>
+        <v>25.562822369907728</v>
       </c>
     </row>
     <row r="19" spans="1:20">
-      <c r="C19" s="111"/>
-      <c r="D19" s="100"/>
-      <c r="E19" s="110"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="53"/>
     </row>
     <row r="20" spans="1:20">
-      <c r="C20" s="111"/>
-      <c r="D20" s="100"/>
-      <c r="E20" s="110"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="53"/>
     </row>
     <row r="21" spans="1:20">
-      <c r="C21" s="111"/>
-      <c r="D21" s="100"/>
-      <c r="E21" s="110"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="53"/>
     </row>
     <row r="22" spans="1:20">
-      <c r="C22" s="111"/>
-      <c r="D22" s="100"/>
-      <c r="E22" s="110"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="53"/>
     </row>
     <row r="23" spans="1:20">
-      <c r="C23" s="111"/>
-      <c r="D23" s="100"/>
-      <c r="E23" s="110"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="53"/>
     </row>
     <row r="24" spans="1:20">
-      <c r="C24" s="111"/>
-      <c r="D24" s="100"/>
-      <c r="E24" s="110"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="53"/>
     </row>
     <row r="25" spans="1:20">
-      <c r="C25" s="111"/>
-      <c r="D25" s="100"/>
-      <c r="E25" s="110"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="53"/>
+      <c r="M25" s="12"/>
     </row>
     <row r="26" spans="1:20">
-      <c r="C26" s="111"/>
-      <c r="D26" s="100"/>
-      <c r="E26" s="110"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="53"/>
     </row>
     <row r="27" spans="1:20">
-      <c r="C27" s="111"/>
-      <c r="D27" s="100"/>
-      <c r="E27" s="110"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="53"/>
     </row>
     <row r="28" spans="1:20">
-      <c r="C28" s="111"/>
-      <c r="D28" s="100"/>
-      <c r="E28" s="110"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="53"/>
     </row>
     <row r="29" spans="1:20">
-      <c r="C29" s="111"/>
-      <c r="D29" s="100"/>
-      <c r="E29" s="110"/>
-      <c r="J29" s="60"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="53"/>
+      <c r="J29" s="12"/>
     </row>
     <row r="30" spans="1:20">
-      <c r="C30" s="111"/>
-      <c r="D30" s="100"/>
-      <c r="E30" s="110"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="53"/>
     </row>
     <row r="31" spans="1:20">
-      <c r="C31" s="111"/>
-      <c r="D31" s="100"/>
-      <c r="E31" s="110"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="53"/>
     </row>
     <row r="32" spans="1:20">
-      <c r="C32" s="111"/>
-      <c r="D32" s="100"/>
-      <c r="E32" s="110"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="53"/>
     </row>
     <row r="33" spans="3:3">
-      <c r="C33" s="100"/>
+      <c r="C33" s="52"/>
     </row>
     <row r="34" spans="3:3">
-      <c r="C34" s="100"/>
+      <c r="C34" s="52"/>
     </row>
     <row r="35" spans="3:3">
-      <c r="C35" s="100"/>
+      <c r="C35" s="52"/>
     </row>
     <row r="36" spans="3:3">
-      <c r="C36" s="100"/>
+      <c r="C36" s="52"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
Update benchmarking procedure for 22 SMCs and optimize Molovol large probe
</commit_message>
<xml_diff>
--- a/results/quantitative-analysis.xlsx
+++ b/results/quantitative-analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gyorgy Szaloki\Papers\Cavity calculations\Benchmarking\Structures for benchmarking\QUANTITATIVE ANALYSIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A18792F-8711-4D0C-A5EF-4DFE1DC82123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE215D6A-8DB7-491F-9A02-327A8DD92612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" tabRatio="500" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" tabRatio="500" firstSheet="4" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="53">
   <si>
     <t>Cage</t>
   </si>
@@ -129,61 +129,64 @@
     <t>B10</t>
   </si>
   <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>2 guests</t>
+  </si>
+  <si>
     <t>B12</t>
   </si>
   <si>
-    <t>2 guests</t>
-  </si>
-  <si>
     <t>B13</t>
   </si>
   <si>
+    <t>C70</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>MRE</t>
+  </si>
+  <si>
+    <t>MRAE</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Mean Error</t>
+  </si>
+  <si>
+    <t>RE</t>
+  </si>
+  <si>
+    <t>Relative Error</t>
+  </si>
+  <si>
+    <t>Mean Relative Error</t>
+  </si>
+  <si>
+    <t>RAE</t>
+  </si>
+  <si>
+    <t>Relative Absolute Error</t>
+  </si>
+  <si>
+    <t>Mean Relative Absolute Error</t>
+  </si>
+  <si>
     <t>B14</t>
-  </si>
-  <si>
-    <t>C70</t>
-  </si>
-  <si>
-    <t>ME</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>MRE</t>
-  </si>
-  <si>
-    <t>MRAE</t>
-  </si>
-  <si>
-    <t>Legend</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>Mean Error</t>
-  </si>
-  <si>
-    <t>RE</t>
-  </si>
-  <si>
-    <t>Relative Error</t>
-  </si>
-  <si>
-    <t>Mean Relative Error</t>
-  </si>
-  <si>
-    <t>RAE</t>
-  </si>
-  <si>
-    <t>Relative Absolute Error</t>
-  </si>
-  <si>
-    <t>Mean Relative Absolute Error</t>
   </si>
   <si>
     <t>Formula: Error (E) = Calculated Volume - Estimated Volume [true]</t>
@@ -1260,6 +1263,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1306,9 +1312,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1677,8 +1680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2088FB93-14C1-42DA-AB49-CBCB57E4F20C}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1798,7 +1801,7 @@
       </c>
       <c r="G3" s="18" t="str">
         <f>ROUND('Cavity Volume'!G3,0)&amp;" ("&amp;ROUND(RE!D3*100,1)&amp;"%)"</f>
-        <v>289 (2.7%)</v>
+        <v>288 (2.6%)</v>
       </c>
       <c r="H3" s="18" t="str">
         <f>ROUND('Cavity Volume'!H3,0)&amp;" ("&amp;ROUND(RE!E3*100,1)&amp;"%)"</f>
@@ -2372,7 +2375,7 @@
       </c>
       <c r="G15" s="128">
         <f>E!D15</f>
-        <v>-116.52050349650345</v>
+        <v>-116.53711888111883</v>
       </c>
       <c r="H15" s="128">
         <f>E!E15</f>
@@ -2418,7 +2421,7 @@
       </c>
       <c r="G16" s="107">
         <f>RE!D15</f>
-        <v>-0.22702371285222134</v>
+        <v>-0.22708285764245148</v>
       </c>
       <c r="H16" s="107">
         <f>RE!E15</f>
@@ -2464,7 +2467,7 @@
       </c>
       <c r="G17" s="111">
         <f>RAE!D15</f>
-        <v>0.23374279842875711</v>
+        <v>0.23368365363852697</v>
       </c>
       <c r="H17" s="111">
         <f>RAE!E15</f>
@@ -2488,72 +2491,72 @@
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="145" t="s">
+      <c r="A19" s="146" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="146"/>
-      <c r="C19" s="146"/>
-      <c r="D19" s="147"/>
+      <c r="B19" s="147"/>
+      <c r="C19" s="147"/>
+      <c r="D19" s="148"/>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="148" t="s">
+      <c r="B20" s="149" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="148"/>
-      <c r="D20" s="149"/>
+      <c r="C20" s="149"/>
+      <c r="D20" s="150"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="150" t="s">
+      <c r="B21" s="151" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="150"/>
-      <c r="D21" s="151"/>
+      <c r="C21" s="151"/>
+      <c r="D21" s="152"/>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="150" t="s">
+      <c r="B22" s="151" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="150"/>
-      <c r="D22" s="151"/>
+      <c r="C22" s="151"/>
+      <c r="D22" s="152"/>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="150" t="s">
+      <c r="B23" s="151" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="150"/>
-      <c r="D23" s="151"/>
+      <c r="C23" s="151"/>
+      <c r="D23" s="152"/>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="93" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="152" t="s">
+      <c r="B24" s="153" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="152"/>
-      <c r="D24" s="153"/>
+      <c r="C24" s="153"/>
+      <c r="D24" s="154"/>
     </row>
     <row r="25" spans="1:12" ht="12.75" customHeight="1">
       <c r="A25" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="143" t="s">
+      <c r="B25" s="144" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="143"/>
-      <c r="D25" s="144"/>
+      <c r="C25" s="144"/>
+      <c r="D25" s="145"/>
     </row>
     <row r="30" spans="1:12">
       <c r="D30" s="22"/>
@@ -2579,8 +2582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670A7F8F-95E9-4101-8C0C-944E3FC16B0B}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2673,7 +2676,7 @@
       <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="157">
+      <c r="C3" s="141">
         <v>154.51</v>
       </c>
       <c r="D3" s="134">
@@ -2687,7 +2690,7 @@
         <v>289.06</v>
       </c>
       <c r="G3" s="28">
-        <v>288.57600000000002</v>
+        <v>288.36</v>
       </c>
       <c r="H3" s="29">
         <v>279.30099999999999</v>
@@ -2712,7 +2715,7 @@
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="141">
+      <c r="C4" s="142">
         <v>136.63</v>
       </c>
       <c r="D4" s="134">
@@ -2751,7 +2754,7 @@
       <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="141">
+      <c r="C5" s="142">
         <v>309.11</v>
       </c>
       <c r="D5" s="134">
@@ -2790,7 +2793,7 @@
       <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="141">
+      <c r="C6" s="142">
         <v>49.62</v>
       </c>
       <c r="D6" s="134">
@@ -2829,7 +2832,7 @@
       <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="141">
+      <c r="C7" s="142">
         <v>52.68</v>
       </c>
       <c r="D7" s="134">
@@ -2868,7 +2871,7 @@
       <c r="B8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="141">
+      <c r="C8" s="142">
         <v>519.20000000000005</v>
       </c>
       <c r="D8" s="134">
@@ -2907,7 +2910,7 @@
       <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="141">
+      <c r="C9" s="142">
         <v>511.7</v>
       </c>
       <c r="D9" s="134">
@@ -2946,7 +2949,7 @@
       <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="141">
+      <c r="C10" s="142">
         <v>141.16</v>
       </c>
       <c r="D10" s="134">
@@ -2985,7 +2988,7 @@
       <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="141">
+      <c r="C11" s="142">
         <v>150.5</v>
       </c>
       <c r="D11" s="134">
@@ -3019,12 +3022,12 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="141">
+      <c r="C12" s="142">
         <v>306.64</v>
       </c>
       <c r="D12" s="134">
@@ -3058,12 +3061,12 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="141">
+      <c r="C13" s="142">
         <v>524.47</v>
       </c>
       <c r="D13" s="134">
@@ -3097,12 +3100,12 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="4" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="142">
+      <c r="C14" s="143">
         <v>617.54999999999995</v>
       </c>
       <c r="D14" s="135">
@@ -3144,7 +3147,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3240,7 +3243,7 @@
       </c>
       <c r="D3" s="45">
         <f>'Cavity Volume'!G3-'Cavity Volume'!D3</f>
-        <v>7.6487272727273421</v>
+        <v>7.4327272727273339</v>
       </c>
       <c r="E3" s="46">
         <f>'Cavity Volume'!H3-'Cavity Volume'!D3</f>
@@ -3684,7 +3687,7 @@
       </c>
       <c r="D15" s="130">
         <f t="shared" si="0"/>
-        <v>-116.52050349650345</v>
+        <v>-116.53711888111883</v>
       </c>
       <c r="E15" s="130">
         <f t="shared" si="0"/>
@@ -3708,28 +3711,28 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="154" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="154"/>
-      <c r="C17" s="154"/>
-      <c r="D17" s="154"/>
-      <c r="E17" s="154"/>
-      <c r="F17" s="154"/>
-      <c r="G17" s="154"/>
-      <c r="H17" s="154"/>
-      <c r="I17" s="154"/>
+      <c r="A17" s="155" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="155"/>
+      <c r="C17" s="155"/>
+      <c r="D17" s="155"/>
+      <c r="E17" s="155"/>
+      <c r="F17" s="155"/>
+      <c r="G17" s="155"/>
+      <c r="H17" s="155"/>
+      <c r="I17" s="155"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="154"/>
-      <c r="B18" s="154"/>
-      <c r="C18" s="154"/>
-      <c r="D18" s="154"/>
-      <c r="E18" s="154"/>
-      <c r="F18" s="154"/>
-      <c r="G18" s="154"/>
-      <c r="H18" s="154"/>
-      <c r="I18" s="154"/>
+      <c r="A18" s="155"/>
+      <c r="B18" s="155"/>
+      <c r="C18" s="155"/>
+      <c r="D18" s="155"/>
+      <c r="E18" s="155"/>
+      <c r="F18" s="155"/>
+      <c r="G18" s="155"/>
+      <c r="H18" s="155"/>
+      <c r="I18" s="155"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3744,7 +3747,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3840,7 +3843,7 @@
       </c>
       <c r="D3" s="58">
         <f>('Cavity Volume'!G3-'Cavity Volume'!D3)/'Cavity Volume'!D3</f>
-        <v>2.7226716717364822E-2</v>
+        <v>2.6457834444372753E-2</v>
       </c>
       <c r="E3" s="59">
         <f>('Cavity Volume'!H3-'Cavity Volume'!D3)/'Cavity Volume'!D3</f>
@@ -4284,7 +4287,7 @@
       </c>
       <c r="D15" s="74">
         <f t="shared" si="0"/>
-        <v>-0.22702371285222134</v>
+        <v>-0.22708285764245148</v>
       </c>
       <c r="E15" s="74">
         <f t="shared" si="0"/>
@@ -4308,28 +4311,28 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A17" s="155" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="156"/>
-      <c r="C17" s="156"/>
-      <c r="D17" s="156"/>
-      <c r="E17" s="156"/>
-      <c r="F17" s="156"/>
-      <c r="G17" s="156"/>
-      <c r="H17" s="156"/>
-      <c r="I17" s="156"/>
+      <c r="A17" s="156" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="157"/>
+      <c r="C17" s="157"/>
+      <c r="D17" s="157"/>
+      <c r="E17" s="157"/>
+      <c r="F17" s="157"/>
+      <c r="G17" s="157"/>
+      <c r="H17" s="157"/>
+      <c r="I17" s="157"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="155"/>
-      <c r="B18" s="156"/>
-      <c r="C18" s="156"/>
-      <c r="D18" s="156"/>
-      <c r="E18" s="156"/>
-      <c r="F18" s="156"/>
-      <c r="G18" s="156"/>
-      <c r="H18" s="156"/>
-      <c r="I18" s="156"/>
+      <c r="A18" s="156"/>
+      <c r="B18" s="157"/>
+      <c r="C18" s="157"/>
+      <c r="D18" s="157"/>
+      <c r="E18" s="157"/>
+      <c r="F18" s="157"/>
+      <c r="G18" s="157"/>
+      <c r="H18" s="157"/>
+      <c r="I18" s="157"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4343,8 +4346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{444A8883-6D6F-4C76-A0E2-94D465E0A1C3}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4440,7 +4443,7 @@
       </c>
       <c r="D3" s="58">
         <f>ABS('Cavity Volume'!G3-'Cavity Volume'!D3)/'Cavity Volume'!D3</f>
-        <v>2.7226716717364822E-2</v>
+        <v>2.6457834444372753E-2</v>
       </c>
       <c r="E3" s="59">
         <f>ABS('Cavity Volume'!H3-'Cavity Volume'!D3)/'Cavity Volume'!D3</f>
@@ -4884,7 +4887,7 @@
       </c>
       <c r="D15" s="74">
         <f t="shared" si="0"/>
-        <v>0.23374279842875711</v>
+        <v>0.23368365363852697</v>
       </c>
       <c r="E15" s="74">
         <f t="shared" si="0"/>
@@ -4908,28 +4911,28 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A17" s="155" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="156"/>
-      <c r="C17" s="156"/>
-      <c r="D17" s="156"/>
-      <c r="E17" s="156"/>
-      <c r="F17" s="156"/>
-      <c r="G17" s="156"/>
-      <c r="H17" s="156"/>
-      <c r="I17" s="156"/>
+      <c r="A17" s="156" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="157"/>
+      <c r="C17" s="157"/>
+      <c r="D17" s="157"/>
+      <c r="E17" s="157"/>
+      <c r="F17" s="157"/>
+      <c r="G17" s="157"/>
+      <c r="H17" s="157"/>
+      <c r="I17" s="157"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="155"/>
-      <c r="B18" s="156"/>
-      <c r="C18" s="156"/>
-      <c r="D18" s="156"/>
-      <c r="E18" s="156"/>
-      <c r="F18" s="156"/>
-      <c r="G18" s="156"/>
-      <c r="H18" s="156"/>
-      <c r="I18" s="156"/>
+      <c r="A18" s="156"/>
+      <c r="B18" s="157"/>
+      <c r="C18" s="157"/>
+      <c r="D18" s="157"/>
+      <c r="E18" s="157"/>
+      <c r="F18" s="157"/>
+      <c r="G18" s="157"/>
+      <c r="H18" s="157"/>
+      <c r="I18" s="157"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>